<commit_message>
Results with single bin.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +93,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,10 +123,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -123,8 +136,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,10 +462,8 @@
     <col min="23" max="23" width="2.85546875" customWidth="1"/>
     <col min="24" max="24" width="4.140625" customWidth="1"/>
     <col min="25" max="25" width="3" customWidth="1"/>
-    <col min="26" max="26" width="2.85546875" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" customWidth="1"/>
-    <col min="28" max="28" width="3" customWidth="1"/>
-    <col min="29" max="29" width="5" customWidth="1"/>
+    <col min="26" max="27" width="6" customWidth="1"/>
+    <col min="28" max="29" width="5" customWidth="1"/>
     <col min="30" max="31" width="6" customWidth="1"/>
     <col min="32" max="32" width="2.85546875" customWidth="1"/>
     <col min="33" max="33" width="4.140625" customWidth="1"/>
@@ -726,6 +739,69 @@
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="4">
+        <v>0.498</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.248</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.161</v>
+      </c>
+      <c r="H4">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.112</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.186</v>
+      </c>
+      <c r="K4">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="T4">
+        <v>0.97</v>
+      </c>
+      <c r="U4" s="4">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0.443</v>
+      </c>
+      <c r="Z4">
+        <v>9.4E-2</v>
+      </c>
+      <c r="AA4">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AB4">
+        <v>0.06</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -810,17 +886,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -831,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1019,17 +1095,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated results (single bin), and moving the PCA reduction stuff in.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,6 +1091,42 @@
     <row r="4" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="I4">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BP4D baseline addition. DISFA retrained on new features. Updated results for DISFA trained models.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
-    <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="BP4D_intensity" sheetId="3" r:id="rId2"/>
+    <sheet name="SEMAINE" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="28">
   <si>
     <t>DEVEL</t>
   </si>
@@ -79,13 +79,34 @@
   </si>
   <si>
     <t>AU45</t>
+  </si>
+  <si>
+    <t>DISFA training with generic PCA and new alignment (masked and bigger), static model</t>
+  </si>
+  <si>
+    <t>DISFA training with generic PCA and new alignment (masked and bigger), dynamic model (per participant)</t>
+  </si>
+  <si>
+    <t>BP4D trained (static), generic PCA</t>
+  </si>
+  <si>
+    <t>DISFA training with generic PCA and new alignment (masked and bigger), dynamic model (per video)</t>
+  </si>
+  <si>
+    <t>DISFA training with generic PCA and new alignment (masked and bigger), dynamic model</t>
+  </si>
+  <si>
+    <t>SEMAINE trained (static), generic PCA</t>
+  </si>
+  <si>
+    <t>SEMAINE trained (dynamic) generic PCA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +117,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,11 +150,91 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -127,16 +243,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -227,7 +367,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -262,7 +401,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,30 +576,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="5" customWidth="1"/>
-    <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="2.85546875" customWidth="1"/>
-    <col min="15" max="15" width="4.140625" customWidth="1"/>
-    <col min="16" max="16" width="3" customWidth="1"/>
-    <col min="17" max="17" width="2.85546875" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" customWidth="1"/>
-    <col min="19" max="19" width="3" customWidth="1"/>
+    <col min="1" max="1" width="70.5703125" customWidth="1"/>
+    <col min="2" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="10" width="5.140625" customWidth="1"/>
+    <col min="11" max="12" width="4.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" customWidth="1"/>
+    <col min="17" max="17" width="6" customWidth="1"/>
+    <col min="18" max="18" width="5" customWidth="1"/>
+    <col min="19" max="19" width="5.5703125" customWidth="1"/>
     <col min="20" max="20" width="5" customWidth="1"/>
-    <col min="21" max="22" width="6" customWidth="1"/>
-    <col min="23" max="23" width="2.85546875" customWidth="1"/>
-    <col min="24" max="24" width="4.140625" customWidth="1"/>
-    <col min="25" max="25" width="3" customWidth="1"/>
+    <col min="21" max="21" width="4.85546875" customWidth="1"/>
+    <col min="22" max="22" width="5.140625" customWidth="1"/>
+    <col min="23" max="25" width="5.42578125" customWidth="1"/>
     <col min="26" max="27" width="6" customWidth="1"/>
     <col min="28" max="29" width="5" customWidth="1"/>
     <col min="30" max="31" width="6" customWidth="1"/>
@@ -470,419 +609,745 @@
     <col min="34" max="34" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:34">
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="L1" s="18"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3" t="s">
+      <c r="O1" s="18"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3" t="s">
+      <c r="R1" s="18"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3" t="s">
+      <c r="U1" s="18"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3" t="s">
+      <c r="X1" s="18"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3" t="s">
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3" t="s">
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="19"/>
+    </row>
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:34">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.48799999999999999</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>0.24099999999999999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>0.32300000000000001</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="12">
         <v>0.69699999999999995</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="13">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="14">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>0.61599999999999999</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>0.10299999999999999</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="7">
         <v>0.17699999999999999</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>0.91800000000000004</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="4">
         <v>0.34</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="7">
         <v>0.496</v>
       </c>
-      <c r="N3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T3">
+      <c r="N3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="3">
         <v>0.98</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="4">
         <v>0.26100000000000001</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="7">
         <v>0.41199999999999998</v>
       </c>
-      <c r="W3" t="s">
-        <v>16</v>
-      </c>
-      <c r="X3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC3">
+      <c r="W3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC3" s="3">
         <v>0.89</v>
       </c>
-      <c r="AD3">
+      <c r="AD3" s="4">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="7">
         <v>5.5E-2</v>
       </c>
-      <c r="AF3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="AF3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
+      <c r="A4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.498</v>
       </c>
       <c r="C4" s="4">
         <v>0.248</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="7">
         <v>0.33100000000000002</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="6">
         <v>0.73699999999999999</v>
       </c>
       <c r="F4" s="4">
         <v>0.09</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="7">
         <v>0.161</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>0.54600000000000004</v>
       </c>
       <c r="I4" s="4">
         <v>0.112</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="7">
         <v>0.186</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>0.91700000000000004</v>
       </c>
       <c r="L4" s="4">
         <v>0.36599999999999999</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="7">
         <v>0.52300000000000002</v>
       </c>
-      <c r="T4">
+      <c r="N4" s="3"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="3">
         <v>0.97</v>
       </c>
       <c r="U4" s="4">
         <v>0.28699999999999998</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="7">
         <v>0.443</v>
       </c>
-      <c r="Z4">
+      <c r="W4" s="3"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="3">
         <v>9.4E-2</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="5">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="8">
         <v>0.06</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC4" s="3">
         <v>0.88600000000000001</v>
       </c>
       <c r="AD4" s="4">
         <v>3.1E-2</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AE4" s="7">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="7"/>
+    </row>
+    <row r="5" spans="1:34">
+      <c r="A5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.311</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.122</v>
+      </c>
+      <c r="J5">
+        <v>0.193</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0.433</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="3">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U5" s="4">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="V5" s="7">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="W5" s="3"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="7"/>
+    </row>
+    <row r="6" spans="1:34" ht="16.5" customHeight="1">
+      <c r="A6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.223</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.376</v>
+      </c>
+      <c r="I6">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="J6">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="L6">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="M6">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="3">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0.42</v>
+      </c>
+      <c r="V6" s="8">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="W6" s="3"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="3">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AB6" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0.751</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>0.104</v>
+      </c>
+      <c r="AE6" s="8">
+        <v>0.182</v>
+      </c>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="7"/>
+    </row>
+    <row r="7" spans="1:34">
+      <c r="A7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.127</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.113</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="3">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="U7" s="4">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="V7" s="7">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="W7" s="3"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="6">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="AB7" s="7">
+        <v>2E-3</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="AE7" s="7">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="7"/>
+    </row>
+    <row r="8" spans="1:34">
+      <c r="A8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.42809999999999998</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.37480000000000002</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.25259999999999999</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.43859999999999999</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.3206</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.39050000000000001</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0.56469999999999998</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.4617</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.68940000000000001</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0.88360000000000005</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.77449999999999997</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.66279999999999994</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0.77190000000000003</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>0.77070000000000005</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0.95709999999999995</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0.85389999999999999</v>
+      </c>
+      <c r="T8" s="3">
+        <v>0.82889999999999997</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0.92810000000000004</v>
+      </c>
+      <c r="V8" s="7">
+        <v>0.87570000000000003</v>
+      </c>
+      <c r="W8" s="6">
+        <v>0.52159999999999995</v>
+      </c>
+      <c r="X8" s="5">
+        <v>0.8659</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="7"/>
+    </row>
+    <row r="9" spans="1:34">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:34">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:34">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:34">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:34">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:34">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:34">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:34">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -904,16 +1369,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AH8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="63.85546875" customWidth="1"/>
     <col min="2" max="11" width="6" customWidth="1"/>
     <col min="12" max="12" width="5" customWidth="1"/>
     <col min="13" max="14" width="6" customWidth="1"/>
@@ -923,54 +1402,54 @@
     <col min="19" max="19" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:34">
+      <c r="B1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3" t="s">
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="20"/>
+    </row>
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1029,8 +1508,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -1054,7 +1533,7 @@
       <c r="H3">
         <v>0.20899999999999999</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>0.61299999999999999</v>
       </c>
       <c r="J3">
@@ -1088,45 +1567,209 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:34">
+      <c r="A4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>0.46899999999999997</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>0.51100000000000001</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>0.48899999999999999</v>
       </c>
       <c r="E4">
         <v>0.51600000000000001</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <v>0.46300000000000002</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4">
         <v>0.48799999999999999</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <v>0.23899999999999999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>0.61199999999999999</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4">
         <v>0.34300000000000003</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <v>0.54600000000000004</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4">
         <v>0.379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="15" customHeight="1">
+      <c r="A5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>0.16</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="D5">
+        <v>0.248</v>
+      </c>
+      <c r="E5">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="F5">
+        <v>0.372</v>
+      </c>
+      <c r="G5">
+        <v>0.439</v>
+      </c>
+      <c r="H5">
+        <v>0.02</v>
+      </c>
+      <c r="I5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K5">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="L5">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="M5">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="15" customHeight="1">
+      <c r="A6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="C6">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="F6">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="I6">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.311</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
+      <c r="A7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>0.23719999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.36880000000000002</v>
+      </c>
+      <c r="D7">
+        <v>0.28870000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.52629999999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.4753</v>
+      </c>
+      <c r="G7">
+        <v>0.4995</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="I7">
+        <v>0.1711</v>
+      </c>
+      <c r="J7">
+        <v>0.21859999999999999</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.36120000000000002</v>
+      </c>
+      <c r="L7">
+        <v>0.45269999999999999</v>
+      </c>
+      <c r="M7">
+        <v>0.40179999999999999</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.75680000000000003</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>5.0700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
+      <c r="A8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.62619999999999998</v>
+      </c>
+      <c r="C8">
+        <v>0.42080000000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.50329999999999997</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.67179999999999995</v>
+      </c>
+      <c r="F8">
+        <v>0.45319999999999999</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.54120000000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.2737</v>
+      </c>
+      <c r="I8">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="J8">
+        <v>0.10100000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1144,17 +1787,6 @@
     <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New BP4D baseline results.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="29">
   <si>
     <t>DEVEL</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>SEMAINE trained (dynamic) generic PCA</t>
+  </si>
+  <si>
+    <t>BP4D trained (dynamic) generic PCA</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -277,6 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -579,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -601,12 +605,13 @@
     <col min="21" max="21" width="4.85546875" customWidth="1"/>
     <col min="22" max="22" width="5.140625" customWidth="1"/>
     <col min="23" max="25" width="5.42578125" customWidth="1"/>
-    <col min="26" max="27" width="6" customWidth="1"/>
+    <col min="26" max="27" width="5.28515625" customWidth="1"/>
     <col min="28" max="29" width="5" customWidth="1"/>
-    <col min="30" max="31" width="6" customWidth="1"/>
-    <col min="32" max="32" width="2.85546875" customWidth="1"/>
-    <col min="33" max="33" width="4.140625" customWidth="1"/>
-    <col min="34" max="34" width="3" customWidth="1"/>
+    <col min="30" max="30" width="5.7109375" customWidth="1"/>
+    <col min="31" max="31" width="5.42578125" customWidth="1"/>
+    <col min="32" max="32" width="4.85546875" customWidth="1"/>
+    <col min="33" max="33" width="5.5703125" customWidth="1"/>
+    <col min="34" max="34" width="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -660,7 +665,7 @@
       </c>
       <c r="AD1" s="18"/>
       <c r="AE1" s="19"/>
-      <c r="AF1" s="17" t="s">
+      <c r="AF1" s="18" t="s">
         <v>15</v>
       </c>
       <c r="AG1" s="18"/>
@@ -760,7 +765,7 @@
       <c r="AE2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AF2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="AG2" s="10" t="s">
@@ -864,7 +869,7 @@
       <c r="AE3" s="7">
         <v>5.5E-2</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AF3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="AG3" s="4" t="s">
@@ -950,7 +955,7 @@
       <c r="AE4" s="7">
         <v>0.06</v>
       </c>
-      <c r="AF4" s="3"/>
+      <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
       <c r="AH4" s="7"/>
     </row>
@@ -970,10 +975,10 @@
       <c r="E5" s="3">
         <v>0.30299999999999999</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>0.31900000000000001</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>0.311</v>
       </c>
       <c r="H5" s="3">
@@ -982,7 +987,7 @@
       <c r="I5" s="4">
         <v>0.122</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="7">
         <v>0.193</v>
       </c>
       <c r="K5" s="3">
@@ -1030,7 +1035,7 @@
       <c r="AE5" s="7">
         <v>0</v>
       </c>
-      <c r="AF5" s="3"/>
+      <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
       <c r="AH5" s="7"/>
     </row>
@@ -1059,19 +1064,19 @@
       <c r="H6" s="3">
         <v>0.376</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>0.28699999999999998</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="7">
         <v>0.32500000000000001</v>
       </c>
       <c r="K6" s="6">
         <v>0.95699999999999996</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="4">
         <v>0.39200000000000002</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="7">
         <v>0.55600000000000005</v>
       </c>
       <c r="N6" s="3"/>
@@ -1110,7 +1115,7 @@
       <c r="AE6" s="8">
         <v>0.182</v>
       </c>
-      <c r="AF6" s="3"/>
+      <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
       <c r="AH6" s="7"/>
     </row>
@@ -1190,7 +1195,7 @@
       <c r="AE7" s="7">
         <v>0.13200000000000001</v>
       </c>
-      <c r="AF7" s="3"/>
+      <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
       <c r="AH7" s="7"/>
     </row>
@@ -1270,30 +1275,227 @@
       <c r="Y8" s="8">
         <v>0.65100000000000002</v>
       </c>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="4"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="7"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="4"/>
-      <c r="AH8" s="7"/>
+      <c r="Z8" s="3">
+        <v>0.3372</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>0.64849999999999997</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>0.44369999999999998</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0.50590000000000002</v>
+      </c>
+      <c r="AD8" s="21">
+        <v>0.79569999999999996</v>
+      </c>
+      <c r="AE8" s="7">
+        <v>0.61850000000000005</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>0.4118</v>
+      </c>
+      <c r="AG8" s="21">
+        <v>0.49659999999999999</v>
+      </c>
+      <c r="AH8" s="7">
+        <v>0.45019999999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" s="1"/>
+      <c r="A9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.39240000000000003</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0.47739999999999999</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.43080000000000002</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.37469999999999998</v>
+      </c>
+      <c r="F9" s="21">
+        <v>0.25240000000000001</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.30159999999999998</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="7"/>
     </row>
     <row r="10" spans="1:34">
       <c r="A10" s="1"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="7"/>
     </row>
     <row r="11" spans="1:34">
       <c r="A11" s="1"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="7"/>
     </row>
     <row r="12" spans="1:34">
       <c r="A12" s="1"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="7"/>
     </row>
     <row r="13" spans="1:34">
       <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="7"/>
     </row>
     <row r="14" spans="1:34">
       <c r="A14" s="1"/>
@@ -1351,17 +1553,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1774,17 +1976,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Some more results, something is odd about AU1, AU2 BP4D static though.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
-    <sheet name="BP4D_intensity" sheetId="3" r:id="rId2"/>
-    <sheet name="SEMAINE" sheetId="2" r:id="rId3"/>
+    <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
+    <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>DEVEL</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>DISFA train, gen PCA, dynamic model (p. video)</t>
+  </si>
+  <si>
+    <t>BP4D trained (static), specific PCA</t>
+  </si>
+  <si>
+    <t>BP4D trained (dynamic) specific PCA</t>
+  </si>
+  <si>
+    <t>SEMAINE MLP static</t>
+  </si>
+  <si>
+    <t>SEMAINE MLP dynamic</t>
+  </si>
+  <si>
+    <t>SEMAINE MLP joint</t>
+  </si>
+  <si>
+    <t>SEMAINE MLP pretrained</t>
   </si>
 </sst>
 </file>
@@ -279,18 +297,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -305,6 +311,18 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -610,7 +628,7 @@
   <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH13" sqref="AH13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,66 +638,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="7" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="7" t="s">
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="7" t="s">
+      <c r="O1" s="21"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="7" t="s">
+      <c r="R1" s="21"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="8"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="7" t="s">
+      <c r="U1" s="21"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="7" t="s">
+      <c r="X1" s="21"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="7" t="s">
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="8" t="s">
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="8" t="s">
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="9"/>
+      <c r="AJ1" s="21"/>
+      <c r="AK1" s="22"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -798,114 +816,114 @@
       <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="11">
         <v>0.48799999999999999</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="12">
         <v>0.24099999999999999</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="13">
         <v>0.32300000000000001</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="18">
         <v>0.69699999999999995</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="19">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="20">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="16">
         <v>0.61599999999999999</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="12">
         <v>0.10299999999999999</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="13">
         <v>0.17699999999999999</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="11">
         <v>0.91800000000000004</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="12">
         <v>0.34</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="13">
         <v>0.496</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="S3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="15">
+      <c r="T3" s="11">
         <v>0.98</v>
       </c>
-      <c r="U3" s="16">
+      <c r="U3" s="12">
         <v>0.26100000000000001</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="13">
         <v>0.41199999999999998</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="W3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Y3" s="17" t="s">
+      <c r="Y3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="15" t="s">
+      <c r="Z3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="16" t="s">
+      <c r="AA3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="17" t="s">
+      <c r="AB3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="15">
+      <c r="AC3" s="11">
         <v>0.89</v>
       </c>
-      <c r="AD3" s="16">
+      <c r="AD3" s="12">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AE3" s="17">
+      <c r="AE3" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="AF3" s="16" t="s">
+      <c r="AF3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AG3" s="16" t="s">
+      <c r="AG3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AH3" s="17" t="s">
+      <c r="AH3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="22">
+      <c r="AI3" s="18">
         <f>AVERAGE(B3,E3,H3,K3,N3,Q3,T3,W3,Z3,AC3,AF3)</f>
         <v>0.76483333333333337</v>
       </c>
-      <c r="AJ3" s="23">
+      <c r="AJ3" s="19">
         <f t="shared" ref="AJ3:AK3" si="0">AVERAGE(C3,F3,I3,L3,O3,R3,U3,X3,AA3,AD3,AG3)</f>
         <v>0.17583333333333331</v>
       </c>
-      <c r="AK3" s="24">
+      <c r="AK3" s="20">
         <f t="shared" si="0"/>
         <v>0.26816666666666661</v>
       </c>
@@ -914,91 +932,91 @@
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="11">
         <v>0.498</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="12">
         <v>0.248</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="13">
         <v>0.33100000000000002</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="16">
         <v>0.73699999999999999</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="12">
         <v>0.09</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="13">
         <v>0.161</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="11">
         <v>0.54600000000000004</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="12">
         <v>0.112</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="13">
         <v>0.186</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="11">
         <v>0.91700000000000004</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="12">
         <v>0.36599999999999999</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="13">
         <v>0.52300000000000002</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="15">
+      <c r="N4" s="11"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="11">
         <v>0.97</v>
       </c>
-      <c r="U4" s="16">
+      <c r="U4" s="12">
         <v>0.28699999999999998</v>
       </c>
-      <c r="V4" s="17">
+      <c r="V4" s="13">
         <v>0.443</v>
       </c>
-      <c r="W4" s="15"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="15">
+      <c r="W4" s="11"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="11">
         <v>9.4E-2</v>
       </c>
-      <c r="AA4" s="18">
+      <c r="AA4" s="14">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AB4" s="21">
+      <c r="AB4" s="17">
         <v>0.06</v>
       </c>
-      <c r="AC4" s="15">
+      <c r="AC4" s="11">
         <v>0.88600000000000001</v>
       </c>
-      <c r="AD4" s="16">
+      <c r="AD4" s="12">
         <v>3.1E-2</v>
       </c>
-      <c r="AE4" s="17">
+      <c r="AE4" s="13">
         <v>0.06</v>
       </c>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="17"/>
-      <c r="AI4" s="15">
-        <f t="shared" ref="AI4:AI13" si="1">AVERAGE(B4,E4,H4,K4,N4,Q4,T4,W4,Z4,AC4,AF4)</f>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="11">
+        <f t="shared" ref="AI4:AI9" si="1">AVERAGE(B4,E4,H4,K4,N4,Q4,T4,W4,Z4,AC4,AF4)</f>
         <v>0.66399999999999992</v>
       </c>
-      <c r="AJ4" s="16">
-        <f t="shared" ref="AJ4:AJ13" si="2">AVERAGE(C4,F4,I4,L4,O4,R4,U4,X4,AA4,AD4,AG4)</f>
+      <c r="AJ4" s="12">
+        <f t="shared" ref="AJ4:AJ10" si="2">AVERAGE(C4,F4,I4,L4,O4,R4,U4,X4,AA4,AD4,AG4)</f>
         <v>0.16657142857142856</v>
       </c>
-      <c r="AK4" s="17">
-        <f t="shared" ref="AK4:AK13" si="3">AVERAGE(D4,G4,J4,M4,P4,S4,V4,Y4,AB4,AE4,AH4)</f>
+      <c r="AK4" s="13">
+        <f t="shared" ref="AK4:AK10" si="3">AVERAGE(D4,G4,J4,M4,P4,S4,V4,Y4,AB4,AE4,AH4)</f>
         <v>0.25200000000000006</v>
       </c>
     </row>
@@ -1006,90 +1024,90 @@
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="11">
         <v>0.39</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="12">
         <v>0.27900000000000003</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="13">
         <v>0.32500000000000001</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <v>0.30299999999999999</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="12">
         <v>0.31900000000000001</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="13">
         <v>0.311</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="11">
         <v>0.46</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="12">
         <v>0.122</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="13">
         <v>0.193</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="11">
         <v>0.94599999999999995</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="12">
         <v>0.28000000000000003</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="13">
         <v>0.433</v>
       </c>
-      <c r="N5" s="15"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="15">
+      <c r="N5" s="11"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="11">
         <v>0.96499999999999997</v>
       </c>
-      <c r="U5" s="16">
+      <c r="U5" s="12">
         <v>0.23699999999999999</v>
       </c>
-      <c r="V5" s="17">
+      <c r="V5" s="13">
         <v>0.38100000000000001</v>
       </c>
-      <c r="W5" s="15"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="15">
+      <c r="W5" s="11"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="11">
         <v>0</v>
       </c>
-      <c r="AA5" s="16">
+      <c r="AA5" s="12">
         <v>0</v>
       </c>
-      <c r="AB5" s="17">
+      <c r="AB5" s="13">
         <v>0</v>
       </c>
-      <c r="AC5" s="15">
+      <c r="AC5" s="11">
         <v>0</v>
       </c>
-      <c r="AD5" s="16">
+      <c r="AD5" s="12">
         <v>0</v>
       </c>
-      <c r="AE5" s="17">
+      <c r="AE5" s="13">
         <v>0</v>
       </c>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="17"/>
-      <c r="AI5" s="15">
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="11">
         <f t="shared" si="1"/>
         <v>0.43771428571428572</v>
       </c>
-      <c r="AJ5" s="16">
+      <c r="AJ5" s="12">
         <f t="shared" si="2"/>
         <v>0.17671428571428574</v>
       </c>
-      <c r="AK5" s="17">
+      <c r="AK5" s="13">
         <f t="shared" si="3"/>
         <v>0.23471428571428571</v>
       </c>
@@ -1098,90 +1116,90 @@
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="11">
         <v>0.52600000000000002</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="12">
         <v>0.35099999999999998</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="17">
         <v>0.42099999999999999</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="11">
         <v>0.50800000000000001</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="12">
         <v>0.223</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="13">
         <v>0.31</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="11">
         <v>0.376</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="12">
         <v>0.28699999999999998</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="13">
         <v>0.32500000000000001</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="16">
         <v>0.95699999999999996</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="12">
         <v>0.39200000000000002</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="13">
         <v>0.55600000000000005</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="15">
+      <c r="N6" s="11"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="11">
         <v>0.94599999999999995</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="14">
         <v>0.42</v>
       </c>
-      <c r="V6" s="21">
+      <c r="V6" s="17">
         <v>0.58199999999999996</v>
       </c>
-      <c r="W6" s="15"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="15">
+      <c r="W6" s="11"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="11">
         <v>0.35699999999999998</v>
       </c>
-      <c r="AA6" s="16">
+      <c r="AA6" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AB6" s="17">
+      <c r="AB6" s="13">
         <v>0.01</v>
       </c>
-      <c r="AC6" s="15">
+      <c r="AC6" s="11">
         <v>0.751</v>
       </c>
-      <c r="AD6" s="18">
+      <c r="AD6" s="14">
         <v>0.104</v>
       </c>
-      <c r="AE6" s="21">
+      <c r="AE6" s="17">
         <v>0.182</v>
       </c>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="15">
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="11">
         <f t="shared" si="1"/>
         <v>0.63157142857142856</v>
       </c>
-      <c r="AJ6" s="16">
+      <c r="AJ6" s="12">
         <f t="shared" si="2"/>
         <v>0.25457142857142856</v>
       </c>
-      <c r="AK6" s="17">
+      <c r="AK6" s="13">
         <f t="shared" si="3"/>
         <v>0.3408571428571428</v>
       </c>
@@ -1190,90 +1208,90 @@
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="16">
         <v>0.59199999999999997</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>0.22600000000000001</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>0.32800000000000001</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="11">
         <v>0.54300000000000004</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>0.127</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="13">
         <v>0.20599999999999999</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="11">
         <v>0.29599999999999999</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="12">
         <v>0.113</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="13">
         <v>0.16400000000000001</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="11">
         <v>0.91600000000000004</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="12">
         <v>0.17799999999999999</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="13">
         <v>0.29799999999999999</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="15">
+      <c r="N7" s="11"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="11">
         <v>0.93799999999999994</v>
       </c>
-      <c r="U7" s="16">
+      <c r="U7" s="12">
         <v>0.25800000000000001</v>
       </c>
-      <c r="V7" s="17">
+      <c r="V7" s="13">
         <v>0.40500000000000003</v>
       </c>
-      <c r="W7" s="15"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="20">
+      <c r="W7" s="11"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="16">
         <v>0.61899999999999999</v>
       </c>
-      <c r="AA7" s="16">
+      <c r="AA7" s="12">
         <v>1E-3</v>
       </c>
-      <c r="AB7" s="17">
+      <c r="AB7" s="13">
         <v>2E-3</v>
       </c>
-      <c r="AC7" s="15">
+      <c r="AC7" s="11">
         <v>0.85099999999999998</v>
       </c>
-      <c r="AD7" s="16">
+      <c r="AD7" s="12">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="AE7" s="17">
+      <c r="AE7" s="13">
         <v>0.13200000000000001</v>
       </c>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="17"/>
-      <c r="AI7" s="15">
+      <c r="AF7" s="12"/>
+      <c r="AG7" s="12"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="11">
         <f t="shared" si="1"/>
         <v>0.67928571428571427</v>
       </c>
-      <c r="AJ7" s="16">
+      <c r="AJ7" s="12">
         <f t="shared" si="2"/>
         <v>0.13928571428571426</v>
       </c>
-      <c r="AK7" s="17">
+      <c r="AK7" s="13">
         <f t="shared" si="3"/>
         <v>0.21928571428571431</v>
       </c>
@@ -1282,114 +1300,114 @@
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="11">
         <v>0.33300000000000002</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <v>0.42809999999999998</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="13">
         <v>0.37480000000000002</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="11">
         <v>0.25259999999999999</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="14">
         <v>0.43859999999999999</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <v>0.3206</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="11">
         <v>0.39050000000000001</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="14">
         <v>0.56469999999999998</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="17">
         <v>0.4617</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="11">
         <v>0.68940000000000001</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <v>0.88360000000000005</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="17">
         <v>0.77449999999999997</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="11">
         <v>0.66279999999999994</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="14">
         <v>0.92400000000000004</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="13">
         <v>0.77190000000000003</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="16">
         <v>0.77070000000000005</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="14">
         <v>0.95709999999999995</v>
       </c>
-      <c r="S8" s="21">
+      <c r="S8" s="17">
         <v>0.85389999999999999</v>
       </c>
-      <c r="T8" s="15">
+      <c r="T8" s="11">
         <v>0.82889999999999997</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="14">
         <v>0.92810000000000004</v>
       </c>
-      <c r="V8" s="17">
+      <c r="V8" s="13">
         <v>0.87570000000000003</v>
       </c>
-      <c r="W8" s="20">
+      <c r="W8" s="16">
         <v>0.52159999999999995</v>
       </c>
-      <c r="X8" s="18">
+      <c r="X8" s="14">
         <v>0.8659</v>
       </c>
-      <c r="Y8" s="21">
+      <c r="Y8" s="17">
         <v>0.65100000000000002</v>
       </c>
-      <c r="Z8" s="15">
+      <c r="Z8" s="11">
         <v>0.3372</v>
       </c>
-      <c r="AA8" s="18">
+      <c r="AA8" s="14">
         <v>0.64849999999999997</v>
       </c>
-      <c r="AB8" s="17">
+      <c r="AB8" s="13">
         <v>0.44369999999999998</v>
       </c>
-      <c r="AC8" s="15">
+      <c r="AC8" s="11">
         <v>0.50590000000000002</v>
       </c>
-      <c r="AD8" s="16">
+      <c r="AD8" s="12">
         <v>0.79569999999999996</v>
       </c>
-      <c r="AE8" s="17">
+      <c r="AE8" s="13">
         <v>0.61850000000000005</v>
       </c>
-      <c r="AF8" s="16">
+      <c r="AF8" s="12">
         <v>0.4118</v>
       </c>
-      <c r="AG8" s="16">
+      <c r="AG8" s="12">
         <v>0.49659999999999999</v>
       </c>
-      <c r="AH8" s="17">
+      <c r="AH8" s="13">
         <v>0.45019999999999999</v>
       </c>
-      <c r="AI8" s="15">
+      <c r="AI8" s="11">
         <f t="shared" si="1"/>
         <v>0.51858181818181825</v>
       </c>
-      <c r="AJ8" s="16">
+      <c r="AJ8" s="12">
         <f t="shared" si="2"/>
         <v>0.72099090909090902</v>
       </c>
-      <c r="AK8" s="17">
+      <c r="AK8" s="13">
         <f t="shared" si="3"/>
         <v>0.59968181818181809</v>
       </c>
@@ -1398,219 +1416,313 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="11">
         <v>0.39240000000000003</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>0.47739999999999999</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <v>0.43080000000000002</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="11">
         <v>0.37469999999999998</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>0.25240000000000001</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="13">
         <v>0.30159999999999998</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="17"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="17"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="17"/>
-      <c r="AI9" s="15">
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="12"/>
+      <c r="AH9" s="12"/>
+      <c r="AI9" s="11">
         <f t="shared" si="1"/>
         <v>0.38355</v>
       </c>
-      <c r="AJ9" s="16">
+      <c r="AJ9" s="12">
         <f t="shared" si="2"/>
         <v>0.3649</v>
       </c>
-      <c r="AK9" s="17">
+      <c r="AK9" s="13">
         <f t="shared" si="3"/>
         <v>0.36619999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="12"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="14"/>
-      <c r="AI10" s="12"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="14"/>
+      <c r="A10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.3664</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.47889999999999999</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.41510000000000002</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="10"/>
+      <c r="AI10" s="11">
+        <f>AVERAGE(B10,E10,H10,K10,N10,Q10,T10,W10,Z10,AC10,AF10)</f>
+        <v>0.3664</v>
+      </c>
+      <c r="AJ10" s="12">
+        <f t="shared" si="2"/>
+        <v>0.47889999999999999</v>
+      </c>
+      <c r="AK10" s="13">
+        <f t="shared" si="3"/>
+        <v>0.41510000000000002</v>
+      </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="13"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13"/>
-      <c r="AH11" s="14"/>
-      <c r="AI11" s="12"/>
-      <c r="AJ11" s="13"/>
-      <c r="AK11" s="14"/>
+      <c r="A11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.39410000000000001</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.47189999999999999</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.42949999999999999</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.31580000000000003</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.30869999999999997</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.31219999999999998</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.64290000000000003</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.53349999999999997</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.6925</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="M11" s="10">
+        <v>0.78569999999999995</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.65669999999999995</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0.89770000000000005</v>
+      </c>
+      <c r="P11" s="10">
+        <v>0.75849999999999995</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0.88260000000000005</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0.38340000000000002</v>
+      </c>
+      <c r="S11" s="10">
+        <v>0.53459999999999996</v>
+      </c>
+      <c r="T11" s="8">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="U11" s="9">
+        <v>0.66849999999999998</v>
+      </c>
+      <c r="V11" s="10">
+        <v>0.76490000000000002</v>
+      </c>
+      <c r="W11" s="8">
+        <v>0.46829999999999999</v>
+      </c>
+      <c r="X11" s="9">
+        <v>0.94679999999999997</v>
+      </c>
+      <c r="Y11" s="10">
+        <v>0.62670000000000003</v>
+      </c>
+      <c r="Z11" s="8">
+        <v>0.4219</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="AB11" s="10">
+        <v>0.4032</v>
+      </c>
+      <c r="AC11" s="8">
+        <v>0.51690000000000003</v>
+      </c>
+      <c r="AD11" s="9">
+        <v>0.79259999999999997</v>
+      </c>
+      <c r="AE11" s="10">
+        <v>0.62570000000000003</v>
+      </c>
+      <c r="AF11" s="9">
+        <v>0.42659999999999998</v>
+      </c>
+      <c r="AG11" s="9">
+        <v>0.40439999999999998</v>
+      </c>
+      <c r="AH11" s="10">
+        <v>0.41520000000000001</v>
+      </c>
+      <c r="AI11" s="11">
+        <f t="shared" ref="AI11:AI13" si="4">AVERAGE(B11,E11,H11,K11,N11,Q11,T11,W11,Z11,AC11,AF11)</f>
+        <v>0.55684545454545453</v>
+      </c>
+      <c r="AJ11" s="12">
+        <f t="shared" ref="AJ11:AJ13" si="5">AVERAGE(C11,F11,I11,L11,O11,R11,U11,X11,AA11,AD11,AG11)</f>
+        <v>0.6191545454545454</v>
+      </c>
+      <c r="AK11" s="13">
+        <f t="shared" ref="AK11:AK13" si="6">AVERAGE(D11,G11,J11,M11,P11,S11,V11,Y11,AB11,AE11,AH11)</f>
+        <v>0.56269999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="13"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="12"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="13"/>
-      <c r="AG12" s="13"/>
-      <c r="AH12" s="14"/>
-      <c r="AI12" s="12"/>
-      <c r="AJ12" s="13"/>
-      <c r="AK12" s="14"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="12"/>
+      <c r="AK12" s="13"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="13"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="13"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="14"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="13"/>
-      <c r="AK13" s="14"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="10"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="12"/>
+      <c r="AK13" s="13"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -1682,6 +1794,138 @@
     <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G9">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J9">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M9">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P9">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S9">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V9">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y9">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB9">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE9">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH9">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK3:AK13">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -1693,7 +1937,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G9">
+  <conditionalFormatting sqref="D3:D11">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1705,7 +1949,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -1717,7 +1961,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M9">
+  <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -1729,7 +1973,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P9">
+  <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1741,7 +1985,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S9">
+  <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1753,7 +1997,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V9">
+  <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1765,7 +2009,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y9">
+  <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1777,7 +2021,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB9">
+  <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1789,7 +2033,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE9">
+  <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1801,7 +2045,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH9">
+  <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1813,7 +2057,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK3:AK9">
+  <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1832,24 +2076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,53 +2104,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="7" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="7" t="s">
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="7" t="s">
+      <c r="O1" s="21"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="7" t="s">
+      <c r="R1" s="21"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="8"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1994,57 +2224,57 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="11">
         <v>0.46100000000000002</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="12">
         <v>0.45700000000000002</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="13">
         <v>0.45900000000000002</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <v>0.52400000000000002</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="12">
         <v>0.45500000000000002</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="13">
         <v>0.48699999999999999</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="11">
         <v>0.20899999999999999</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="14">
         <v>0.61299999999999999</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="13">
         <v>0.312</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="11">
         <v>0.28799999999999998</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="12">
         <v>0.54100000000000004</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="13">
         <v>0.376</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="12">
+      <c r="N3" s="11"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="8">
         <f>AVERAGE(B3,E3,H3,K3,N3,Q3)</f>
         <v>0.37050000000000005</v>
       </c>
-      <c r="U3" s="13">
+      <c r="U3" s="9">
         <f>AVERAGE(C3,F3,I3,L3,O3,R3)</f>
         <v>0.51649999999999996</v>
       </c>
-      <c r="V3" s="14">
+      <c r="V3" s="10">
         <f>AVERAGE(D3,G3,J3,M3,P3,S3)</f>
         <v>0.40849999999999997</v>
       </c>
@@ -2053,57 +2283,57 @@
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="11">
         <v>0.46899999999999997</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="12">
         <v>0.51100000000000001</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="13">
         <v>0.48899999999999999</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <v>0.51600000000000001</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="12">
         <v>0.46300000000000002</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="13">
         <v>0.48799999999999999</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="11">
         <v>0.23899999999999999</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
         <v>0.61199999999999999</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="13">
         <v>0.34300000000000003</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="12">
         <v>0.54600000000000004</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="13">
         <v>0.379</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="12">
+      <c r="N4" s="11"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="8">
         <f t="shared" ref="T4:T8" si="0">AVERAGE(B4,E4,H4,K4,N4,Q4)</f>
         <v>0.3785</v>
       </c>
-      <c r="U4" s="13">
+      <c r="U4" s="9">
         <f t="shared" ref="U4:U8" si="1">AVERAGE(C4,F4,I4,L4,O4,R4)</f>
         <v>0.53299999999999992</v>
       </c>
-      <c r="V4" s="14">
+      <c r="V4" s="10">
         <f t="shared" ref="V4:V8" si="2">AVERAGE(D4,G4,J4,M4,P4,S4)</f>
         <v>0.42475000000000002</v>
       </c>
@@ -2112,57 +2342,57 @@
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="11">
         <v>0.16</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="15">
         <v>0.55500000000000005</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="13">
         <v>0.248</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <v>0.53600000000000003</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="12">
         <v>0.372</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="13">
         <v>0.439</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="11">
         <v>0.02</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="12">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="13">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="11">
         <v>0.30199999999999999</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="12">
         <v>0.65200000000000002</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="13">
         <v>0.41199999999999998</v>
       </c>
-      <c r="N5" s="15"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="12">
+      <c r="N5" s="11"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="8">
         <f t="shared" si="0"/>
         <v>0.2545</v>
       </c>
-      <c r="U5" s="13">
+      <c r="U5" s="9">
         <f t="shared" si="1"/>
         <v>0.39550000000000002</v>
       </c>
-      <c r="V5" s="14">
+      <c r="V5" s="10">
         <f t="shared" si="2"/>
         <v>0.27600000000000002</v>
       </c>
@@ -2171,57 +2401,57 @@
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="11">
         <v>0.40400000000000003</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="12">
         <v>0.51200000000000001</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="13">
         <v>0.45200000000000001</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="11">
         <v>0.52800000000000002</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="12">
         <v>0.38400000000000001</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="13">
         <v>0.44400000000000001</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="16">
         <v>0.27300000000000002</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="12">
         <v>0.54400000000000004</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="17">
         <v>0.36299999999999999</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="11">
         <v>0.311</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="14">
         <v>0.77700000000000002</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="17">
         <v>0.44400000000000001</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="12">
+      <c r="N6" s="11"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="8">
         <f t="shared" si="0"/>
         <v>0.379</v>
       </c>
-      <c r="U6" s="13">
+      <c r="U6" s="9">
         <f t="shared" si="1"/>
         <v>0.55425000000000002</v>
       </c>
-      <c r="V6" s="14">
+      <c r="V6" s="10">
         <f t="shared" si="2"/>
         <v>0.42574999999999996</v>
       </c>
@@ -2230,69 +2460,69 @@
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="11">
         <v>0.23719999999999999</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>0.36880000000000002</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>0.28870000000000001</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="11">
         <v>0.52629999999999999</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="14">
         <v>0.4753</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="13">
         <v>0.4995</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="16">
         <v>0.30249999999999999</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="12">
         <v>0.1711</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="13">
         <v>0.21859999999999999</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7" s="16">
         <v>0.36120000000000002</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="12">
         <v>0.45269999999999999</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="13">
         <v>0.40179999999999999</v>
       </c>
-      <c r="N7" s="20">
+      <c r="N7" s="16">
         <v>0.75680000000000003</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="14">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="17">
         <v>5.0700000000000002E-2</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="11">
         <v>0.23649999999999999</v>
       </c>
-      <c r="R7" s="18">
+      <c r="R7" s="14">
         <v>0.62429999999999997</v>
       </c>
-      <c r="S7" s="21">
+      <c r="S7" s="17">
         <v>0.34300000000000003</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="8">
         <f t="shared" si="0"/>
         <v>0.40341666666666659</v>
       </c>
-      <c r="U7" s="13">
+      <c r="U7" s="9">
         <f t="shared" si="1"/>
         <v>0.3530666666666667</v>
       </c>
-      <c r="V7" s="14">
+      <c r="V7" s="10">
         <f t="shared" si="2"/>
         <v>0.30038333333333328</v>
       </c>
@@ -2301,69 +2531,69 @@
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="16">
         <v>0.62619999999999998</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="12">
         <v>0.42080000000000001</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="17">
         <v>0.50329999999999997</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="16">
         <v>0.67179999999999995</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="12">
         <v>0.45319999999999999</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <v>0.54120000000000001</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="11">
         <v>0.2737</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="12">
         <v>6.2199999999999998E-2</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="13">
         <v>0.10100000000000001</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="11">
         <v>0.28420000000000001</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="12">
         <v>0.48730000000000001</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="13">
         <v>0.35899999999999999</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="11">
         <v>0.69089999999999996</v>
       </c>
-      <c r="O8" s="16">
+      <c r="O8" s="12">
         <v>3.56E-2</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="13">
         <v>6.7699999999999996E-2</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="11">
         <v>0.35859999999999997</v>
       </c>
-      <c r="R8" s="16">
+      <c r="R8" s="12">
         <v>0.53359999999999996</v>
       </c>
-      <c r="S8" s="17">
+      <c r="S8" s="13">
         <v>0.4289</v>
       </c>
-      <c r="T8" s="12">
+      <c r="T8" s="8">
         <f t="shared" si="0"/>
         <v>0.48423333333333335</v>
       </c>
-      <c r="U8" s="13">
+      <c r="U8" s="9">
         <f t="shared" si="1"/>
         <v>0.33211666666666667</v>
       </c>
-      <c r="V8" s="14">
+      <c r="V8" s="10">
         <f t="shared" si="2"/>
         <v>0.33351666666666668</v>
       </c>
@@ -2372,70 +2602,70 @@
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="8">
         <v>0.17879999999999999</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="9">
         <v>0.53620000000000001</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="10">
         <v>0.2681</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="8">
         <v>0.65390000000000004</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="9">
         <v>0.44230000000000003</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="10">
         <v>0.52769999999999995</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="8">
         <v>5.74E-2</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="9">
         <v>0.55200000000000005</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="10">
         <v>0.10390000000000001</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="8">
         <v>0.28110000000000002</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="9">
         <v>0.70089999999999997</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="10">
         <v>0.40129999999999999</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="8">
         <v>5.7299999999999997E-2</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="9">
         <v>0.72819999999999996</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="10">
         <v>0.10630000000000001</v>
       </c>
-      <c r="Q9" s="12">
+      <c r="Q9" s="8">
         <v>0.19520000000000001</v>
       </c>
-      <c r="R9" s="13">
+      <c r="R9" s="9">
         <v>0.83430000000000004</v>
       </c>
-      <c r="S9" s="14">
+      <c r="S9" s="10">
         <v>0.31630000000000003</v>
       </c>
-      <c r="T9" s="12">
-        <f t="shared" ref="T9:T12" si="3">AVERAGE(B9,E9,H9,K9,N9,Q9)</f>
+      <c r="T9" s="8">
+        <f t="shared" ref="T9:T10" si="3">AVERAGE(B9,E9,H9,K9,N9,Q9)</f>
         <v>0.23728333333333332</v>
       </c>
-      <c r="U9" s="13">
-        <f t="shared" ref="U9:U12" si="4">AVERAGE(C9,F9,I9,L9,O9,R9)</f>
+      <c r="U9" s="9">
+        <f t="shared" ref="U9:U10" si="4">AVERAGE(C9,F9,I9,L9,O9,R9)</f>
         <v>0.63231666666666664</v>
       </c>
-      <c r="V9" s="14">
-        <f t="shared" ref="V9:V12" si="5">AVERAGE(D9,G9,J9,M9,P9,S9)</f>
+      <c r="V9" s="10">
+        <f t="shared" ref="V9:V10" si="5">AVERAGE(D9,G9,J9,M9,P9,S9)</f>
         <v>0.28726666666666667</v>
       </c>
     </row>
@@ -2443,247 +2673,259 @@
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="8">
         <v>0.63719999999999999</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="9">
         <v>0.48530000000000001</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="10">
         <v>0.55100000000000005</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="8">
         <v>0.65390000000000004</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="9">
         <v>0.44230000000000003</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="10">
         <v>0.52769999999999995</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="8">
         <v>0.2051</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="9">
         <v>0.104</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="10">
         <v>0.13800000000000001</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="8">
         <v>0.27329999999999999</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="9">
         <v>0.83299999999999996</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="10">
         <v>0.41160000000000002</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="8">
         <v>1</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="9">
         <v>3.56E-2</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="10">
         <v>6.88E-2</v>
       </c>
-      <c r="Q10" s="12">
+      <c r="Q10" s="8">
         <v>0.34899999999999998</v>
       </c>
-      <c r="R10" s="13">
+      <c r="R10" s="9">
         <v>0.53939999999999999</v>
       </c>
-      <c r="S10" s="14">
+      <c r="S10" s="10">
         <v>0.42380000000000001</v>
       </c>
-      <c r="T10" s="12">
+      <c r="T10" s="8">
         <f t="shared" si="3"/>
         <v>0.51975000000000005</v>
       </c>
-      <c r="U10" s="13">
+      <c r="U10" s="9">
         <f t="shared" si="4"/>
         <v>0.40660000000000002</v>
       </c>
-      <c r="V10" s="14">
+      <c r="V10" s="10">
         <f t="shared" si="5"/>
         <v>0.35348333333333332</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="14"/>
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="10"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="14"/>
+      <c r="A12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="10"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="14"/>
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="10"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="14"/>
+      <c r="A14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="10"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="7">
@@ -2772,4 +3014,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final BP4D statoc PCA results.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1593,23 +1593,35 @@
       <c r="AB10" s="10">
         <v>0.42599999999999999</v>
       </c>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="9"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="10"/>
+      <c r="AC10" s="8">
+        <v>0.503</v>
+      </c>
+      <c r="AD10" s="9">
+        <v>0.79779999999999995</v>
+      </c>
+      <c r="AE10" s="10">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="AF10" s="9">
+        <v>0.32969999999999999</v>
+      </c>
+      <c r="AG10" s="9">
+        <v>0.66320000000000001</v>
+      </c>
+      <c r="AH10" s="10">
+        <v>0.44040000000000001</v>
+      </c>
       <c r="AI10" s="11">
         <f>AVERAGE(B10,E10,H10,K10,N10,Q10,T10,W10,Z10,AC10,AF10)</f>
-        <v>0.54724444444444442</v>
+        <v>0.52344545454545444</v>
       </c>
       <c r="AJ10" s="12">
         <f t="shared" si="2"/>
-        <v>0.67431111111111108</v>
+        <v>0.68452727272727265</v>
       </c>
       <c r="AK10" s="13">
         <f t="shared" si="3"/>
-        <v>0.59762222222222217</v>
+        <v>0.58509090909090911</v>
       </c>
     </row>
     <row r="11" spans="1:37">
@@ -2997,17 +3009,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="7">

</xml_diff>

<commit_message>
Caelum results on BP4D.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" refMode="R1C1"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -141,8 +141,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +413,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -447,6 +448,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -622,20 +624,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
@@ -697,7 +699,7 @@
       <c r="AJ1" s="21"/>
       <c r="AK1" s="22"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -810,7 +812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
@@ -926,7 +928,7 @@
         <v>0.26816666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1018,7 +1020,7 @@
         <v>0.25200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>0.23471428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1">
+    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -1202,7 +1204,7 @@
         <v>0.3408571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
@@ -1294,27 +1296,27 @@
         <v>0.21928571428571431</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="11">
-        <v>0.33300000000000002</v>
+        <v>0.3589</v>
       </c>
       <c r="C8" s="14">
-        <v>0.42809999999999998</v>
+        <v>0.47289999999999999</v>
       </c>
       <c r="D8" s="13">
-        <v>0.37480000000000002</v>
+        <v>0.40810000000000002</v>
       </c>
       <c r="E8" s="11">
-        <v>0.25259999999999999</v>
+        <v>0.29859999999999998</v>
       </c>
       <c r="F8" s="14">
-        <v>0.43859999999999999</v>
+        <v>0.41889999999999999</v>
       </c>
       <c r="G8" s="17">
-        <v>0.3206</v>
+        <v>0.34870000000000001</v>
       </c>
       <c r="H8" s="11">
         <v>0.39050000000000001</v>
@@ -1344,22 +1346,22 @@
         <v>0.77190000000000003</v>
       </c>
       <c r="Q8" s="16">
-        <v>0.77070000000000005</v>
+        <v>0.72309999999999997</v>
       </c>
       <c r="R8" s="14">
-        <v>0.95709999999999995</v>
+        <v>0.77410000000000001</v>
       </c>
       <c r="S8" s="17">
-        <v>0.85389999999999999</v>
+        <v>0.74770000000000003</v>
       </c>
       <c r="T8" s="11">
-        <v>0.82889999999999997</v>
+        <v>0.82520000000000004</v>
       </c>
       <c r="U8" s="14">
-        <v>0.92810000000000004</v>
+        <v>0.76139999999999997</v>
       </c>
       <c r="V8" s="13">
-        <v>0.87570000000000003</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="W8" s="16">
         <v>0.52159999999999995</v>
@@ -1399,18 +1401,18 @@
       </c>
       <c r="AI8" s="11">
         <f t="shared" si="1"/>
-        <v>0.51858181818181825</v>
+        <v>0.5204545454545455</v>
       </c>
       <c r="AJ8" s="12">
         <f t="shared" si="2"/>
-        <v>0.72099090909090902</v>
+        <v>0.6914818181818182</v>
       </c>
       <c r="AK8" s="13">
         <f t="shared" si="3"/>
-        <v>0.59968181818181809</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37">
+        <v>0.58799999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1460,22 +1462,22 @@
         <v>0.75519999999999998</v>
       </c>
       <c r="Q9" s="11">
-        <v>0.73240000000000005</v>
+        <v>0.76339999999999997</v>
       </c>
       <c r="R9" s="12">
-        <v>0.94779999999999998</v>
+        <v>0.70699999999999996</v>
       </c>
       <c r="S9" s="13">
-        <v>0.82630000000000003</v>
+        <v>0.73409999999999997</v>
       </c>
       <c r="T9" s="11">
-        <v>0.79690000000000005</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="U9" s="12">
-        <v>0.91659999999999997</v>
+        <v>0.7732</v>
       </c>
       <c r="V9" s="13">
-        <v>0.85260000000000002</v>
+        <v>0.81389999999999996</v>
       </c>
       <c r="W9" s="11">
         <v>0.46279999999999999</v>
@@ -1486,29 +1488,47 @@
       <c r="Y9" s="13">
         <v>0.62270000000000003</v>
       </c>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="12"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="12"/>
-      <c r="AG9" s="12"/>
-      <c r="AH9" s="12"/>
+      <c r="Z9" s="11">
+        <v>0.41310000000000002</v>
+      </c>
+      <c r="AA9" s="12">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="AB9" s="13">
+        <v>0.38069999999999998</v>
+      </c>
+      <c r="AC9" s="11">
+        <v>0.51229999999999998</v>
+      </c>
+      <c r="AD9" s="12">
+        <v>0.81130000000000002</v>
+      </c>
+      <c r="AE9" s="13">
+        <v>0.628</v>
+      </c>
+      <c r="AF9" s="12">
+        <v>0.42549999999999999</v>
+      </c>
+      <c r="AG9" s="12">
+        <v>0.38590000000000002</v>
+      </c>
+      <c r="AH9" s="12">
+        <v>0.4047</v>
+      </c>
       <c r="AI9" s="11">
         <f t="shared" si="1"/>
-        <v>0.56838749999999993</v>
+        <v>0.54464545454545454</v>
       </c>
       <c r="AJ9" s="12">
         <f t="shared" si="2"/>
-        <v>0.75114999999999998</v>
+        <v>0.65229090909090914</v>
       </c>
       <c r="AK9" s="13">
         <f t="shared" si="3"/>
-        <v>0.63821249999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37">
+        <v>0.58074545454545456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -1624,7 +1644,7 @@
         <v>0.58509090909090911</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
@@ -1740,7 +1760,7 @@
         <v>0.56269999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1779,7 +1799,7 @@
       <c r="AJ12" s="12"/>
       <c r="AK12" s="13"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1818,58 +1838,58 @@
       <c r="AJ13" s="12"/>
       <c r="AK13" s="13"/>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
   </sheetData>
@@ -1890,9 +1910,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1902,9 +1922,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1914,9 +1934,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1926,9 +1946,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1938,9 +1958,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1950,9 +1970,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1962,9 +1982,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1974,9 +1994,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1986,9 +2006,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -1998,9 +2018,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2010,9 +2030,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2022,9 +2042,9 @@
   <conditionalFormatting sqref="AK3:AK13">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2034,9 +2054,9 @@
   <conditionalFormatting sqref="D3:D11">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2046,9 +2066,9 @@
   <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2058,9 +2078,9 @@
   <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2070,9 +2090,9 @@
   <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2082,9 +2102,9 @@
   <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2094,9 +2114,9 @@
   <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2106,9 +2126,9 @@
   <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2118,9 +2138,9 @@
   <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2130,9 +2150,9 @@
   <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2142,9 +2162,9 @@
   <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2154,9 +2174,9 @@
   <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -2169,14 +2189,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.85546875" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -2197,7 +2217,7 @@
     <col min="22" max="22" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" s="23" t="s">
         <v>4</v>
       </c>
@@ -2246,7 +2266,7 @@
       <c r="AG1" s="24"/>
       <c r="AH1" s="24"/>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2314,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" customHeight="1">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -2373,7 +2393,7 @@
         <v>0.40849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -2432,7 +2452,7 @@
         <v>0.42475000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1">
+    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -2491,7 +2511,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1">
+    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -2550,7 +2570,7 @@
         <v>0.42574999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -2621,7 +2641,7 @@
         <v>0.30038333333333328</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -2692,7 +2712,7 @@
         <v>0.33351666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -2763,7 +2783,7 @@
         <v>0.28726666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -2834,7 +2854,7 @@
         <v>0.35348333333333332</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
@@ -2860,7 +2880,7 @@
       <c r="U11" s="9"/>
       <c r="V11" s="10"/>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
@@ -2886,7 +2906,7 @@
       <c r="U12" s="9"/>
       <c r="V12" s="10"/>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -2912,7 +2932,7 @@
       <c r="U13" s="9"/>
       <c r="V13" s="10"/>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -2938,7 +2958,7 @@
       <c r="U14" s="9"/>
       <c r="V14" s="10"/>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -2961,7 +2981,7 @@
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2984,7 +3004,7 @@
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
     </row>
-    <row r="17" spans="2:22">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -3009,24 +3029,24 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3036,9 +3056,9 @@
   <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3048,9 +3068,9 @@
   <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3060,9 +3080,9 @@
   <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3072,9 +3092,9 @@
   <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3084,9 +3104,9 @@
   <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3096,9 +3116,9 @@
   <conditionalFormatting sqref="V3:V10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3111,14 +3131,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify some source files, adding new baselines for BP4D trained and SEMAINE tested (still need to run them though).
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
   <si>
     <t>DEVEL</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>SEMAINE MLP pretrained</t>
+  </si>
+  <si>
+    <t>SEMAINE train, spec PCA (static)</t>
+  </si>
+  <si>
+    <t>SEMAINE train, spec PCA (dynamic)</t>
+  </si>
+  <si>
+    <t>SEMAINE train, gen PCA (static)</t>
+  </si>
+  <si>
+    <t>SEMAINE train, gen PCA (dynamic)</t>
   </si>
 </sst>
 </file>
@@ -285,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -323,6 +335,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -628,7 +642,7 @@
   <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,17 +661,17 @@
         <v>4</v>
       </c>
       <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="23" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
+      <c r="M1" s="21"/>
       <c r="N1" s="23" t="s">
         <v>7</v>
       </c>
@@ -718,7 +732,7 @@
       <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -727,7 +741,7 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -736,7 +750,7 @@
       <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="2" t="s">
@@ -831,7 +845,7 @@
       <c r="F3" s="19">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="19">
         <v>0.14599999999999999</v>
       </c>
       <c r="H3" s="16">
@@ -840,7 +854,7 @@
       <c r="I3" s="12">
         <v>0.10299999999999999</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <v>0.17699999999999999</v>
       </c>
       <c r="K3" s="11">
@@ -849,7 +863,7 @@
       <c r="L3" s="12">
         <v>0.34</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="12">
         <v>0.496</v>
       </c>
       <c r="N3" s="11" t="s">
@@ -947,7 +961,7 @@
       <c r="F4" s="12">
         <v>0.09</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>0.161</v>
       </c>
       <c r="H4" s="11">
@@ -956,7 +970,7 @@
       <c r="I4" s="12">
         <v>0.112</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <v>0.186</v>
       </c>
       <c r="K4" s="11">
@@ -965,7 +979,7 @@
       <c r="L4" s="12">
         <v>0.36599999999999999</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="12">
         <v>0.52300000000000002</v>
       </c>
       <c r="N4" s="11"/>
@@ -1039,7 +1053,7 @@
       <c r="F5" s="12">
         <v>0.31900000000000001</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>0.311</v>
       </c>
       <c r="H5" s="11">
@@ -1048,7 +1062,7 @@
       <c r="I5" s="12">
         <v>0.122</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <v>0.193</v>
       </c>
       <c r="K5" s="11">
@@ -1057,7 +1071,7 @@
       <c r="L5" s="12">
         <v>0.28000000000000003</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="12">
         <v>0.433</v>
       </c>
       <c r="N5" s="11"/>
@@ -1131,7 +1145,7 @@
       <c r="F6" s="12">
         <v>0.223</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>0.31</v>
       </c>
       <c r="H6" s="11">
@@ -1140,7 +1154,7 @@
       <c r="I6" s="12">
         <v>0.28699999999999998</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <v>0.32500000000000001</v>
       </c>
       <c r="K6" s="16">
@@ -1149,7 +1163,7 @@
       <c r="L6" s="12">
         <v>0.39200000000000002</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="12">
         <v>0.55600000000000005</v>
       </c>
       <c r="N6" s="11"/>
@@ -1223,7 +1237,7 @@
       <c r="F7" s="12">
         <v>0.127</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>0.20599999999999999</v>
       </c>
       <c r="H7" s="11">
@@ -1232,7 +1246,7 @@
       <c r="I7" s="12">
         <v>0.113</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <v>0.16400000000000001</v>
       </c>
       <c r="K7" s="11">
@@ -1241,7 +1255,7 @@
       <c r="L7" s="12">
         <v>0.17799999999999999</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="12">
         <v>0.29799999999999999</v>
       </c>
       <c r="N7" s="11"/>
@@ -1315,7 +1329,7 @@
       <c r="F8" s="14">
         <v>0.41889999999999999</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="14">
         <v>0.34870000000000001</v>
       </c>
       <c r="H8" s="11">
@@ -1324,7 +1338,7 @@
       <c r="I8" s="14">
         <v>0.56469999999999998</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="14">
         <v>0.4617</v>
       </c>
       <c r="K8" s="11">
@@ -1333,7 +1347,7 @@
       <c r="L8" s="14">
         <v>0.88360000000000005</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="14">
         <v>0.77449999999999997</v>
       </c>
       <c r="N8" s="11">
@@ -1431,7 +1445,7 @@
       <c r="F9" s="12">
         <v>0.25240000000000001</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>0.30159999999999998</v>
       </c>
       <c r="H9" s="11">
@@ -1440,7 +1454,7 @@
       <c r="I9" s="12">
         <v>0.6472</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <v>0.53159999999999996</v>
       </c>
       <c r="K9" s="11">
@@ -1449,7 +1463,7 @@
       <c r="L9" s="12">
         <v>0.91459999999999997</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="12">
         <v>0.78490000000000004</v>
       </c>
       <c r="N9" s="11">
@@ -1547,7 +1561,7 @@
       <c r="F10" s="9">
         <v>0.38890000000000002</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>0.31540000000000001</v>
       </c>
       <c r="H10" s="8">
@@ -1556,7 +1570,7 @@
       <c r="I10" s="9">
         <v>0.6169</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>0.45729999999999998</v>
       </c>
       <c r="K10" s="8">
@@ -1565,7 +1579,7 @@
       <c r="L10" s="9">
         <v>0.82850000000000001</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <v>0.78359999999999996</v>
       </c>
       <c r="N10" s="8">
@@ -1663,7 +1677,7 @@
       <c r="F11" s="9">
         <v>0.30869999999999997</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>0.31219999999999998</v>
       </c>
       <c r="H11" s="8">
@@ -1672,7 +1686,7 @@
       <c r="I11" s="9">
         <v>0.64290000000000003</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>0.53349999999999997</v>
       </c>
       <c r="K11" s="8">
@@ -1681,7 +1695,7 @@
       <c r="L11" s="9">
         <v>0.90780000000000005</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <v>0.78569999999999995</v>
       </c>
       <c r="N11" s="8">
@@ -1761,19 +1775,21 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="8"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="8"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="10"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9"/>
       <c r="P12" s="10"/>
@@ -1800,19 +1816,21 @@
       <c r="AK12" s="13"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="8"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
+      <c r="J13" s="9"/>
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="10"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="8"/>
       <c r="O13" s="9"/>
       <c r="P13" s="10"/>
@@ -1839,10 +1857,86 @@
       <c r="AK13" s="13"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="10"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="10"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="12"/>
+      <c r="AK14" s="13"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="10"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="10"/>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="12"/>
+      <c r="AK15" s="13"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -2039,7 +2133,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK3:AK13">
+  <conditionalFormatting sqref="AK3:AK15">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Entering results into spreadsheet.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="48">
   <si>
     <t>DEVEL</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>SEMAINE train, gen PCA (dynamic)</t>
+  </si>
+  <si>
+    <t>BP4D train, spec PCA (static)</t>
+  </si>
+  <si>
+    <t>BP4D train, spec PCA (dynamic)</t>
+  </si>
+  <si>
+    <t>BP4D train, gen PCA (static)</t>
+  </si>
+  <si>
+    <t>BP4D train, gen PCA (dynamic)</t>
   </si>
 </sst>
 </file>
@@ -297,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -323,6 +335,8 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,8 +349,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -641,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,66 +667,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="23" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="23" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="23" t="s">
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="23" t="s">
+      <c r="O1" s="23"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="23" t="s">
+      <c r="R1" s="23"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="21"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="23" t="s">
+      <c r="U1" s="23"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="23" t="s">
+      <c r="X1" s="23"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="23" t="s">
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="21" t="s">
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="21" t="s">
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="22"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="24"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1781,9 +1796,15 @@
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="E12" s="8">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.26700000000000002</v>
+      </c>
       <c r="H12" s="8"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -1796,24 +1817,45 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="9"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="10"/>
+      <c r="T12" s="8">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="U12" s="9">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="V12" s="10">
+        <v>0.45100000000000001</v>
+      </c>
       <c r="W12" s="8"/>
       <c r="X12" s="9"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="9"/>
       <c r="AB12" s="10"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="10"/>
+      <c r="AC12" s="8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="AD12" s="9">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AE12" s="10">
+        <v>0.10299999999999999</v>
+      </c>
       <c r="AF12" s="9"/>
       <c r="AG12" s="9"/>
       <c r="AH12" s="10"/>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="12"/>
-      <c r="AK12" s="13"/>
+      <c r="AI12" s="11">
+        <f t="shared" ref="AI12:AI15" si="7">AVERAGE(B12,E12,H12,K12,N12,Q12,T12,W12,Z12,AC12,AF12)</f>
+        <v>0.17066666666666666</v>
+      </c>
+      <c r="AJ12" s="12">
+        <f t="shared" ref="AJ12:AJ15" si="8">AVERAGE(C12,F12,I12,L12,O12,R12,U12,X12,AA12,AD12,AG12)</f>
+        <v>0.89366666666666672</v>
+      </c>
+      <c r="AK12" s="13">
+        <f t="shared" ref="AK12:AK15" si="9">AVERAGE(D12,G12,J12,M12,P12,S12,V12,Y12,AB12,AE12,AH12)</f>
+        <v>0.27366666666666667</v>
+      </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1822,9 +1864,15 @@
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="E13" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.27700000000000002</v>
+      </c>
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -1837,106 +1885,181 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="9"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="10"/>
+      <c r="T13" s="8">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="U13" s="9">
+        <v>0.504</v>
+      </c>
+      <c r="V13" s="10">
+        <v>0.437</v>
+      </c>
       <c r="W13" s="8"/>
       <c r="X13" s="9"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="9"/>
       <c r="AB13" s="10"/>
-      <c r="AC13" s="8"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="10"/>
+      <c r="AC13" s="8">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="AD13" s="9">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="AE13" s="10">
+        <v>0.109</v>
+      </c>
       <c r="AF13" s="9"/>
       <c r="AG13" s="9"/>
       <c r="AH13" s="10"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="13"/>
+      <c r="AI13" s="11">
+        <f t="shared" si="7"/>
+        <v>0.21133333333333337</v>
+      </c>
+      <c r="AJ13" s="12">
+        <f t="shared" si="8"/>
+        <v>0.65666666666666662</v>
+      </c>
+      <c r="AK13" s="13">
+        <f t="shared" si="9"/>
+        <v>0.27433333333333332</v>
+      </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="27">
+        <v>0.13</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="G14" s="29">
+        <v>0.223</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="9"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="10"/>
+      <c r="T14" s="8">
+        <v>0.317</v>
+      </c>
+      <c r="U14" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="V14" s="10">
+        <v>0.46899999999999997</v>
+      </c>
       <c r="W14" s="8"/>
       <c r="X14" s="9"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="9"/>
       <c r="AB14" s="10"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="10"/>
+      <c r="AC14" s="8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="AD14" s="9">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AE14" s="10">
+        <v>0.104</v>
+      </c>
       <c r="AF14" s="9"/>
       <c r="AG14" s="9"/>
       <c r="AH14" s="10"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="12"/>
-      <c r="AK14" s="13"/>
+      <c r="AI14" s="11">
+        <f t="shared" si="7"/>
+        <v>0.16733333333333333</v>
+      </c>
+      <c r="AJ14" s="12">
+        <f t="shared" si="8"/>
+        <v>0.87966666666666671</v>
+      </c>
+      <c r="AK14" s="13">
+        <f t="shared" si="9"/>
+        <v>0.26533333333333331</v>
+      </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="27">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="F15" s="28">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="10"/>
+      <c r="T15" s="8">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="U15" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="V15" s="10">
+        <v>0.44800000000000001</v>
+      </c>
       <c r="W15" s="8"/>
       <c r="X15" s="9"/>
       <c r="Y15" s="10"/>
       <c r="Z15" s="8"/>
       <c r="AA15" s="9"/>
       <c r="AB15" s="10"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="10"/>
+      <c r="AC15" s="8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="AD15" s="9">
+        <v>0.97</v>
+      </c>
+      <c r="AE15" s="10">
+        <v>0.105</v>
+      </c>
       <c r="AF15" s="9"/>
       <c r="AG15" s="9"/>
       <c r="AH15" s="10"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="12"/>
-      <c r="AK15" s="13"/>
+      <c r="AI15" s="11">
+        <f t="shared" si="7"/>
+        <v>0.21533333333333335</v>
+      </c>
+      <c r="AJ15" s="12">
+        <f t="shared" si="8"/>
+        <v>0.69600000000000006</v>
+      </c>
+      <c r="AK15" s="13">
+        <f t="shared" si="9"/>
+        <v>0.29233333333333333</v>
+      </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -2002,6 +2125,42 @@
     <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G9">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J9">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2013,7 +2172,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G9">
+  <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -2025,7 +2184,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -2037,7 +2196,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M9">
+  <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2049,7 +2208,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P9">
+  <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2061,7 +2220,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S9">
+  <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2073,7 +2232,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V9">
+  <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -2085,7 +2244,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y9">
+  <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2097,7 +2256,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB9">
+  <conditionalFormatting sqref="AK3:AK15">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2109,7 +2268,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE9">
+  <conditionalFormatting sqref="D3:D11">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2121,7 +2280,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH9">
+  <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2133,7 +2292,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK3:AK15">
+  <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2145,7 +2304,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D11">
+  <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2157,7 +2316,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G11">
+  <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2169,7 +2328,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J11">
+  <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2181,7 +2340,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M11">
+  <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2193,7 +2352,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P11">
+  <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2205,7 +2364,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S11">
+  <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2217,7 +2376,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V11">
+  <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2229,7 +2388,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y11">
+  <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2241,7 +2400,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB11">
+  <conditionalFormatting sqref="G3:G15">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2253,7 +2412,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE11">
+  <conditionalFormatting sqref="V3:V15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2265,7 +2424,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH11">
+  <conditionalFormatting sqref="AE3:AE15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2284,10 +2443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH17"/>
+  <dimension ref="A1:AH18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,53 +2471,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="23" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="23" t="s">
+      <c r="L1" s="23"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="23" t="s">
+      <c r="O1" s="23"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="23" t="s">
+      <c r="R1" s="23"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="21"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2950,17 +3109,35 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.315</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.53500000000000003</v>
+      </c>
       <c r="K11" s="8"/>
       <c r="L11" s="9"/>
       <c r="M11" s="10"/>
@@ -2970,23 +3147,50 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="9"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="10"/>
+      <c r="T11" s="8">
+        <f>AVERAGE(B11,E11,H11,K11,N11,Q11)</f>
+        <v>0.4323333333333334</v>
+      </c>
+      <c r="U11" s="9">
+        <f>AVERAGE(C11,F11,I11,L11,O11,R11)</f>
+        <v>0.85699999999999987</v>
+      </c>
+      <c r="V11" s="10">
+        <f>AVERAGE(D11,G11,J11,M11,P11,S11)</f>
+        <v>0.54500000000000004</v>
+      </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+        <v>45</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.123</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.93</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0.02</v>
+      </c>
       <c r="K12" s="8"/>
       <c r="L12" s="9"/>
       <c r="M12" s="10"/>
@@ -2996,23 +3200,50 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="9"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="10"/>
+      <c r="T12" s="8">
+        <f t="shared" ref="T12:T14" si="6">AVERAGE(B12,E12,H12,K12,N12,Q12)</f>
+        <v>0.57366666666666666</v>
+      </c>
+      <c r="U12" s="9">
+        <f t="shared" ref="U12:U14" si="7">AVERAGE(C12,F12,I12,L12,O12,R12)</f>
+        <v>0.15666666666666668</v>
+      </c>
+      <c r="V12" s="10">
+        <f t="shared" ref="V12:V14" si="8">AVERAGE(D12,G12,J12,M12,P12,S12)</f>
+        <v>0.23700000000000002</v>
+      </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.76</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.52600000000000002</v>
+      </c>
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
       <c r="M13" s="10"/>
@@ -3022,23 +3253,50 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="9"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="10"/>
+      <c r="T13" s="8">
+        <f>AVERAGE(B13,E13,H13,K13,N13,Q13)</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="U13" s="9">
+        <f>AVERAGE(C13,F13,I13,L13,O13,R13)</f>
+        <v>0.83833333333333337</v>
+      </c>
+      <c r="V13" s="10">
+        <f>AVERAGE(D13,G13,J13,M13,P13,S13)</f>
+        <v>0.53633333333333333</v>
+      </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+        <v>47</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.219</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="I14" s="9">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="J14" s="10">
+        <v>3.9E-2</v>
+      </c>
       <c r="K14" s="8"/>
       <c r="L14" s="9"/>
       <c r="M14" s="10"/>
@@ -3048,11 +3306,23 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="9"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="10"/>
+      <c r="T14" s="8">
+        <f t="shared" si="6"/>
+        <v>0.57633333333333325</v>
+      </c>
+      <c r="U14" s="9">
+        <f t="shared" si="7"/>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="V14" s="10">
+        <f t="shared" si="8"/>
+        <v>0.24966666666666668</v>
+      </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -3076,6 +3346,9 @@
       <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -3098,7 +3371,10 @@
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -3121,21 +3397,62 @@
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
     </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G10">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3147,7 +3464,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G10">
+  <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3159,7 +3476,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10">
+  <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3171,7 +3488,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M10">
+  <conditionalFormatting sqref="V3:V14">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3183,7 +3500,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P7:P10">
+  <conditionalFormatting sqref="D3:D14">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3195,7 +3512,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S7:S10">
+  <conditionalFormatting sqref="G3:G14">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3207,7 +3524,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V10">
+  <conditionalFormatting sqref="J3:J14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Updating results and introducing joint model training.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
   <si>
     <t>DEVEL</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>BP4D train, gen PCA (dynamic)</t>
+  </si>
+  <si>
+    <t>Combined train, static</t>
+  </si>
+  <si>
+    <t>Combined train, dynamic</t>
   </si>
 </sst>
 </file>
@@ -309,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -337,6 +343,9 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -349,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -656,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,66 +676,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="25" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="25" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="25" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="25" t="s">
+      <c r="O1" s="26"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="23"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="25" t="s">
+      <c r="R1" s="26"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="23"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="25" t="s">
+      <c r="U1" s="26"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="25" t="s">
+      <c r="X1" s="26"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="25" t="s">
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="23" t="s">
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="23" t="s">
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="24"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="27"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1375,22 +1384,22 @@
         <v>0.77190000000000003</v>
       </c>
       <c r="Q8" s="16">
-        <v>0.72309999999999997</v>
+        <v>0.77070000000000005</v>
       </c>
       <c r="R8" s="14">
-        <v>0.77410000000000001</v>
+        <v>0.95709999999999995</v>
       </c>
       <c r="S8" s="17">
-        <v>0.74770000000000003</v>
+        <v>0.85389999999999999</v>
       </c>
       <c r="T8" s="11">
-        <v>0.82520000000000004</v>
+        <v>0.82889999999999997</v>
       </c>
       <c r="U8" s="14">
-        <v>0.76139999999999997</v>
+        <v>0.92810000000000004</v>
       </c>
       <c r="V8" s="13">
-        <v>0.79200000000000004</v>
+        <v>0.87570000000000003</v>
       </c>
       <c r="W8" s="16">
         <v>0.52159999999999995</v>
@@ -1430,15 +1439,15 @@
       </c>
       <c r="AI8" s="11">
         <f t="shared" si="1"/>
-        <v>0.5204545454545455</v>
+        <v>0.52511818181818182</v>
       </c>
       <c r="AJ8" s="12">
         <f t="shared" si="2"/>
-        <v>0.6914818181818182</v>
+        <v>0.72327272727272718</v>
       </c>
       <c r="AK8" s="13">
         <f t="shared" si="3"/>
-        <v>0.58799999999999997</v>
+        <v>0.60526363636363623</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -1491,22 +1500,22 @@
         <v>0.75519999999999998</v>
       </c>
       <c r="Q9" s="11">
-        <v>0.76339999999999997</v>
+        <v>0.73240000000000005</v>
       </c>
       <c r="R9" s="12">
-        <v>0.70699999999999996</v>
+        <v>0.94779999999999998</v>
       </c>
       <c r="S9" s="13">
-        <v>0.73409999999999997</v>
+        <v>0.82630000000000003</v>
       </c>
       <c r="T9" s="11">
-        <v>0.85899999999999999</v>
+        <v>0.79690000000000005</v>
       </c>
       <c r="U9" s="12">
-        <v>0.7732</v>
+        <v>0.91659999999999997</v>
       </c>
       <c r="V9" s="13">
-        <v>0.81389999999999996</v>
+        <v>0.85260000000000002</v>
       </c>
       <c r="W9" s="11">
         <v>0.46279999999999999</v>
@@ -1546,15 +1555,15 @@
       </c>
       <c r="AI9" s="11">
         <f t="shared" si="1"/>
-        <v>0.54464545454545454</v>
+        <v>0.5361818181818182</v>
       </c>
       <c r="AJ9" s="12">
         <f t="shared" si="2"/>
-        <v>0.65229090909090914</v>
+        <v>0.68721818181818184</v>
       </c>
       <c r="AK9" s="13">
         <f t="shared" si="3"/>
-        <v>0.58074545454545456</v>
+        <v>0.59264545454545459</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -1607,22 +1616,22 @@
         <v>0.76500000000000001</v>
       </c>
       <c r="Q10" s="8">
-        <v>0.75560000000000005</v>
+        <v>0.86070000000000002</v>
       </c>
       <c r="R10" s="9">
-        <v>0.73839999999999995</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="S10" s="10">
-        <v>0.74690000000000001</v>
+        <v>0.82869999999999999</v>
       </c>
       <c r="T10" s="8">
-        <v>0.78939999999999999</v>
+        <v>0.89859999999999995</v>
       </c>
       <c r="U10" s="9">
-        <v>0.82099999999999995</v>
+        <v>0.8367</v>
       </c>
       <c r="V10" s="10">
-        <v>0.80489999999999995</v>
+        <v>0.86650000000000005</v>
       </c>
       <c r="W10" s="8">
         <v>0.6109</v>
@@ -1662,15 +1671,15 @@
       </c>
       <c r="AI10" s="11">
         <f>AVERAGE(B10,E10,H10,K10,N10,Q10,T10,W10,Z10,AC10,AF10)</f>
-        <v>0.52344545454545444</v>
+        <v>0.5429272727272727</v>
       </c>
       <c r="AJ10" s="12">
         <f t="shared" si="2"/>
-        <v>0.68452727272727265</v>
+        <v>0.69146363636363628</v>
       </c>
       <c r="AK10" s="13">
         <f t="shared" si="3"/>
-        <v>0.58509090909090911</v>
+        <v>0.59812727272727273</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -1723,22 +1732,22 @@
         <v>0.75849999999999995</v>
       </c>
       <c r="Q11" s="8">
-        <v>0.88260000000000005</v>
+        <v>0.73919999999999997</v>
       </c>
       <c r="R11" s="9">
-        <v>0.38340000000000002</v>
+        <v>0.94450000000000001</v>
       </c>
       <c r="S11" s="10">
-        <v>0.53459999999999996</v>
+        <v>0.82930000000000004</v>
       </c>
       <c r="T11" s="8">
-        <v>0.89400000000000002</v>
+        <v>0.77729999999999999</v>
       </c>
       <c r="U11" s="9">
-        <v>0.66849999999999998</v>
+        <v>0.9456</v>
       </c>
       <c r="V11" s="10">
-        <v>0.76490000000000002</v>
+        <v>0.85319999999999996</v>
       </c>
       <c r="W11" s="8">
         <v>0.46829999999999999</v>
@@ -1778,32 +1787,32 @@
       </c>
       <c r="AI11" s="11">
         <f t="shared" ref="AI11" si="4">AVERAGE(B11,E11,H11,K11,N11,Q11,T11,W11,Z11,AC11,AF11)</f>
-        <v>0.55684545454545453</v>
+        <v>0.5331999999999999</v>
       </c>
       <c r="AJ11" s="12">
         <f t="shared" ref="AJ11" si="5">AVERAGE(C11,F11,I11,L11,O11,R11,U11,X11,AA11,AD11,AG11)</f>
-        <v>0.6191545454545454</v>
+        <v>0.69535454545454545</v>
       </c>
       <c r="AK11" s="13">
         <f t="shared" ref="AK11" si="6">AVERAGE(D11,G11,J11,M11,P11,S11,V11,Y11,AB11,AE11,AH11)</f>
-        <v>0.56269999999999998</v>
+        <v>0.59751818181818195</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="8">
-        <v>0.16300000000000001</v>
+        <v>0.19470000000000001</v>
       </c>
       <c r="F12" s="9">
-        <v>0.74399999999999999</v>
+        <v>0.81969999999999998</v>
       </c>
       <c r="G12" s="9">
-        <v>0.26700000000000002</v>
+        <v>0.31469999999999998</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="9"/>
@@ -1818,13 +1827,13 @@
       <c r="R12" s="9"/>
       <c r="S12" s="10"/>
       <c r="T12" s="8">
-        <v>0.29499999999999998</v>
+        <v>0.72030000000000005</v>
       </c>
       <c r="U12" s="9">
-        <v>0.96199999999999997</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="V12" s="10">
-        <v>0.45100000000000001</v>
+        <v>0.78480000000000005</v>
       </c>
       <c r="W12" s="8"/>
       <c r="X12" s="9"/>
@@ -1833,45 +1842,45 @@
       <c r="AA12" s="9"/>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8">
-        <v>5.3999999999999999E-2</v>
+        <v>0.38229999999999997</v>
       </c>
       <c r="AD12" s="9">
-        <v>0.97499999999999998</v>
+        <v>0.88829999999999998</v>
       </c>
       <c r="AE12" s="10">
-        <v>0.10299999999999999</v>
+        <v>0.53459999999999996</v>
       </c>
       <c r="AF12" s="9"/>
       <c r="AG12" s="9"/>
       <c r="AH12" s="10"/>
       <c r="AI12" s="11">
         <f t="shared" ref="AI12:AI15" si="7">AVERAGE(B12,E12,H12,K12,N12,Q12,T12,W12,Z12,AC12,AF12)</f>
-        <v>0.17066666666666666</v>
+        <v>0.43243333333333328</v>
       </c>
       <c r="AJ12" s="12">
         <f t="shared" ref="AJ12:AJ15" si="8">AVERAGE(C12,F12,I12,L12,O12,R12,U12,X12,AA12,AD12,AG12)</f>
-        <v>0.89366666666666672</v>
+        <v>0.85666666666666658</v>
       </c>
       <c r="AK12" s="13">
         <f t="shared" ref="AK12:AK15" si="9">AVERAGE(D12,G12,J12,M12,P12,S12,V12,Y12,AB12,AE12,AH12)</f>
-        <v>0.27366666666666667</v>
+        <v>0.54469999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="8">
-        <v>0.19</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="9">
-        <v>0.50900000000000001</v>
+        <v>0.1236</v>
       </c>
       <c r="G13" s="9">
-        <v>0.27700000000000002</v>
+        <v>0.19819999999999999</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
@@ -1886,13 +1895,13 @@
       <c r="R13" s="9"/>
       <c r="S13" s="10"/>
       <c r="T13" s="8">
-        <v>0.38600000000000001</v>
+        <v>0.93089999999999995</v>
       </c>
       <c r="U13" s="9">
-        <v>0.504</v>
+        <v>0.33550000000000002</v>
       </c>
       <c r="V13" s="10">
-        <v>0.437</v>
+        <v>0.49320000000000003</v>
       </c>
       <c r="W13" s="8"/>
       <c r="X13" s="9"/>
@@ -1901,45 +1910,45 @@
       <c r="AA13" s="9"/>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8">
-        <v>5.8000000000000003E-2</v>
+        <v>0.2908</v>
       </c>
       <c r="AD13" s="9">
-        <v>0.95699999999999996</v>
+        <v>1.03E-2</v>
       </c>
       <c r="AE13" s="10">
-        <v>0.109</v>
+        <v>0.02</v>
       </c>
       <c r="AF13" s="9"/>
       <c r="AG13" s="9"/>
       <c r="AH13" s="10"/>
       <c r="AI13" s="11">
         <f t="shared" si="7"/>
-        <v>0.21133333333333337</v>
+        <v>0.57389999999999997</v>
       </c>
       <c r="AJ13" s="12">
         <f t="shared" si="8"/>
-        <v>0.65666666666666662</v>
+        <v>0.15646666666666667</v>
       </c>
       <c r="AK13" s="13">
         <f t="shared" si="9"/>
-        <v>0.27433333333333332</v>
+        <v>0.23713333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
-      <c r="E14" s="27">
-        <v>0.13</v>
-      </c>
-      <c r="F14" s="28">
-        <v>0.76300000000000001</v>
-      </c>
-      <c r="G14" s="29">
-        <v>0.223</v>
+      <c r="E14" s="23">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="F14" s="24">
+        <v>0.77370000000000005</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0.32279999999999998</v>
       </c>
       <c r="H14" s="21"/>
       <c r="I14" s="22"/>
@@ -1954,13 +1963,13 @@
       <c r="R14" s="9"/>
       <c r="S14" s="10"/>
       <c r="T14" s="8">
-        <v>0.317</v>
+        <v>0.66579999999999995</v>
       </c>
       <c r="U14" s="9">
-        <v>0.9</v>
+        <v>0.88560000000000005</v>
       </c>
       <c r="V14" s="10">
-        <v>0.46899999999999997</v>
+        <v>0.7601</v>
       </c>
       <c r="W14" s="8"/>
       <c r="X14" s="9"/>
@@ -1969,45 +1978,45 @@
       <c r="AA14" s="9"/>
       <c r="AB14" s="10"/>
       <c r="AC14" s="8">
-        <v>5.5E-2</v>
+        <v>0.38019999999999998</v>
       </c>
       <c r="AD14" s="9">
-        <v>0.97599999999999998</v>
+        <v>0.85519999999999996</v>
       </c>
       <c r="AE14" s="10">
-        <v>0.104</v>
+        <v>0.52639999999999998</v>
       </c>
       <c r="AF14" s="9"/>
       <c r="AG14" s="9"/>
       <c r="AH14" s="10"/>
       <c r="AI14" s="11">
         <f t="shared" si="7"/>
-        <v>0.16733333333333333</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="AJ14" s="12">
         <f t="shared" si="8"/>
-        <v>0.87966666666666671</v>
+        <v>0.83816666666666662</v>
       </c>
       <c r="AK14" s="13">
         <f t="shared" si="9"/>
-        <v>0.26533333333333331</v>
+        <v>0.53643333333333332</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="27">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="F15" s="28">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="G15" s="29">
-        <v>0.32400000000000001</v>
+      <c r="E15" s="23">
+        <v>0.52129999999999999</v>
+      </c>
+      <c r="F15" s="24">
+        <v>0.1389</v>
+      </c>
+      <c r="G15" s="25">
+        <v>0.21929999999999999</v>
       </c>
       <c r="H15" s="21"/>
       <c r="I15" s="22"/>
@@ -2022,13 +2031,13 @@
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
       <c r="T15" s="8">
-        <v>0.34899999999999998</v>
+        <v>0.92249999999999999</v>
       </c>
       <c r="U15" s="9">
-        <v>0.627</v>
+        <v>0.33489999999999998</v>
       </c>
       <c r="V15" s="10">
-        <v>0.44800000000000001</v>
+        <v>0.4914</v>
       </c>
       <c r="W15" s="8"/>
       <c r="X15" s="9"/>
@@ -2037,76 +2046,224 @@
       <c r="AA15" s="9"/>
       <c r="AB15" s="10"/>
       <c r="AC15" s="8">
-        <v>5.5E-2</v>
+        <v>0.28539999999999999</v>
       </c>
       <c r="AD15" s="9">
-        <v>0.97</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="AE15" s="10">
-        <v>0.105</v>
+        <v>3.8800000000000001E-2</v>
       </c>
       <c r="AF15" s="9"/>
       <c r="AG15" s="9"/>
       <c r="AH15" s="10"/>
       <c r="AI15" s="11">
         <f t="shared" si="7"/>
-        <v>0.21533333333333335</v>
+        <v>0.57640000000000002</v>
       </c>
       <c r="AJ15" s="12">
         <f t="shared" si="8"/>
-        <v>0.69600000000000006</v>
+        <v>0.16486666666666666</v>
       </c>
       <c r="AK15" s="13">
         <f t="shared" si="9"/>
-        <v>0.29233333333333333</v>
+        <v>0.24983333333333335</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="10"/>
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="12"/>
+      <c r="AK16" s="13"/>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="11"/>
+      <c r="AJ17" s="12"/>
+      <c r="AK17" s="13"/>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="8"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="12"/>
+      <c r="AK18" s="13"/>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="12"/>
+      <c r="AK19" s="13"/>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
   </sheetData>
@@ -2256,7 +2413,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK3:AK15">
+  <conditionalFormatting sqref="AK3:AK19">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2400,7 +2557,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G15">
+  <conditionalFormatting sqref="G3:G19">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2412,7 +2569,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V15">
+  <conditionalFormatting sqref="V3:V19">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2424,7 +2581,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE15">
+  <conditionalFormatting sqref="AE3:AE19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2445,8 +2602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,53 +2628,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="25" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="25" t="s">
+      <c r="O1" s="26"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="23"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="25" t="s">
+      <c r="R1" s="26"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="23"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3109,34 +3266,34 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="8">
-        <v>0.19500000000000001</v>
+        <v>0.1303</v>
       </c>
       <c r="C11" s="9">
-        <v>0.82</v>
+        <v>0.76329999999999998</v>
       </c>
       <c r="D11" s="10">
-        <v>0.315</v>
+        <v>0.22259999999999999</v>
       </c>
       <c r="E11" s="8">
-        <v>0.72</v>
+        <v>0.31159999999999999</v>
       </c>
       <c r="F11" s="9">
-        <v>0.86199999999999999</v>
+        <v>0.9264</v>
       </c>
       <c r="G11" s="10">
-        <v>0.78500000000000003</v>
+        <v>0.46629999999999999</v>
       </c>
       <c r="H11" s="8">
-        <v>0.38200000000000001</v>
+        <v>5.4899999999999997E-2</v>
       </c>
       <c r="I11" s="9">
-        <v>0.88900000000000001</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="J11" s="10">
-        <v>0.53500000000000003</v>
+        <v>0.104</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="9"/>
@@ -3149,47 +3306,47 @@
       <c r="S11" s="10"/>
       <c r="T11" s="8">
         <f>AVERAGE(B11,E11,H11,K11,N11,Q11)</f>
-        <v>0.4323333333333334</v>
+        <v>0.1656</v>
       </c>
       <c r="U11" s="9">
         <f>AVERAGE(C11,F11,I11,L11,O11,R11)</f>
-        <v>0.85699999999999987</v>
+        <v>0.88856666666666673</v>
       </c>
       <c r="V11" s="10">
         <f>AVERAGE(D11,G11,J11,M11,P11,S11)</f>
-        <v>0.54500000000000004</v>
+        <v>0.26429999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" s="8">
-        <v>0.5</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="C12" s="9">
-        <v>0.123</v>
+        <v>0.4909</v>
       </c>
       <c r="D12" s="10">
-        <v>0.19700000000000001</v>
+        <v>0.32419999999999999</v>
       </c>
       <c r="E12" s="8">
-        <v>0.93</v>
+        <v>0.3306</v>
       </c>
       <c r="F12" s="9">
-        <v>0.33700000000000002</v>
+        <v>0.86760000000000004</v>
       </c>
       <c r="G12" s="10">
-        <v>0.49399999999999999</v>
+        <v>0.4788</v>
       </c>
       <c r="H12" s="8">
-        <v>0.29099999999999998</v>
+        <v>5.5399999999999998E-2</v>
       </c>
       <c r="I12" s="9">
-        <v>0.01</v>
+        <v>0.97050000000000003</v>
       </c>
       <c r="J12" s="10">
-        <v>0.02</v>
+        <v>0.1047</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="9"/>
@@ -3202,47 +3359,47 @@
       <c r="S12" s="10"/>
       <c r="T12" s="8">
         <f t="shared" ref="T12:T14" si="6">AVERAGE(B12,E12,H12,K12,N12,Q12)</f>
-        <v>0.57366666666666666</v>
+        <v>0.20933333333333334</v>
       </c>
       <c r="U12" s="9">
         <f t="shared" ref="U12:U14" si="7">AVERAGE(C12,F12,I12,L12,O12,R12)</f>
-        <v>0.15666666666666668</v>
+        <v>0.77633333333333343</v>
       </c>
       <c r="V12" s="10">
         <f t="shared" ref="V12:V14" si="8">AVERAGE(D12,G12,J12,M12,P12,S12)</f>
-        <v>0.23700000000000002</v>
+        <v>0.30256666666666665</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="8">
-        <v>0.20399999999999999</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="C13" s="9">
-        <v>0.77400000000000002</v>
+        <v>0.74350000000000005</v>
       </c>
       <c r="D13" s="10">
-        <v>0.32300000000000001</v>
+        <v>0.26740000000000003</v>
       </c>
       <c r="E13" s="8">
-        <v>0.66600000000000004</v>
+        <v>0.31790000000000002</v>
       </c>
       <c r="F13" s="9">
-        <v>0.88600000000000001</v>
+        <v>0.91090000000000004</v>
       </c>
       <c r="G13" s="10">
-        <v>0.76</v>
+        <v>0.4713</v>
       </c>
       <c r="H13" s="8">
-        <v>0.38</v>
+        <v>5.4199999999999998E-2</v>
       </c>
       <c r="I13" s="9">
-        <v>0.85499999999999998</v>
+        <v>0.9748</v>
       </c>
       <c r="J13" s="10">
-        <v>0.52600000000000002</v>
+        <v>0.1026</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
@@ -3255,47 +3412,47 @@
       <c r="S13" s="10"/>
       <c r="T13" s="8">
         <f>AVERAGE(B13,E13,H13,K13,N13,Q13)</f>
-        <v>0.41666666666666669</v>
+        <v>0.17836666666666667</v>
       </c>
       <c r="U13" s="9">
         <f>AVERAGE(C13,F13,I13,L13,O13,R13)</f>
-        <v>0.83833333333333337</v>
+        <v>0.87639999999999996</v>
       </c>
       <c r="V13" s="10">
         <f>AVERAGE(D13,G13,J13,M13,P13,S13)</f>
-        <v>0.53633333333333333</v>
+        <v>0.28043333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="8">
-        <v>0.52100000000000002</v>
+        <v>0.19009999999999999</v>
       </c>
       <c r="C14" s="9">
-        <v>0.13900000000000001</v>
+        <v>0.5091</v>
       </c>
       <c r="D14" s="10">
-        <v>0.219</v>
+        <v>0.27679999999999999</v>
       </c>
       <c r="E14" s="8">
-        <v>0.92300000000000004</v>
+        <v>0.31850000000000001</v>
       </c>
       <c r="F14" s="9">
-        <v>0.33500000000000002</v>
+        <v>0.95520000000000005</v>
       </c>
       <c r="G14" s="10">
-        <v>0.49099999999999999</v>
+        <v>0.47770000000000001</v>
       </c>
       <c r="H14" s="8">
-        <v>0.28499999999999998</v>
+        <v>5.7599999999999998E-2</v>
       </c>
       <c r="I14" s="9">
-        <v>2.1000000000000001E-2</v>
+        <v>0.95689999999999997</v>
       </c>
       <c r="J14" s="10">
-        <v>3.9E-2</v>
+        <v>0.1086</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="9"/>
@@ -3308,15 +3465,15 @@
       <c r="S14" s="10"/>
       <c r="T14" s="8">
         <f t="shared" si="6"/>
-        <v>0.57633333333333325</v>
+        <v>0.18873333333333331</v>
       </c>
       <c r="U14" s="9">
         <f t="shared" si="7"/>
-        <v>0.16500000000000001</v>
+        <v>0.80706666666666671</v>
       </c>
       <c r="V14" s="10">
         <f t="shared" si="8"/>
-        <v>0.24966666666666668</v>
+        <v>0.28770000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
@@ -3404,17 +3561,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="10">

</xml_diff>

<commit_message>
Updated results of joint training (helps with some AUs in some cases).
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
   <si>
     <t>DEVEL</t>
   </si>
@@ -315,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -327,7 +327,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -346,6 +345,9 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,9 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -665,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,114 +853,114 @@
       <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>0.48799999999999999</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>0.24099999999999999</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>0.32300000000000001</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>0.69699999999999995</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="18">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="18">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>0.61599999999999999</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>0.10299999999999999</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>0.17699999999999999</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>0.91800000000000004</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <v>0.34</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <v>0.496</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="S3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="10">
         <v>0.98</v>
       </c>
-      <c r="U3" s="12">
+      <c r="U3" s="11">
         <v>0.26100000000000001</v>
       </c>
-      <c r="V3" s="13">
+      <c r="V3" s="12">
         <v>0.41199999999999998</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Y3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="Z3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="13" t="s">
+      <c r="AB3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="11">
+      <c r="AC3" s="10">
         <v>0.89</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AD3" s="11">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AE3" s="13">
+      <c r="AE3" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AF3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AG3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AH3" s="13" t="s">
+      <c r="AH3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="18">
+      <c r="AI3" s="17">
         <f>AVERAGE(B3,E3,H3,K3,N3,Q3,T3,W3,Z3,AC3,AF3)</f>
         <v>0.76483333333333337</v>
       </c>
-      <c r="AJ3" s="19">
+      <c r="AJ3" s="18">
         <f t="shared" ref="AJ3:AK3" si="0">AVERAGE(C3,F3,I3,L3,O3,R3,U3,X3,AA3,AD3,AG3)</f>
         <v>0.17583333333333331</v>
       </c>
-      <c r="AK3" s="20">
+      <c r="AK3" s="19">
         <f t="shared" si="0"/>
         <v>0.26816666666666661</v>
       </c>
@@ -970,90 +969,90 @@
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>0.498</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>0.248</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>0.33100000000000002</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>0.73699999999999999</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>0.09</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>0.161</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>0.54600000000000004</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <v>0.112</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <v>0.186</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
         <v>0.91700000000000004</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="11">
         <v>0.36599999999999999</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <v>0.52300000000000002</v>
       </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="11">
+      <c r="N4" s="10"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="10">
         <v>0.97</v>
       </c>
-      <c r="U4" s="12">
+      <c r="U4" s="11">
         <v>0.28699999999999998</v>
       </c>
-      <c r="V4" s="13">
+      <c r="V4" s="12">
         <v>0.443</v>
       </c>
-      <c r="W4" s="11"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="11">
+      <c r="W4" s="10"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="10">
         <v>9.4E-2</v>
       </c>
-      <c r="AA4" s="14">
+      <c r="AA4" s="13">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AB4" s="17">
+      <c r="AB4" s="16">
         <v>0.06</v>
       </c>
-      <c r="AC4" s="11">
+      <c r="AC4" s="10">
         <v>0.88600000000000001</v>
       </c>
-      <c r="AD4" s="12">
+      <c r="AD4" s="11">
         <v>3.1E-2</v>
       </c>
-      <c r="AE4" s="13">
+      <c r="AE4" s="12">
         <v>0.06</v>
       </c>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="11">
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="10">
         <f t="shared" ref="AI4:AI9" si="1">AVERAGE(B4,E4,H4,K4,N4,Q4,T4,W4,Z4,AC4,AF4)</f>
         <v>0.66399999999999992</v>
       </c>
-      <c r="AJ4" s="12">
+      <c r="AJ4" s="11">
         <f t="shared" ref="AJ4:AJ10" si="2">AVERAGE(C4,F4,I4,L4,O4,R4,U4,X4,AA4,AD4,AG4)</f>
         <v>0.16657142857142856</v>
       </c>
-      <c r="AK4" s="13">
+      <c r="AK4" s="12">
         <f t="shared" ref="AK4:AK10" si="3">AVERAGE(D4,G4,J4,M4,P4,S4,V4,Y4,AB4,AE4,AH4)</f>
         <v>0.25200000000000006</v>
       </c>
@@ -1062,90 +1061,90 @@
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>0.39</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>0.27900000000000003</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.32500000000000001</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>0.30299999999999999</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>0.31900000000000001</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>0.311</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>0.46</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>0.122</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>0.193</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <v>0.94599999999999995</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="11">
         <v>0.433</v>
       </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="11">
+      <c r="N5" s="10"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="10">
         <v>0.96499999999999997</v>
       </c>
-      <c r="U5" s="12">
+      <c r="U5" s="11">
         <v>0.23699999999999999</v>
       </c>
-      <c r="V5" s="13">
+      <c r="V5" s="12">
         <v>0.38100000000000001</v>
       </c>
-      <c r="W5" s="11"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="11">
+      <c r="W5" s="10"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="10">
         <v>0</v>
       </c>
-      <c r="AA5" s="12">
+      <c r="AA5" s="11">
         <v>0</v>
       </c>
-      <c r="AB5" s="13">
+      <c r="AB5" s="12">
         <v>0</v>
       </c>
-      <c r="AC5" s="11">
+      <c r="AC5" s="10">
         <v>0</v>
       </c>
-      <c r="AD5" s="12">
+      <c r="AD5" s="11">
         <v>0</v>
       </c>
-      <c r="AE5" s="13">
+      <c r="AE5" s="12">
         <v>0</v>
       </c>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="11">
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="10">
         <f t="shared" si="1"/>
         <v>0.43771428571428572</v>
       </c>
-      <c r="AJ5" s="12">
+      <c r="AJ5" s="11">
         <f t="shared" si="2"/>
         <v>0.17671428571428574</v>
       </c>
-      <c r="AK5" s="13">
+      <c r="AK5" s="12">
         <f t="shared" si="3"/>
         <v>0.23471428571428571</v>
       </c>
@@ -1154,90 +1153,90 @@
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>0.52600000000000002</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>0.35099999999999998</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>0.42099999999999999</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>0.50800000000000001</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>0.223</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>0.31</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>0.376</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <v>0.28699999999999998</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="11">
         <v>0.32500000000000001</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="15">
         <v>0.95699999999999996</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="11">
         <v>0.39200000000000002</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="11">
         <v>0.55600000000000005</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="11">
+      <c r="N6" s="10"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="10">
         <v>0.94599999999999995</v>
       </c>
-      <c r="U6" s="14">
+      <c r="U6" s="13">
         <v>0.42</v>
       </c>
-      <c r="V6" s="17">
+      <c r="V6" s="16">
         <v>0.58199999999999996</v>
       </c>
-      <c r="W6" s="11"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="11">
+      <c r="W6" s="10"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="10">
         <v>0.35699999999999998</v>
       </c>
-      <c r="AA6" s="12">
+      <c r="AA6" s="11">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AB6" s="12">
         <v>0.01</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6" s="10">
         <v>0.751</v>
       </c>
-      <c r="AD6" s="14">
+      <c r="AD6" s="13">
         <v>0.104</v>
       </c>
-      <c r="AE6" s="17">
+      <c r="AE6" s="16">
         <v>0.182</v>
       </c>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="11">
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="12"/>
+      <c r="AI6" s="10">
         <f t="shared" si="1"/>
         <v>0.63157142857142856</v>
       </c>
-      <c r="AJ6" s="12">
+      <c r="AJ6" s="11">
         <f t="shared" si="2"/>
         <v>0.25457142857142856</v>
       </c>
-      <c r="AK6" s="13">
+      <c r="AK6" s="12">
         <f t="shared" si="3"/>
         <v>0.3408571428571428</v>
       </c>
@@ -1246,90 +1245,90 @@
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>0.59199999999999997</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>0.22600000000000001</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>0.32800000000000001</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>0.54300000000000004</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>0.127</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>0.20599999999999999</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>0.29599999999999999</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>0.113</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>0.16400000000000001</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>0.91600000000000004</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <v>0.17799999999999999</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <v>0.29799999999999999</v>
       </c>
-      <c r="N7" s="11"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="11">
+      <c r="N7" s="10"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="10">
         <v>0.93799999999999994</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U7" s="11">
         <v>0.25800000000000001</v>
       </c>
-      <c r="V7" s="13">
+      <c r="V7" s="12">
         <v>0.40500000000000003</v>
       </c>
-      <c r="W7" s="11"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="16">
+      <c r="W7" s="10"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="15">
         <v>0.61899999999999999</v>
       </c>
-      <c r="AA7" s="12">
+      <c r="AA7" s="11">
         <v>1E-3</v>
       </c>
-      <c r="AB7" s="13">
+      <c r="AB7" s="12">
         <v>2E-3</v>
       </c>
-      <c r="AC7" s="11">
+      <c r="AC7" s="10">
         <v>0.85099999999999998</v>
       </c>
-      <c r="AD7" s="12">
+      <c r="AD7" s="11">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="AE7" s="13">
+      <c r="AE7" s="12">
         <v>0.13200000000000001</v>
       </c>
-      <c r="AF7" s="12"/>
-      <c r="AG7" s="12"/>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="11">
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="12"/>
+      <c r="AI7" s="10">
         <f t="shared" si="1"/>
         <v>0.67928571428571427</v>
       </c>
-      <c r="AJ7" s="12">
+      <c r="AJ7" s="11">
         <f t="shared" si="2"/>
         <v>0.13928571428571426</v>
       </c>
-      <c r="AK7" s="13">
+      <c r="AK7" s="12">
         <f t="shared" si="3"/>
         <v>0.21928571428571431</v>
       </c>
@@ -1338,114 +1337,114 @@
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>0.3589</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>0.47289999999999999</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>0.40810000000000002</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>0.29859999999999998</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>0.41889999999999999</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>0.34870000000000001</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>0.39050000000000001</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <v>0.56469999999999998</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <v>0.4617</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <v>0.68940000000000001</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <v>0.88360000000000005</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="13">
         <v>0.77449999999999997</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="10">
         <v>0.66279999999999994</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="13">
         <v>0.92400000000000004</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="12">
         <v>0.77190000000000003</v>
       </c>
-      <c r="Q8" s="16">
+      <c r="Q8" s="15">
         <v>0.77070000000000005</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8" s="13">
         <v>0.95709999999999995</v>
       </c>
-      <c r="S8" s="17">
+      <c r="S8" s="16">
         <v>0.85389999999999999</v>
       </c>
-      <c r="T8" s="11">
+      <c r="T8" s="10">
         <v>0.82889999999999997</v>
       </c>
-      <c r="U8" s="14">
+      <c r="U8" s="13">
         <v>0.92810000000000004</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="12">
         <v>0.87570000000000003</v>
       </c>
-      <c r="W8" s="16">
+      <c r="W8" s="15">
         <v>0.52159999999999995</v>
       </c>
-      <c r="X8" s="14">
+      <c r="X8" s="13">
         <v>0.8659</v>
       </c>
-      <c r="Y8" s="17">
+      <c r="Y8" s="16">
         <v>0.65100000000000002</v>
       </c>
-      <c r="Z8" s="11">
+      <c r="Z8" s="10">
         <v>0.3372</v>
       </c>
-      <c r="AA8" s="14">
+      <c r="AA8" s="13">
         <v>0.64849999999999997</v>
       </c>
-      <c r="AB8" s="13">
+      <c r="AB8" s="12">
         <v>0.44369999999999998</v>
       </c>
-      <c r="AC8" s="11">
+      <c r="AC8" s="10">
         <v>0.50590000000000002</v>
       </c>
-      <c r="AD8" s="12">
+      <c r="AD8" s="11">
         <v>0.79569999999999996</v>
       </c>
-      <c r="AE8" s="13">
+      <c r="AE8" s="12">
         <v>0.61850000000000005</v>
       </c>
-      <c r="AF8" s="12">
+      <c r="AF8" s="11">
         <v>0.4118</v>
       </c>
-      <c r="AG8" s="12">
+      <c r="AG8" s="11">
         <v>0.49659999999999999</v>
       </c>
-      <c r="AH8" s="13">
+      <c r="AH8" s="12">
         <v>0.45019999999999999</v>
       </c>
-      <c r="AI8" s="11">
+      <c r="AI8" s="10">
         <f t="shared" si="1"/>
         <v>0.52511818181818182</v>
       </c>
-      <c r="AJ8" s="12">
+      <c r="AJ8" s="11">
         <f t="shared" si="2"/>
         <v>0.72327272727272718</v>
       </c>
-      <c r="AK8" s="13">
+      <c r="AK8" s="12">
         <f t="shared" si="3"/>
         <v>0.60526363636363623</v>
       </c>
@@ -1454,114 +1453,114 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>0.39240000000000003</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>0.47739999999999999</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>0.43080000000000002</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>0.37469999999999998</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>0.25240000000000001</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>0.30159999999999998</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>0.45100000000000001</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="11">
         <v>0.6472</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="11">
         <v>0.53159999999999996</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>0.68730000000000002</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="11">
         <v>0.91459999999999997</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="11">
         <v>0.78490000000000004</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="10">
         <v>0.64959999999999996</v>
       </c>
-      <c r="O9" s="12">
+      <c r="O9" s="11">
         <v>0.90180000000000005</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="12">
         <v>0.75519999999999998</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="Q9" s="10">
         <v>0.73240000000000005</v>
       </c>
-      <c r="R9" s="12">
+      <c r="R9" s="11">
         <v>0.94779999999999998</v>
       </c>
-      <c r="S9" s="13">
+      <c r="S9" s="12">
         <v>0.82630000000000003</v>
       </c>
-      <c r="T9" s="11">
+      <c r="T9" s="10">
         <v>0.79690000000000005</v>
       </c>
-      <c r="U9" s="12">
+      <c r="U9" s="11">
         <v>0.91659999999999997</v>
       </c>
-      <c r="V9" s="13">
+      <c r="V9" s="12">
         <v>0.85260000000000002</v>
       </c>
-      <c r="W9" s="11">
+      <c r="W9" s="10">
         <v>0.46279999999999999</v>
       </c>
-      <c r="X9" s="12">
+      <c r="X9" s="11">
         <v>0.95140000000000002</v>
       </c>
-      <c r="Y9" s="13">
+      <c r="Y9" s="12">
         <v>0.62270000000000003</v>
       </c>
-      <c r="Z9" s="11">
+      <c r="Z9" s="10">
         <v>0.41310000000000002</v>
       </c>
-      <c r="AA9" s="12">
+      <c r="AA9" s="11">
         <v>0.35299999999999998</v>
       </c>
-      <c r="AB9" s="13">
+      <c r="AB9" s="12">
         <v>0.38069999999999998</v>
       </c>
-      <c r="AC9" s="11">
+      <c r="AC9" s="10">
         <v>0.51229999999999998</v>
       </c>
-      <c r="AD9" s="12">
+      <c r="AD9" s="11">
         <v>0.81130000000000002</v>
       </c>
-      <c r="AE9" s="13">
+      <c r="AE9" s="12">
         <v>0.628</v>
       </c>
-      <c r="AF9" s="12">
+      <c r="AF9" s="11">
         <v>0.42549999999999999</v>
       </c>
-      <c r="AG9" s="12">
+      <c r="AG9" s="11">
         <v>0.38590000000000002</v>
       </c>
-      <c r="AH9" s="12">
+      <c r="AH9" s="11">
         <v>0.4047</v>
       </c>
-      <c r="AI9" s="11">
+      <c r="AI9" s="10">
         <f t="shared" si="1"/>
         <v>0.5361818181818182</v>
       </c>
-      <c r="AJ9" s="12">
+      <c r="AJ9" s="11">
         <f t="shared" si="2"/>
         <v>0.68721818181818184</v>
       </c>
-      <c r="AK9" s="13">
+      <c r="AK9" s="12">
         <f t="shared" si="3"/>
         <v>0.59264545454545459</v>
       </c>
@@ -1570,114 +1569,114 @@
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>0.3664</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.47889999999999999</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>0.41510000000000002</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>0.26529999999999998</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>0.38890000000000002</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>0.31540000000000001</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>0.36330000000000001</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>0.6169</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <v>0.45729999999999998</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="7">
         <v>0.74339999999999995</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="8">
         <v>0.82850000000000001</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="8">
         <v>0.78359999999999996</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <v>0.71189999999999998</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="8">
         <v>0.82669999999999999</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="9">
         <v>0.76500000000000001</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="Q10" s="7">
         <v>0.86070000000000002</v>
       </c>
-      <c r="R10" s="9">
+      <c r="R10" s="8">
         <v>0.79900000000000004</v>
       </c>
-      <c r="S10" s="10">
+      <c r="S10" s="9">
         <v>0.82869999999999999</v>
       </c>
-      <c r="T10" s="8">
+      <c r="T10" s="7">
         <v>0.89859999999999995</v>
       </c>
-      <c r="U10" s="9">
+      <c r="U10" s="8">
         <v>0.8367</v>
       </c>
-      <c r="V10" s="10">
+      <c r="V10" s="9">
         <v>0.86650000000000005</v>
       </c>
-      <c r="W10" s="8">
+      <c r="W10" s="7">
         <v>0.6109</v>
       </c>
-      <c r="X10" s="9">
+      <c r="X10" s="8">
         <v>0.72829999999999995</v>
       </c>
-      <c r="Y10" s="10">
+      <c r="Y10" s="9">
         <v>0.66439999999999999</v>
       </c>
-      <c r="Z10" s="8">
+      <c r="Z10" s="7">
         <v>0.31900000000000001</v>
       </c>
-      <c r="AA10" s="9">
+      <c r="AA10" s="8">
         <v>0.64119999999999999</v>
       </c>
-      <c r="AB10" s="10">
+      <c r="AB10" s="9">
         <v>0.42599999999999999</v>
       </c>
-      <c r="AC10" s="8">
+      <c r="AC10" s="7">
         <v>0.503</v>
       </c>
-      <c r="AD10" s="9">
+      <c r="AD10" s="8">
         <v>0.79779999999999995</v>
       </c>
-      <c r="AE10" s="10">
+      <c r="AE10" s="9">
         <v>0.61699999999999999</v>
       </c>
-      <c r="AF10" s="9">
+      <c r="AF10" s="8">
         <v>0.32969999999999999</v>
       </c>
-      <c r="AG10" s="9">
+      <c r="AG10" s="8">
         <v>0.66320000000000001</v>
       </c>
-      <c r="AH10" s="10">
+      <c r="AH10" s="9">
         <v>0.44040000000000001</v>
       </c>
-      <c r="AI10" s="11">
+      <c r="AI10" s="10">
         <f>AVERAGE(B10,E10,H10,K10,N10,Q10,T10,W10,Z10,AC10,AF10)</f>
         <v>0.5429272727272727</v>
       </c>
-      <c r="AJ10" s="12">
+      <c r="AJ10" s="11">
         <f t="shared" si="2"/>
         <v>0.69146363636363628</v>
       </c>
-      <c r="AK10" s="13">
+      <c r="AK10" s="12">
         <f t="shared" si="3"/>
         <v>0.59812727272727273</v>
       </c>
@@ -1686,114 +1685,114 @@
       <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>0.39410000000000001</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.47189999999999999</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>0.42949999999999999</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>0.31580000000000003</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>0.30869999999999997</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>0.31219999999999998</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <v>0.45590000000000003</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <v>0.64290000000000003</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>0.53349999999999997</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="7">
         <v>0.6925</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="8">
         <v>0.90780000000000005</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="8">
         <v>0.78569999999999995</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <v>0.65669999999999995</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="8">
         <v>0.89770000000000005</v>
       </c>
-      <c r="P11" s="10">
+      <c r="P11" s="9">
         <v>0.75849999999999995</v>
       </c>
-      <c r="Q11" s="8">
+      <c r="Q11" s="7">
         <v>0.73919999999999997</v>
       </c>
-      <c r="R11" s="9">
+      <c r="R11" s="8">
         <v>0.94450000000000001</v>
       </c>
-      <c r="S11" s="10">
+      <c r="S11" s="9">
         <v>0.82930000000000004</v>
       </c>
-      <c r="T11" s="8">
+      <c r="T11" s="7">
         <v>0.77729999999999999</v>
       </c>
-      <c r="U11" s="9">
+      <c r="U11" s="8">
         <v>0.9456</v>
       </c>
-      <c r="V11" s="10">
+      <c r="V11" s="9">
         <v>0.85319999999999996</v>
       </c>
-      <c r="W11" s="8">
+      <c r="W11" s="7">
         <v>0.46829999999999999</v>
       </c>
-      <c r="X11" s="9">
+      <c r="X11" s="8">
         <v>0.94679999999999997</v>
       </c>
-      <c r="Y11" s="10">
+      <c r="Y11" s="9">
         <v>0.62670000000000003</v>
       </c>
-      <c r="Z11" s="8">
+      <c r="Z11" s="7">
         <v>0.4219</v>
       </c>
-      <c r="AA11" s="9">
+      <c r="AA11" s="8">
         <v>0.38600000000000001</v>
       </c>
-      <c r="AB11" s="10">
+      <c r="AB11" s="9">
         <v>0.4032</v>
       </c>
-      <c r="AC11" s="8">
+      <c r="AC11" s="7">
         <v>0.51690000000000003</v>
       </c>
-      <c r="AD11" s="9">
+      <c r="AD11" s="8">
         <v>0.79259999999999997</v>
       </c>
-      <c r="AE11" s="10">
+      <c r="AE11" s="9">
         <v>0.62570000000000003</v>
       </c>
-      <c r="AF11" s="9">
+      <c r="AF11" s="8">
         <v>0.42659999999999998</v>
       </c>
-      <c r="AG11" s="9">
+      <c r="AG11" s="8">
         <v>0.40439999999999998</v>
       </c>
-      <c r="AH11" s="10">
+      <c r="AH11" s="9">
         <v>0.41520000000000001</v>
       </c>
-      <c r="AI11" s="11">
+      <c r="AI11" s="10">
         <f t="shared" ref="AI11" si="4">AVERAGE(B11,E11,H11,K11,N11,Q11,T11,W11,Z11,AC11,AF11)</f>
         <v>0.5331999999999999</v>
       </c>
-      <c r="AJ11" s="12">
+      <c r="AJ11" s="11">
         <f t="shared" ref="AJ11" si="5">AVERAGE(C11,F11,I11,L11,O11,R11,U11,X11,AA11,AD11,AG11)</f>
         <v>0.69535454545454545</v>
       </c>
-      <c r="AK11" s="13">
+      <c r="AK11" s="12">
         <f t="shared" ref="AK11" si="6">AVERAGE(D11,G11,J11,M11,P11,S11,V11,Y11,AB11,AE11,AH11)</f>
         <v>0.59751818181818195</v>
       </c>
@@ -1802,66 +1801,66 @@
       <c r="A12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>0.19470000000000001</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>0.81969999999999998</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>0.31469999999999998</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="8">
+      <c r="H12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="7">
         <v>0.72030000000000005</v>
       </c>
-      <c r="U12" s="9">
+      <c r="U12" s="8">
         <v>0.86199999999999999</v>
       </c>
-      <c r="V12" s="10">
+      <c r="V12" s="9">
         <v>0.78480000000000005</v>
       </c>
-      <c r="W12" s="8"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="10"/>
-      <c r="AC12" s="8">
+      <c r="W12" s="7"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="7">
         <v>0.38229999999999997</v>
       </c>
-      <c r="AD12" s="9">
+      <c r="AD12" s="8">
         <v>0.88829999999999998</v>
       </c>
-      <c r="AE12" s="10">
+      <c r="AE12" s="9">
         <v>0.53459999999999996</v>
       </c>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="10"/>
-      <c r="AI12" s="11">
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="10">
         <f t="shared" ref="AI12:AI15" si="7">AVERAGE(B12,E12,H12,K12,N12,Q12,T12,W12,Z12,AC12,AF12)</f>
         <v>0.43243333333333328</v>
       </c>
-      <c r="AJ12" s="12">
+      <c r="AJ12" s="11">
         <f t="shared" ref="AJ12:AJ15" si="8">AVERAGE(C12,F12,I12,L12,O12,R12,U12,X12,AA12,AD12,AG12)</f>
         <v>0.85666666666666658</v>
       </c>
-      <c r="AK12" s="13">
+      <c r="AK12" s="12">
         <f t="shared" ref="AK12:AK15" si="9">AVERAGE(D12,G12,J12,M12,P12,S12,V12,Y12,AB12,AE12,AH12)</f>
         <v>0.54469999999999996</v>
       </c>
@@ -1870,66 +1869,66 @@
       <c r="A13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>0.5</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>0.1236</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>0.19819999999999999</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="8">
+      <c r="H13" s="7"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="7">
         <v>0.93089999999999995</v>
       </c>
-      <c r="U13" s="9">
+      <c r="U13" s="8">
         <v>0.33550000000000002</v>
       </c>
-      <c r="V13" s="10">
+      <c r="V13" s="9">
         <v>0.49320000000000003</v>
       </c>
-      <c r="W13" s="8"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="10"/>
-      <c r="AC13" s="8">
+      <c r="W13" s="7"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="7">
         <v>0.2908</v>
       </c>
-      <c r="AD13" s="9">
+      <c r="AD13" s="8">
         <v>1.03E-2</v>
       </c>
-      <c r="AE13" s="10">
+      <c r="AE13" s="9">
         <v>0.02</v>
       </c>
-      <c r="AF13" s="9"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="10"/>
-      <c r="AI13" s="11">
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="10">
         <f t="shared" si="7"/>
         <v>0.57389999999999997</v>
       </c>
-      <c r="AJ13" s="12">
+      <c r="AJ13" s="11">
         <f t="shared" si="8"/>
         <v>0.15646666666666667</v>
       </c>
-      <c r="AK13" s="13">
+      <c r="AK13" s="12">
         <f t="shared" si="9"/>
         <v>0.23713333333333333</v>
       </c>
@@ -1938,66 +1937,66 @@
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23">
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="22">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="23">
         <v>0.77370000000000005</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="24">
         <v>0.32279999999999998</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="8">
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="7">
         <v>0.66579999999999995</v>
       </c>
-      <c r="U14" s="9">
+      <c r="U14" s="8">
         <v>0.88560000000000005</v>
       </c>
-      <c r="V14" s="10">
+      <c r="V14" s="9">
         <v>0.7601</v>
       </c>
-      <c r="W14" s="8"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="8">
+      <c r="W14" s="7"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="7">
         <v>0.38019999999999998</v>
       </c>
-      <c r="AD14" s="9">
+      <c r="AD14" s="8">
         <v>0.85519999999999996</v>
       </c>
-      <c r="AE14" s="10">
+      <c r="AE14" s="9">
         <v>0.52639999999999998</v>
       </c>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="11">
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="10">
         <f t="shared" si="7"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="AJ14" s="12">
+      <c r="AJ14" s="11">
         <f t="shared" si="8"/>
         <v>0.83816666666666662</v>
       </c>
-      <c r="AK14" s="13">
+      <c r="AK14" s="12">
         <f t="shared" si="9"/>
         <v>0.53643333333333332</v>
       </c>
@@ -2006,66 +2005,66 @@
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="22">
         <v>0.52129999999999999</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="23">
         <v>0.1389</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="24">
         <v>0.21929999999999999</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="8">
+      <c r="H15" s="20"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="7">
         <v>0.92249999999999999</v>
       </c>
-      <c r="U15" s="9">
+      <c r="U15" s="8">
         <v>0.33489999999999998</v>
       </c>
-      <c r="V15" s="10">
+      <c r="V15" s="9">
         <v>0.4914</v>
       </c>
-      <c r="W15" s="8"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="10"/>
-      <c r="AC15" s="8">
+      <c r="W15" s="7"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="7">
         <v>0.28539999999999999</v>
       </c>
-      <c r="AD15" s="9">
+      <c r="AD15" s="8">
         <v>2.0799999999999999E-2</v>
       </c>
-      <c r="AE15" s="10">
+      <c r="AE15" s="9">
         <v>3.8800000000000001E-2</v>
       </c>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="10"/>
-      <c r="AI15" s="11">
+      <c r="AF15" s="8"/>
+      <c r="AG15" s="8"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="10">
         <f t="shared" si="7"/>
         <v>0.57640000000000002</v>
       </c>
-      <c r="AJ15" s="12">
+      <c r="AJ15" s="11">
         <f t="shared" si="8"/>
         <v>0.16486666666666666</v>
       </c>
-      <c r="AK15" s="13">
+      <c r="AK15" s="12">
         <f t="shared" si="9"/>
         <v>0.24983333333333335</v>
       </c>
@@ -2074,161 +2073,263 @@
       <c r="A16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="10"/>
-      <c r="AI16" s="11"/>
-      <c r="AJ16" s="12"/>
-      <c r="AK16" s="13"/>
+      <c r="B16" s="7">
+        <v>0.34510000000000002</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.52170000000000005</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.41539999999999999</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.44130000000000003</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.33040000000000003</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.47270000000000001</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0.68020000000000003</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.88990000000000002</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="N16" s="7"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="7">
+        <v>0.82679999999999998</v>
+      </c>
+      <c r="U16" s="8">
+        <v>0.90980000000000005</v>
+      </c>
+      <c r="V16" s="9">
+        <v>0.86629999999999996</v>
+      </c>
+      <c r="W16" s="7"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="7">
+        <v>0.34139999999999998</v>
+      </c>
+      <c r="AA16" s="8">
+        <v>0.6149</v>
+      </c>
+      <c r="AB16" s="9">
+        <v>0.439</v>
+      </c>
+      <c r="AC16" s="7">
+        <v>0.50290000000000001</v>
+      </c>
+      <c r="AD16" s="8">
+        <v>0.75060000000000004</v>
+      </c>
+      <c r="AE16" s="9">
+        <v>0.60229999999999995</v>
+      </c>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="10">
+        <f t="shared" ref="AI16:AI17" si="10">AVERAGE(B16,E16,H16,K16,N16,Q16,T16,W16,Z16,AC16,AF16)</f>
+        <v>0.49852857142857143</v>
+      </c>
+      <c r="AJ16" s="11">
+        <f t="shared" ref="AJ16:AJ17" si="11">AVERAGE(C16,F16,I16,L16,O16,R16,U16,X16,AA16,AD16,AG16)</f>
+        <v>0.65727142857142862</v>
+      </c>
+      <c r="AK16" s="12">
+        <f t="shared" ref="AK16:AK17" si="12">AVERAGE(D16,G16,J16,M16,P16,S16,V16,Y16,AB16,AE16,AH16)</f>
+        <v>0.56054285714285712</v>
+      </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="10"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="11"/>
-      <c r="AJ17" s="12"/>
-      <c r="AK17" s="13"/>
+      <c r="B17" s="7">
+        <v>0.49569999999999997</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.4007</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.44319999999999998</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.27639999999999998</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.40889999999999999</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.32979999999999998</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.41049999999999998</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.51559999999999995</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.45710000000000001</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0.74680000000000002</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.85360000000000003</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0.79659999999999997</v>
+      </c>
+      <c r="N17" s="7"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="7">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="U17" s="8">
+        <v>0.86619999999999997</v>
+      </c>
+      <c r="V17" s="9">
+        <v>0.86360000000000003</v>
+      </c>
+      <c r="W17" s="7"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="7">
+        <v>0.31369999999999998</v>
+      </c>
+      <c r="AA17" s="8">
+        <v>0.3992</v>
+      </c>
+      <c r="AB17" s="9">
+        <v>0.3513</v>
+      </c>
+      <c r="AC17" s="7">
+        <v>0.49759999999999999</v>
+      </c>
+      <c r="AD17" s="8">
+        <v>0.70330000000000004</v>
+      </c>
+      <c r="AE17" s="9">
+        <v>0.58279999999999998</v>
+      </c>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="10">
+        <f t="shared" si="10"/>
+        <v>0.51452857142857134</v>
+      </c>
+      <c r="AJ17" s="11">
+        <f t="shared" si="11"/>
+        <v>0.59250000000000003</v>
+      </c>
+      <c r="AK17" s="12">
+        <f t="shared" si="12"/>
+        <v>0.54634285714285713</v>
+      </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="9"/>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="9"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="11"/>
-      <c r="AJ18" s="12"/>
-      <c r="AK18" s="13"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="8"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="10"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="12"/>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="9"/>
-      <c r="AB19" s="10"/>
-      <c r="AC19" s="8"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="9"/>
-      <c r="AH19" s="10"/>
-      <c r="AI19" s="11"/>
-      <c r="AJ19" s="12"/>
-      <c r="AK19" s="13"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="10"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="12"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -2282,6 +2383,42 @@
     <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G9">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J9">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -2293,7 +2430,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G9">
+  <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -2305,7 +2442,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -2317,7 +2454,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M9">
+  <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2329,7 +2466,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P9">
+  <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -2341,7 +2478,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S9">
+  <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -2353,7 +2490,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V9">
+  <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2365,7 +2502,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y9">
+  <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2377,7 +2514,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB9">
+  <conditionalFormatting sqref="AK3:AK19">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2389,7 +2526,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE9">
+  <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -2401,7 +2538,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH9">
+  <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2413,7 +2550,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK3:AK19">
+  <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2425,7 +2562,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D11">
+  <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2437,7 +2574,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G11">
+  <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2449,7 +2586,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J11">
+  <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2461,7 +2598,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M11">
+  <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2473,7 +2610,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P11">
+  <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2485,7 +2622,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S11">
+  <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2497,7 +2634,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V11">
+  <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2509,7 +2646,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y11">
+  <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2521,7 +2658,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB11">
+  <conditionalFormatting sqref="G3:G19">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2533,7 +2670,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE11">
+  <conditionalFormatting sqref="V3:V19">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2545,7 +2682,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH11">
+  <conditionalFormatting sqref="AE3:AE19">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2557,7 +2694,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G19">
+  <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2569,7 +2706,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V19">
+  <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2581,7 +2718,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE19">
+  <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2600,10 +2737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH18"/>
+  <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,57 +2885,57 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>0.46100000000000002</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>0.45700000000000002</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>0.45900000000000002</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>0.52400000000000002</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>0.45500000000000002</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>0.48699999999999999</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>0.20899999999999999</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <v>0.61299999999999999</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <v>0.312</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>0.28799999999999998</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <v>0.54100000000000004</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="12">
         <v>0.376</v>
       </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="8">
+      <c r="N3" s="10"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="7">
         <f>AVERAGE(B3,E3,H3,K3,N3,Q3)</f>
         <v>0.37050000000000005</v>
       </c>
-      <c r="U3" s="9">
+      <c r="U3" s="8">
         <f>AVERAGE(C3,F3,I3,L3,O3,R3)</f>
         <v>0.51649999999999996</v>
       </c>
-      <c r="V3" s="10">
+      <c r="V3" s="9">
         <f>AVERAGE(D3,G3,J3,M3,P3,S3)</f>
         <v>0.40849999999999997</v>
       </c>
@@ -2807,57 +2944,57 @@
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>0.46899999999999997</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>0.51100000000000001</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>0.48899999999999999</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>0.51600000000000001</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>0.46300000000000002</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>0.48799999999999999</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>0.23899999999999999</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <v>0.61199999999999999</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <v>0.34300000000000003</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="11">
         <v>0.54600000000000004</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="12">
         <v>0.379</v>
       </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="8">
+      <c r="N4" s="10"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="7">
         <f t="shared" ref="T4:T8" si="0">AVERAGE(B4,E4,H4,K4,N4,Q4)</f>
         <v>0.3785</v>
       </c>
-      <c r="U4" s="9">
+      <c r="U4" s="8">
         <f t="shared" ref="U4:U8" si="1">AVERAGE(C4,F4,I4,L4,O4,R4)</f>
         <v>0.53299999999999992</v>
       </c>
-      <c r="V4" s="10">
+      <c r="V4" s="9">
         <f t="shared" ref="V4:V8" si="2">AVERAGE(D4,G4,J4,M4,P4,S4)</f>
         <v>0.42475000000000002</v>
       </c>
@@ -2866,57 +3003,57 @@
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>0.16</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>0.55500000000000005</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.248</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>0.53600000000000003</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>0.372</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>0.439</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>0.02</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <v>0.30199999999999999</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <v>0.65200000000000002</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="12">
         <v>0.41199999999999998</v>
       </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="8">
+      <c r="N5" s="10"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="7">
         <f t="shared" si="0"/>
         <v>0.2545</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="8">
         <f t="shared" si="1"/>
         <v>0.39550000000000002</v>
       </c>
-      <c r="V5" s="10">
+      <c r="V5" s="9">
         <f t="shared" si="2"/>
         <v>0.27600000000000002</v>
       </c>
@@ -2925,57 +3062,57 @@
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>0.40400000000000003</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>0.51200000000000001</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>0.45200000000000001</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>0.52800000000000002</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>0.38400000000000001</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>0.44400000000000001</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <v>0.27300000000000002</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <v>0.54400000000000004</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="16">
         <v>0.36299999999999999</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <v>0.311</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <v>0.77700000000000002</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="16">
         <v>0.44400000000000001</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="8">
+      <c r="N6" s="10"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="7">
         <f t="shared" si="0"/>
         <v>0.379</v>
       </c>
-      <c r="U6" s="9">
+      <c r="U6" s="8">
         <f t="shared" si="1"/>
         <v>0.55425000000000002</v>
       </c>
-      <c r="V6" s="10">
+      <c r="V6" s="9">
         <f t="shared" si="2"/>
         <v>0.42574999999999996</v>
       </c>
@@ -2984,69 +3121,69 @@
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>0.23719999999999999</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>0.36880000000000002</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>0.28870000000000001</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>0.52629999999999999</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>0.4753</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>0.4995</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <v>0.30249999999999999</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>0.1711</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <v>0.21859999999999999</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="15">
         <v>0.36120000000000002</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <v>0.45269999999999999</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="12">
         <v>0.40179999999999999</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="15">
         <v>0.75680000000000003</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="13">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="P7" s="17">
+      <c r="P7" s="16">
         <v>5.0700000000000002E-2</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q7" s="10">
         <v>0.23649999999999999</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7" s="13">
         <v>0.62429999999999997</v>
       </c>
-      <c r="S7" s="17">
+      <c r="S7" s="16">
         <v>0.34300000000000003</v>
       </c>
-      <c r="T7" s="8">
+      <c r="T7" s="7">
         <f t="shared" si="0"/>
         <v>0.40341666666666659</v>
       </c>
-      <c r="U7" s="9">
+      <c r="U7" s="8">
         <f t="shared" si="1"/>
         <v>0.3530666666666667</v>
       </c>
-      <c r="V7" s="10">
+      <c r="V7" s="9">
         <f t="shared" si="2"/>
         <v>0.30038333333333328</v>
       </c>
@@ -3055,69 +3192,69 @@
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>0.62619999999999998</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>0.42080000000000001</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>0.50329999999999997</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="15">
         <v>0.67179999999999995</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>0.45319999999999999</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <v>0.54120000000000001</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>0.2737</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>6.2199999999999998E-2</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="12">
         <v>0.10100000000000001</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <v>0.28420000000000001</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="11">
         <v>0.48730000000000001</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <v>0.35899999999999999</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="10">
         <v>0.69089999999999996</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="11">
         <v>3.56E-2</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="12">
         <v>6.7699999999999996E-2</v>
       </c>
-      <c r="Q8" s="11">
+      <c r="Q8" s="10">
         <v>0.35859999999999997</v>
       </c>
-      <c r="R8" s="12">
+      <c r="R8" s="11">
         <v>0.53359999999999996</v>
       </c>
-      <c r="S8" s="13">
+      <c r="S8" s="12">
         <v>0.4289</v>
       </c>
-      <c r="T8" s="8">
+      <c r="T8" s="7">
         <f t="shared" si="0"/>
         <v>0.48423333333333335</v>
       </c>
-      <c r="U8" s="9">
+      <c r="U8" s="8">
         <f t="shared" si="1"/>
         <v>0.33211666666666667</v>
       </c>
-      <c r="V8" s="10">
+      <c r="V8" s="9">
         <f t="shared" si="2"/>
         <v>0.33351666666666668</v>
       </c>
@@ -3126,69 +3263,69 @@
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>0.17879999999999999</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0.53620000000000001</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>0.2681</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>0.65390000000000004</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>0.44230000000000003</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>0.52769999999999995</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>5.74E-2</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="8">
         <v>0.55200000000000005</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>0.10390000000000001</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="7">
         <v>0.28110000000000002</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <v>0.70089999999999997</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="9">
         <v>0.40129999999999999</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <v>5.7299999999999997E-2</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="8">
         <v>0.72819999999999996</v>
       </c>
-      <c r="P9" s="10">
+      <c r="P9" s="9">
         <v>0.10630000000000001</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="Q9" s="7">
         <v>0.19520000000000001</v>
       </c>
-      <c r="R9" s="9">
+      <c r="R9" s="8">
         <v>0.83430000000000004</v>
       </c>
-      <c r="S9" s="10">
+      <c r="S9" s="9">
         <v>0.31630000000000003</v>
       </c>
-      <c r="T9" s="8">
+      <c r="T9" s="7">
         <f t="shared" ref="T9:T10" si="3">AVERAGE(B9,E9,H9,K9,N9,Q9)</f>
         <v>0.23728333333333332</v>
       </c>
-      <c r="U9" s="9">
+      <c r="U9" s="8">
         <f t="shared" ref="U9:U10" si="4">AVERAGE(C9,F9,I9,L9,O9,R9)</f>
         <v>0.63231666666666664</v>
       </c>
-      <c r="V9" s="10">
+      <c r="V9" s="9">
         <f t="shared" ref="V9:V10" si="5">AVERAGE(D9,G9,J9,M9,P9,S9)</f>
         <v>0.28726666666666667</v>
       </c>
@@ -3197,69 +3334,69 @@
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>0.63719999999999999</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.48530000000000001</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>0.55100000000000005</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>0.65390000000000004</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>0.44230000000000003</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>0.52769999999999995</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>0.2051</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>0.104</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>0.13800000000000001</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="7">
         <v>0.27329999999999999</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="8">
         <v>0.83299999999999996</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <v>0.41160000000000002</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <v>1</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="8">
         <v>3.56E-2</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="9">
         <v>6.88E-2</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="Q10" s="7">
         <v>0.34899999999999998</v>
       </c>
-      <c r="R10" s="9">
+      <c r="R10" s="8">
         <v>0.53939999999999999</v>
       </c>
-      <c r="S10" s="10">
+      <c r="S10" s="9">
         <v>0.42380000000000001</v>
       </c>
-      <c r="T10" s="8">
+      <c r="T10" s="7">
         <f t="shared" si="3"/>
         <v>0.51975000000000005</v>
       </c>
-      <c r="U10" s="9">
+      <c r="U10" s="8">
         <f t="shared" si="4"/>
         <v>0.40660000000000002</v>
       </c>
-      <c r="V10" s="10">
+      <c r="V10" s="9">
         <f t="shared" si="5"/>
         <v>0.35348333333333332</v>
       </c>
@@ -3268,51 +3405,51 @@
       <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>0.1303</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.76329999999999998</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>0.22259999999999999</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>0.31159999999999999</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>0.9264</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>0.46629999999999999</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <v>5.4899999999999997E-2</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <v>0.97599999999999998</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>0.104</v>
       </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="8">
+      <c r="K11" s="7"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="7">
         <f>AVERAGE(B11,E11,H11,K11,N11,Q11)</f>
         <v>0.1656</v>
       </c>
-      <c r="U11" s="9">
+      <c r="U11" s="8">
         <f>AVERAGE(C11,F11,I11,L11,O11,R11)</f>
         <v>0.88856666666666673</v>
       </c>
-      <c r="V11" s="10">
+      <c r="V11" s="9">
         <f>AVERAGE(D11,G11,J11,M11,P11,S11)</f>
         <v>0.26429999999999998</v>
       </c>
@@ -3321,52 +3458,52 @@
       <c r="A12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>0.24199999999999999</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>0.4909</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>0.32419999999999999</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>0.3306</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>0.86760000000000004</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>0.4788</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>5.5399999999999998E-2</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <v>0.97050000000000003</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>0.1047</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="8">
-        <f t="shared" ref="T12:T14" si="6">AVERAGE(B12,E12,H12,K12,N12,Q12)</f>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="7">
+        <f t="shared" ref="T12:T16" si="6">AVERAGE(B12,E12,H12,K12,N12,Q12)</f>
         <v>0.20933333333333334</v>
       </c>
-      <c r="U12" s="9">
-        <f t="shared" ref="U12:U14" si="7">AVERAGE(C12,F12,I12,L12,O12,R12)</f>
+      <c r="U12" s="8">
+        <f t="shared" ref="U12:U16" si="7">AVERAGE(C12,F12,I12,L12,O12,R12)</f>
         <v>0.77633333333333343</v>
       </c>
-      <c r="V12" s="10">
-        <f t="shared" ref="V12:V14" si="8">AVERAGE(D12,G12,J12,M12,P12,S12)</f>
+      <c r="V12" s="9">
+        <f t="shared" ref="V12:V16" si="8">AVERAGE(D12,G12,J12,M12,P12,S12)</f>
         <v>0.30256666666666665</v>
       </c>
     </row>
@@ -3374,51 +3511,51 @@
       <c r="A13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>0.16300000000000001</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>0.74350000000000005</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>0.26740000000000003</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>0.31790000000000002</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>0.91090000000000004</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>0.4713</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>5.4199999999999998E-2</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <v>0.9748</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>0.1026</v>
       </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="8">
+      <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="7">
         <f>AVERAGE(B13,E13,H13,K13,N13,Q13)</f>
         <v>0.17836666666666667</v>
       </c>
-      <c r="U13" s="9">
+      <c r="U13" s="8">
         <f>AVERAGE(C13,F13,I13,L13,O13,R13)</f>
         <v>0.87639999999999996</v>
       </c>
-      <c r="V13" s="10">
+      <c r="V13" s="9">
         <f>AVERAGE(D13,G13,J13,M13,P13,S13)</f>
         <v>0.28043333333333337</v>
       </c>
@@ -3427,137 +3564,276 @@
       <c r="A14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>0.19009999999999999</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>0.5091</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>0.27679999999999999</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>0.31850000000000001</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>0.95520000000000005</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>0.47770000000000001</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="8">
         <v>0.95689999999999997</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
         <v>0.1086</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="8">
+      <c r="K14" s="7"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="7">
         <f t="shared" si="6"/>
         <v>0.18873333333333331</v>
       </c>
-      <c r="U14" s="9">
+      <c r="U14" s="8">
         <f t="shared" si="7"/>
         <v>0.80706666666666671</v>
       </c>
-      <c r="V14" s="10">
+      <c r="V14" s="9">
         <f t="shared" si="8"/>
         <v>0.28770000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.28349999999999997</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.53120000000000001</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.36969999999999997</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.38879999999999998</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.7107</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.50270000000000004</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0.32640000000000002</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.45660000000000001</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.38069999999999998</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0.32140000000000002</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.42270000000000002</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0.36520000000000002</v>
+      </c>
       <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="9"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33002500000000001</v>
+      </c>
+      <c r="U15" s="8">
+        <f t="shared" si="7"/>
+        <v>0.53029999999999999</v>
+      </c>
+      <c r="V15" s="9">
+        <f t="shared" si="8"/>
+        <v>0.40457500000000002</v>
+      </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="A16" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.58560000000000001</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.4521</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.51019999999999999</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.49009999999999998</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.68130000000000002</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0.57010000000000005</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.21260000000000001</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.29160000000000003</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0.34210000000000002</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.48859999999999998</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0.40239999999999998</v>
+      </c>
       <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="9"/>
       <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="7">
+        <f t="shared" si="6"/>
+        <v>0.40760000000000002</v>
+      </c>
+      <c r="U16" s="8">
+        <f t="shared" si="7"/>
+        <v>0.52149999999999996</v>
+      </c>
+      <c r="V16" s="9">
+        <f t="shared" si="8"/>
+        <v>0.44357500000000005</v>
+      </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
       <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="9"/>
       <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="9"/>
       <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="9"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="9"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="9"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3574,6 +3850,30 @@
     <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G10">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3585,7 +3885,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G10">
+  <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3597,7 +3897,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10">
+  <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3609,7 +3909,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M10">
+  <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3621,7 +3921,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P7:P10">
+  <conditionalFormatting sqref="V3:V20">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3633,7 +3933,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S7:S10">
+  <conditionalFormatting sqref="D3:D20">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3645,7 +3945,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V14">
+  <conditionalFormatting sqref="G3:G20">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3657,7 +3957,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D14">
+  <conditionalFormatting sqref="J3:J20">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3669,7 +3969,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G14">
+  <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3681,7 +3981,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J14">
+  <conditionalFormatting sqref="M3:M16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Newest results with joint training.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <t>F1</t>
   </si>
   <si>
-    <t>Psyche (trained on DISFA and using multiple bins, neutral is extracted through a median)</t>
-  </si>
-  <si>
     <t>AU1</t>
   </si>
   <si>
@@ -81,15 +78,9 @@
     <t>AU45</t>
   </si>
   <si>
-    <t>DISFA training with generic PCA and new alignment (masked and bigger), static model</t>
-  </si>
-  <si>
     <t>BP4D trained (static), generic PCA</t>
   </si>
   <si>
-    <t>DISFA training with generic PCA and new alignment (masked and bigger), dynamic model</t>
-  </si>
-  <si>
     <t>SEMAINE trained (static), generic PCA</t>
   </si>
   <si>
@@ -166,6 +157,15 @@
   </si>
   <si>
     <t>Combined train, dynamic</t>
+  </si>
+  <si>
+    <t>Psyche (trained on DISFA and using mult bins, neutral is extracted through a median)</t>
+  </si>
+  <si>
+    <t>DISFA training with generic PCA and new alignment, static model</t>
+  </si>
+  <si>
+    <t>DISFA training with generic PCA and new alignment, dynamic model</t>
   </si>
 </sst>
 </file>
@@ -664,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,62 +676,62 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1" s="28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
       <c r="E1" s="28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="26"/>
       <c r="G1" s="26"/>
       <c r="H1" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
       <c r="K1" s="28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
       <c r="N1" s="28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O1" s="26"/>
       <c r="P1" s="27"/>
       <c r="Q1" s="28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R1" s="26"/>
       <c r="S1" s="27"/>
       <c r="T1" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U1" s="26"/>
       <c r="V1" s="27"/>
       <c r="W1" s="28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X1" s="26"/>
       <c r="Y1" s="27"/>
       <c r="Z1" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA1" s="26"/>
       <c r="AB1" s="27"/>
       <c r="AC1" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AD1" s="26"/>
       <c r="AE1" s="27"/>
       <c r="AF1" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG1" s="26"/>
       <c r="AH1" s="27"/>
       <c r="AI1" s="26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AJ1" s="26"/>
       <c r="AK1" s="27"/>
@@ -741,109 +741,109 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="T2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="W2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="Z2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="AB2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="AC2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="AE2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="AF2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="AH2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="AI2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="AK2" s="4" t="s">
         <v>1</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="10">
         <v>0.48799999999999999</v>
@@ -890,22 +890,22 @@
         <v>0.496</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T3" s="10">
         <v>0.98</v>
@@ -917,22 +917,22 @@
         <v>0.41199999999999998</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="X3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AB3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AC3" s="10">
         <v>0.89</v>
@@ -944,13 +944,13 @@
         <v>5.5E-2</v>
       </c>
       <c r="AF3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AG3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AH3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI3" s="17">
         <f>AVERAGE(B3,E3,H3,K3,N3,Q3,T3,W3,Z3,AC3,AF3)</f>
@@ -967,7 +967,7 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>0.498</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="10">
         <v>0.39</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" s="10">
         <v>0.52600000000000002</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" s="15">
         <v>0.59199999999999997</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="10">
         <v>0.3589</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="10">
         <v>0.39240000000000003</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7">
         <v>0.3664</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7">
         <v>0.39410000000000001</v>
@@ -1799,7 +1799,7 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" s="7">
         <v>0.34510000000000002</v>
@@ -2163,7 +2163,7 @@
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" s="7">
         <v>0.49569999999999997</v>
@@ -2254,7 +2254,7 @@
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -2293,7 +2293,7 @@
       <c r="AK18" s="12"/>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -2739,13 +2739,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" customWidth="1"/>
+    <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
     <col min="3" max="6" width="5.140625" customWidth="1"/>
     <col min="7" max="7" width="4.85546875" customWidth="1"/>
@@ -2766,37 +2766,37 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" s="28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
       <c r="E1" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="26"/>
       <c r="G1" s="27"/>
       <c r="H1" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="27"/>
       <c r="K1" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L1" s="26"/>
       <c r="M1" s="27"/>
       <c r="N1" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O1" s="26"/>
       <c r="P1" s="27"/>
       <c r="Q1" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R1" s="26"/>
       <c r="S1" s="27"/>
       <c r="T1" s="28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="U1" s="26"/>
       <c r="V1" s="27"/>
@@ -2818,64 +2818,64 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="T2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>1</v>
@@ -2883,7 +2883,7 @@
     </row>
     <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B3" s="10">
         <v>0.46100000000000002</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>0.46899999999999997</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B5" s="10">
         <v>0.16</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B6" s="10">
         <v>0.40400000000000003</v>
@@ -3119,7 +3119,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="10">
         <v>0.23719999999999999</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="15">
         <v>0.62619999999999998</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
         <v>0.17879999999999999</v>
@@ -3332,7 +3332,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7">
         <v>0.63719999999999999</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11" s="7">
         <v>0.1303</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" s="7">
         <v>0.24199999999999999</v>
@@ -3509,7 +3509,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="7">
         <v>0.16300000000000001</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="7">
         <v>0.19009999999999999</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B15" s="7">
         <v>0.28349999999999997</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B16" s="7">
         <v>0.58560000000000001</v>
@@ -3733,7 +3733,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -3759,7 +3759,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -3785,7 +3785,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -3811,7 +3811,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -4003,7 +4003,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Some more intensity results.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -702,7 +702,7 @@
   <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE19" sqref="AE19"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3003,7 +3003,7 @@
   <dimension ref="A1:AH22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="F19" sqref="F19:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4402,7 +4402,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4576,35 +4576,87 @@
       <c r="A5" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="9"/>
+      <c r="B5" s="7">
+        <v>0.73160000000000003</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.97030000000000005</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.7097</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1.0558000000000001</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.83860000000000001</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.85189999999999999</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.50409999999999999</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1.2313000000000001</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1.1224000000000001</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" ref="L5:L6" si="0">AVERAGE(D5,F5,H5,J5)</f>
+        <v>0.63485000000000003</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" ref="M5:M6" si="1">AVERAGE(E5,G5,I5,K5)</f>
+        <v>1.06535</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="9"/>
+      <c r="B6" s="7">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1.0331999999999999</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.5756</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1.2736000000000001</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.75049999999999994</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1.0584</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.38679999999999998</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1.403</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.43230000000000002</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.96440000000000003</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.5363</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="1"/>
+        <v>1.1748499999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">

</xml_diff>

<commit_message>
Updated results (to reflect added regularisation)
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="62">
   <si>
     <t>DEVEL</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>Trained on intensity (dynamic) - ruonded</t>
+  </si>
+  <si>
+    <t>BP4D trained (static) logistic regression</t>
+  </si>
+  <si>
+    <t>BP4D trained (static) logistic regression - tanh</t>
   </si>
 </sst>
 </file>
@@ -345,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -397,6 +403,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -701,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,103 +2458,505 @@
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="8"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="8"/>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="8"/>
-      <c r="AG20" s="8"/>
-      <c r="AH20" s="9"/>
-      <c r="AI20" s="10"/>
-      <c r="AJ20" s="11"/>
-      <c r="AK20" s="12"/>
+      <c r="A20" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.3674</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.44390000000000002</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.37159999999999999</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.29289999999999999</v>
+      </c>
+      <c r="F20" s="32">
+        <v>0.39040000000000002</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.33410000000000001</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0.37959999999999999</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.52580000000000005</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.44019999999999998</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0.72040000000000004</v>
+      </c>
+      <c r="L20" s="32">
+        <v>0.79179999999999995</v>
+      </c>
+      <c r="M20" s="8">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0.66690000000000005</v>
+      </c>
+      <c r="O20" s="8">
+        <v>0.85360000000000003</v>
+      </c>
+      <c r="P20" s="8">
+        <v>0.73850000000000005</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>0.71560000000000001</v>
+      </c>
+      <c r="R20" s="8">
+        <v>0.94889999999999997</v>
+      </c>
+      <c r="S20" s="9">
+        <v>0.81579999999999997</v>
+      </c>
+      <c r="T20" s="7">
+        <v>0.86739999999999995</v>
+      </c>
+      <c r="U20" s="8">
+        <v>0.81869999999999998</v>
+      </c>
+      <c r="V20" s="9">
+        <v>0.84140000000000004</v>
+      </c>
+      <c r="W20" s="7">
+        <v>0.5464</v>
+      </c>
+      <c r="X20" s="8">
+        <v>0.69489999999999996</v>
+      </c>
+      <c r="Y20" s="8">
+        <v>0.60360000000000003</v>
+      </c>
+      <c r="Z20" s="7">
+        <v>0.31490000000000001</v>
+      </c>
+      <c r="AA20" s="8">
+        <v>0.62809999999999999</v>
+      </c>
+      <c r="AB20" s="8">
+        <v>0.41839999999999999</v>
+      </c>
+      <c r="AC20" s="7">
+        <v>0.51480000000000004</v>
+      </c>
+      <c r="AD20" s="8">
+        <v>0.74239999999999995</v>
+      </c>
+      <c r="AE20" s="8">
+        <v>0.59309999999999996</v>
+      </c>
+      <c r="AF20" s="7">
+        <v>0.43809999999999999</v>
+      </c>
+      <c r="AG20" s="8">
+        <v>0.42959999999999998</v>
+      </c>
+      <c r="AH20" s="9">
+        <v>0.42180000000000001</v>
+      </c>
+      <c r="AI20" s="10">
+        <f>AVERAGE(B20,E20,H20,K20,N20,Q20,T20,W20,Z20,AC20,AF20)</f>
+        <v>0.52949090909090912</v>
+      </c>
+      <c r="AJ20" s="11">
+        <f>AVERAGE(C20,F20,I20,L20,O20,R20,U20,X20,AA20,AD20,AG20)</f>
+        <v>0.66073636363636357</v>
+      </c>
+      <c r="AK20" s="12">
+        <f>AVERAGE(D20,G20,J20,M20,P20,S20,V20,Y20,AB20,AE20,AH20)</f>
+        <v>0.57558181818181819</v>
+      </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="8"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="8"/>
-      <c r="AG21" s="8"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="10"/>
-      <c r="AJ21" s="11"/>
-      <c r="AK21" s="12"/>
+      <c r="A21" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.3196</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.50070000000000003</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.3891</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.3054</v>
+      </c>
+      <c r="F21" s="32">
+        <v>0.42159999999999997</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.35420000000000001</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0.38779999999999998</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0.5534</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0.65920000000000001</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0.82569999999999999</v>
+      </c>
+      <c r="M21" s="8">
+        <v>0.73309999999999997</v>
+      </c>
+      <c r="N21" s="7">
+        <v>0.68159999999999998</v>
+      </c>
+      <c r="O21" s="8">
+        <v>0.87839999999999996</v>
+      </c>
+      <c r="P21" s="8">
+        <v>0.76759999999999995</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0.77390000000000003</v>
+      </c>
+      <c r="R21" s="8">
+        <v>0.88729999999999998</v>
+      </c>
+      <c r="S21" s="9">
+        <v>0.8266</v>
+      </c>
+      <c r="T21" s="7">
+        <v>0.84009999999999996</v>
+      </c>
+      <c r="U21" s="8">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="V21" s="9">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="W21" s="7">
+        <v>0.52180000000000004</v>
+      </c>
+      <c r="X21" s="8">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="Y21" s="9">
+        <v>0.63249999999999995</v>
+      </c>
+      <c r="Z21" s="7">
+        <v>0.314</v>
+      </c>
+      <c r="AA21" s="8">
+        <v>0.68410000000000004</v>
+      </c>
+      <c r="AB21" s="9">
+        <v>0.42920000000000003</v>
+      </c>
+      <c r="AC21" s="7">
+        <v>0.47970000000000002</v>
+      </c>
+      <c r="AD21" s="8">
+        <v>0.81040000000000001</v>
+      </c>
+      <c r="AE21" s="9">
+        <v>0.60260000000000002</v>
+      </c>
+      <c r="AF21" s="8">
+        <v>0.35670000000000002</v>
+      </c>
+      <c r="AG21" s="8">
+        <v>0.56879999999999997</v>
+      </c>
+      <c r="AH21" s="9">
+        <v>0.43590000000000001</v>
+      </c>
+      <c r="AI21" s="10">
+        <f t="shared" ref="AI21" si="16">AVERAGE(B21,E21,H21,K21,N21,Q21,T21,W21,Z21,AC21,AF21)</f>
+        <v>0.512709090909091</v>
+      </c>
+      <c r="AJ21" s="11">
+        <f t="shared" ref="AJ21" si="17">AVERAGE(C21,F21,I21,L21,O21,R21,U21,X21,AA21,AD21,AG21)</f>
+        <v>0.7105818181818182</v>
+      </c>
+      <c r="AK21" s="12">
+        <f t="shared" ref="AK21" si="18">AVERAGE(D21,G21,J21,M21,P21,S21,V21,Y21,AB21,AE21,AH21)</f>
+        <v>0.58974545454545457</v>
+      </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="33"/>
+      <c r="S22" s="33"/>
+      <c r="T22" s="33"/>
+      <c r="U22" s="33"/>
+      <c r="V22" s="33"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="33"/>
+      <c r="Y22" s="33"/>
+      <c r="Z22" s="33"/>
+      <c r="AA22" s="33"/>
+      <c r="AB22" s="33"/>
+      <c r="AC22" s="33"/>
+      <c r="AD22" s="33"/>
+      <c r="AE22" s="33"/>
+      <c r="AF22" s="33"/>
+      <c r="AG22" s="33"/>
+      <c r="AH22" s="33"/>
+      <c r="AI22" s="10"/>
+      <c r="AJ22" s="11"/>
+      <c r="AK22" s="12"/>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="33"/>
+      <c r="U23" s="33"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="33"/>
+      <c r="X23" s="33"/>
+      <c r="Y23" s="33"/>
+      <c r="Z23" s="33"/>
+      <c r="AA23" s="33"/>
+      <c r="AB23" s="33"/>
+      <c r="AC23" s="33"/>
+      <c r="AD23" s="33"/>
+      <c r="AE23" s="33"/>
+      <c r="AF23" s="33"/>
+      <c r="AG23" s="33"/>
+      <c r="AH23" s="33"/>
+      <c r="AI23" s="10"/>
+      <c r="AJ23" s="11"/>
+      <c r="AK23" s="12"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="33"/>
+      <c r="Y24" s="33"/>
+      <c r="Z24" s="33"/>
+      <c r="AA24" s="33"/>
+      <c r="AB24" s="33"/>
+      <c r="AC24" s="33"/>
+      <c r="AD24" s="33"/>
+      <c r="AE24" s="33"/>
+      <c r="AF24" s="33"/>
+      <c r="AG24" s="33"/>
+      <c r="AH24" s="33"/>
+      <c r="AI24" s="10"/>
+      <c r="AJ24" s="11"/>
+      <c r="AK24" s="12"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="33"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="33"/>
+      <c r="U25" s="33"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="33"/>
+      <c r="X25" s="33"/>
+      <c r="Y25" s="33"/>
+      <c r="Z25" s="33"/>
+      <c r="AA25" s="33"/>
+      <c r="AB25" s="33"/>
+      <c r="AC25" s="33"/>
+      <c r="AD25" s="33"/>
+      <c r="AE25" s="33"/>
+      <c r="AF25" s="33"/>
+      <c r="AG25" s="33"/>
+      <c r="AH25" s="33"/>
+      <c r="AI25" s="10"/>
+      <c r="AJ25" s="11"/>
+      <c r="AK25" s="12"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
+      <c r="R26" s="33"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="33"/>
+      <c r="U26" s="33"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
+      <c r="X26" s="33"/>
+      <c r="Y26" s="33"/>
+      <c r="Z26" s="33"/>
+      <c r="AA26" s="33"/>
+      <c r="AB26" s="33"/>
+      <c r="AC26" s="33"/>
+      <c r="AD26" s="33"/>
+      <c r="AE26" s="33"/>
+      <c r="AF26" s="33"/>
+      <c r="AG26" s="33"/>
+      <c r="AH26" s="33"/>
+      <c r="AI26" s="10"/>
+      <c r="AJ26" s="11"/>
+      <c r="AK26" s="12"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="33"/>
+      <c r="T27" s="33"/>
+      <c r="U27" s="33"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="33"/>
+      <c r="X27" s="33"/>
+      <c r="Y27" s="33"/>
+      <c r="Z27" s="33"/>
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="33"/>
+      <c r="AD27" s="33"/>
+      <c r="AE27" s="33"/>
+      <c r="AF27" s="33"/>
+      <c r="AG27" s="33"/>
+      <c r="AH27" s="33"/>
+      <c r="AI27" s="10"/>
+      <c r="AJ27" s="11"/>
+      <c r="AK27" s="12"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="33"/>
+      <c r="X28" s="33"/>
+      <c r="Y28" s="33"/>
+      <c r="Z28" s="33"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="33"/>
+      <c r="AC28" s="33"/>
+      <c r="AD28" s="33"/>
+      <c r="AE28" s="33"/>
+      <c r="AF28" s="33"/>
+      <c r="AG28" s="33"/>
+      <c r="AH28" s="33"/>
+      <c r="AI28" s="10"/>
+      <c r="AJ28" s="11"/>
+      <c r="AK28" s="12"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -2574,6 +2983,174 @@
     <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G9">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J9">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M9">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P9">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S9">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V9">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y9">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB9">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE9">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH9">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK3:AK28">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D17">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G11">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -2585,7 +3162,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G9">
+  <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -2597,7 +3174,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -2609,7 +3186,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M9">
+  <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -2621,7 +3198,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P9">
+  <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -2633,7 +3210,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S9">
+  <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -2645,7 +3222,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V9">
+  <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2657,7 +3234,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y9">
+  <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2669,7 +3246,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB9">
+  <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2681,7 +3258,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE9">
+  <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -2693,7 +3270,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH9">
+  <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -2705,7 +3282,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK3:AK21">
+  <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -2717,7 +3294,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D17">
+  <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2729,7 +3306,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G11">
+  <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -2741,7 +3318,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J11">
+  <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -2753,7 +3330,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M11">
+  <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2765,7 +3342,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P11">
+  <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2777,7 +3354,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S11">
+  <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2789,7 +3366,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V11">
+  <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -2801,7 +3378,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y11">
+  <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2813,7 +3390,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB11">
+  <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2825,7 +3402,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE11">
+  <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2837,7 +3414,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH11">
+  <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2849,7 +3426,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G21">
+  <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2861,7 +3438,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V21">
+  <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2873,7 +3450,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE21">
+  <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2885,7 +3462,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J17">
+  <conditionalFormatting sqref="P3:P27">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2897,7 +3474,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M17">
+  <conditionalFormatting sqref="J3:J31 X29:X30">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2909,7 +3486,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB4:AB17">
+  <conditionalFormatting sqref="G3:G30">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2921,7 +3498,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:S18">
+  <conditionalFormatting sqref="D3:D27">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2933,7 +3510,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y8:Y18">
+  <conditionalFormatting sqref="AH3:AH35">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2945,7 +3522,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y8:Y19">
+  <conditionalFormatting sqref="AE3:AE28">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2957,7 +3534,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:S19">
+  <conditionalFormatting sqref="AB3:AB28">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2969,7 +3546,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M19">
+  <conditionalFormatting sqref="Y3:Y28">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2981,7 +3558,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M20">
+  <conditionalFormatting sqref="M3:M27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4401,8 +4978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Logistic regression fixes, and spreadsheet update.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="64">
   <si>
     <t>DEVEL</t>
   </si>
@@ -205,13 +205,16 @@
   </si>
   <si>
     <t>BP4D trained (static) logistic regression joint</t>
+  </si>
+  <si>
+    <t>BP4D MLP basic joint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +396,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -405,8 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -497,7 +500,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -532,7 +534,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -708,82 +709,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:37">
+      <c r="B1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="30" t="s">
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="30" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="30" t="s">
+      <c r="O1" s="30"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="30" t="s">
+      <c r="R1" s="30"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="28"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="30" t="s">
+      <c r="U1" s="30"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="30" t="s">
+      <c r="X1" s="30"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="30" t="s">
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="28" t="s">
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="28" t="s">
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="29"/>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="31"/>
+    </row>
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -896,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>0.26816666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>0.25200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1196,7 +1197,7 @@
         <v>0.23471428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="16.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1288,7 +1289,7 @@
         <v>0.3408571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1380,7 +1381,7 @@
         <v>0.21928571428571431</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>0.60526363636363623</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>0.59264545454545459</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1728,7 +1729,7 @@
         <v>0.59812727272727273</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>0.59751818181818195</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1912,7 +1913,7 @@
         <v>0.54469999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>0.23713333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>0.53643333333333332</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -2116,7 +2117,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" s="5" t="s">
         <v>45</v>
       </c>
@@ -2208,7 +2209,7 @@
         <v>0.56054285714285712</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" s="25" t="s">
         <v>46</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>0.54634285714285713</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37">
       <c r="A18" s="25" t="s">
         <v>52</v>
       </c>
@@ -2380,7 +2381,7 @@
         <v>0.74680000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37">
       <c r="A19" s="25" t="s">
         <v>53</v>
       </c>
@@ -2396,7 +2397,7 @@
       <c r="K19" s="7">
         <v>0.63329999999999997</v>
       </c>
-      <c r="L19" s="32">
+      <c r="L19" s="28">
         <v>0.92159999999999997</v>
       </c>
       <c r="M19" s="8">
@@ -2460,7 +2461,7 @@
         <v>0.71243999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37">
       <c r="A20" s="25" t="s">
         <v>60</v>
       </c>
@@ -2476,7 +2477,7 @@
       <c r="E20" s="7">
         <v>0.29289999999999999</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="28">
         <v>0.39040000000000002</v>
       </c>
       <c r="G20" s="8">
@@ -2494,7 +2495,7 @@
       <c r="K20" s="7">
         <v>0.72040000000000004</v>
       </c>
-      <c r="L20" s="32">
+      <c r="L20" s="28">
         <v>0.79179999999999995</v>
       </c>
       <c r="M20" s="8">
@@ -2576,7 +2577,7 @@
         <v>0.57558181818181819</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37">
       <c r="A21" s="25" t="s">
         <v>61</v>
       </c>
@@ -2592,7 +2593,7 @@
       <c r="E21" s="7">
         <v>0.3054</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="28">
         <v>0.42159999999999997</v>
       </c>
       <c r="G21" s="8">
@@ -2692,7 +2693,7 @@
         <v>0.58974545454545457</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37">
       <c r="A22" s="25" t="s">
         <v>62</v>
       </c>
@@ -2741,13 +2742,13 @@
       <c r="P22" s="8">
         <v>0.74029999999999996</v>
       </c>
-      <c r="Q22" s="33">
+      <c r="Q22" s="29">
         <v>0.80959999999999999</v>
       </c>
-      <c r="R22" s="33">
+      <c r="R22" s="29">
         <v>0.83950000000000002</v>
       </c>
-      <c r="S22" s="33">
+      <c r="S22" s="29">
         <v>0.82430000000000003</v>
       </c>
       <c r="T22" s="7">
@@ -2808,46 +2809,123 @@
         <v>0.58663636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="8"/>
-      <c r="AB23" s="8"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="8"/>
-      <c r="AE23" s="8"/>
-      <c r="AF23" s="7"/>
-      <c r="AG23" s="8"/>
-      <c r="AH23" s="9"/>
-      <c r="AI23" s="10"/>
-      <c r="AJ23" s="11"/>
-      <c r="AK23" s="12"/>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37">
+      <c r="A23" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="7">
+        <v>0.64290000000000003</v>
+      </c>
+      <c r="C23" s="8">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="I23" s="8">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="J23" s="9">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="K23" s="7">
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="L23" s="8">
+        <v>0.81289999999999996</v>
+      </c>
+      <c r="M23" s="8">
+        <v>0.79059999999999997</v>
+      </c>
+      <c r="N23" s="7">
+        <v>0.74490000000000001</v>
+      </c>
+      <c r="O23" s="8">
+        <v>0.69359999999999999</v>
+      </c>
+      <c r="P23" s="8">
+        <v>0.71830000000000005</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="R23" s="8">
+        <v>0.82650000000000001</v>
+      </c>
+      <c r="S23" s="8">
+        <v>0.83189999999999997</v>
+      </c>
+      <c r="T23" s="7">
+        <v>0.86119999999999997</v>
+      </c>
+      <c r="U23" s="8">
+        <v>0.85189999999999999</v>
+      </c>
+      <c r="V23" s="8">
+        <v>0.85650000000000004</v>
+      </c>
+      <c r="W23" s="7">
+        <v>0.54820000000000002</v>
+      </c>
+      <c r="X23" s="8">
+        <v>0.7268</v>
+      </c>
+      <c r="Y23" s="8">
+        <v>0.625</v>
+      </c>
+      <c r="Z23" s="7">
+        <v>0.60870000000000002</v>
+      </c>
+      <c r="AA23" s="8">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="AB23" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="AC23" s="7">
+        <v>0.68440000000000001</v>
+      </c>
+      <c r="AD23" s="8">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AE23" s="8">
+        <v>1.4E-3</v>
+      </c>
+      <c r="AF23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="10">
+        <f t="shared" ref="AI23" si="22">AVERAGE(B23,E23,H23,K23,N23,Q23,T23,W23,Z23,AC23,AF23)</f>
+        <v>0.57257272727272734</v>
+      </c>
+      <c r="AJ23" s="11">
+        <f t="shared" ref="AJ23" si="23">AVERAGE(C23,F23,I23,L23,O23,R23,U23,X23,AA23,AD23,AG23)</f>
+        <v>0.35589999999999999</v>
+      </c>
+      <c r="AK23" s="12">
+        <f t="shared" ref="AK23" si="24">AVERAGE(D23,G23,J23,M23,P23,S23,V23,Y23,AB23,AE23,AH23)</f>
+        <v>0.34805454545454545</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
       <c r="A24" s="1"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -2886,7 +2964,7 @@
       <c r="AJ24" s="11"/>
       <c r="AK24" s="12"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37">
       <c r="A25" s="1"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -2925,7 +3003,7 @@
       <c r="AJ25" s="11"/>
       <c r="AK25" s="12"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -2964,7 +3042,7 @@
       <c r="AJ26" s="11"/>
       <c r="AK26" s="12"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -3003,48 +3081,48 @@
       <c r="AJ27" s="11"/>
       <c r="AK27" s="12"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37">
       <c r="A28" s="1"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33"/>
-      <c r="V28" s="33"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="33"/>
-      <c r="Y28" s="33"/>
-      <c r="Z28" s="33"/>
-      <c r="AA28" s="33"/>
-      <c r="AB28" s="33"/>
-      <c r="AC28" s="33"/>
-      <c r="AD28" s="33"/>
-      <c r="AE28" s="33"/>
-      <c r="AF28" s="33"/>
-      <c r="AG28" s="33"/>
-      <c r="AH28" s="33"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
+      <c r="AA28" s="29"/>
+      <c r="AB28" s="29"/>
+      <c r="AC28" s="29"/>
+      <c r="AD28" s="29"/>
+      <c r="AE28" s="29"/>
+      <c r="AF28" s="29"/>
+      <c r="AG28" s="29"/>
+      <c r="AH28" s="29"/>
       <c r="AI28" s="10"/>
       <c r="AJ28" s="11"/>
       <c r="AK28" s="12"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37">
       <c r="A31" s="1"/>
     </row>
   </sheetData>
@@ -3065,9 +3143,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3077,9 +3155,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3089,9 +3167,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3101,9 +3179,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3113,9 +3191,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3125,9 +3203,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3137,9 +3215,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3149,9 +3227,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3161,9 +3239,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3173,9 +3251,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3185,9 +3263,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3197,9 +3275,9 @@
   <conditionalFormatting sqref="AK3:AK28">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3209,9 +3287,9 @@
   <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3221,9 +3299,9 @@
   <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3233,9 +3311,9 @@
   <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3245,9 +3323,9 @@
   <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3257,9 +3335,9 @@
   <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3269,9 +3347,9 @@
   <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3281,9 +3359,9 @@
   <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3293,9 +3371,9 @@
   <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3305,9 +3383,9 @@
   <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3317,9 +3395,9 @@
   <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3329,9 +3407,9 @@
   <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3341,9 +3419,9 @@
   <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3353,9 +3431,9 @@
   <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3365,9 +3443,9 @@
   <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="25">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3377,9 +3455,9 @@
   <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3389,9 +3467,9 @@
   <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3401,9 +3479,9 @@
   <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3413,9 +3491,9 @@
   <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3425,9 +3503,9 @@
   <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3437,9 +3515,9 @@
   <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3449,9 +3527,9 @@
   <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3461,9 +3539,9 @@
   <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3473,9 +3551,9 @@
   <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3485,9 +3563,9 @@
   <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3497,9 +3575,9 @@
   <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3509,9 +3587,9 @@
   <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3521,9 +3599,9 @@
   <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3533,9 +3611,9 @@
   <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3545,9 +3623,9 @@
   <conditionalFormatting sqref="P3:P27">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3557,9 +3635,9 @@
   <conditionalFormatting sqref="J3:J31 X29:X30">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3569,9 +3647,9 @@
   <conditionalFormatting sqref="G3:G30">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3581,9 +3659,9 @@
   <conditionalFormatting sqref="D3:D27">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3593,9 +3671,9 @@
   <conditionalFormatting sqref="AH3:AH35">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3605,9 +3683,9 @@
   <conditionalFormatting sqref="AE3:AE28">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3617,9 +3695,9 @@
   <conditionalFormatting sqref="AB3:AB28">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3629,9 +3707,9 @@
   <conditionalFormatting sqref="Y3:Y28">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3641,9 +3719,9 @@
   <conditionalFormatting sqref="M3:M27">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3653,9 +3731,9 @@
   <conditionalFormatting sqref="V3:V27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3668,14 +3746,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -3696,56 +3774,56 @@
     <col min="22" max="22" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:34">
+      <c r="B1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30" t="s">
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="30" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="30"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="30" t="s">
+      <c r="O1" s="30"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="30" t="s">
+      <c r="R1" s="30"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="28"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U1" s="30"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+    </row>
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3813,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>47</v>
       </c>
@@ -3872,7 +3950,7 @@
         <v>0.40849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -3931,7 +4009,7 @@
         <v>0.42475000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -3990,7 +4068,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -4049,7 +4127,7 @@
         <v>0.42574999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -4120,7 +4198,7 @@
         <v>0.30038333333333328</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -4191,7 +4269,7 @@
         <v>0.33351666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -4262,7 +4340,7 @@
         <v>0.28726666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -4333,7 +4411,7 @@
         <v>0.35348333333333332</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="5" t="s">
         <v>43</v>
       </c>
@@ -4386,7 +4464,7 @@
         <v>0.26429999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34">
       <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
@@ -4439,7 +4517,7 @@
         <v>0.30256666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
@@ -4492,7 +4570,7 @@
         <v>0.28043333333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
@@ -4545,7 +4623,7 @@
         <v>0.28770000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34">
       <c r="A15" s="5" t="s">
         <v>45</v>
       </c>
@@ -4604,7 +4682,7 @@
         <v>0.40457500000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34">
       <c r="A16" s="25" t="s">
         <v>46</v>
       </c>
@@ -4663,7 +4741,7 @@
         <v>0.44357500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="25" t="s">
         <v>50</v>
       </c>
@@ -4734,7 +4812,7 @@
         <v>0.24411666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" s="25" t="s">
         <v>51</v>
       </c>
@@ -4805,7 +4883,7 @@
         <v>0.29361666666666664</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" s="5" t="s">
         <v>33</v>
       </c>
@@ -4831,7 +4909,7 @@
       <c r="U19" s="8"/>
       <c r="V19" s="9"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -4857,36 +4935,36 @@
       <c r="U20" s="8"/>
       <c r="V20" s="9"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4896,9 +4974,9 @@
   <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4908,9 +4986,9 @@
   <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4920,9 +4998,9 @@
   <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4932,9 +5010,9 @@
   <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4944,9 +5022,9 @@
   <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4956,9 +5034,9 @@
   <conditionalFormatting sqref="V3:V20">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4968,9 +5046,9 @@
   <conditionalFormatting sqref="D3:D20">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4980,9 +5058,9 @@
   <conditionalFormatting sqref="G3:G20">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4992,9 +5070,9 @@
   <conditionalFormatting sqref="J3:J20">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5004,9 +5082,9 @@
   <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5016,9 +5094,9 @@
   <conditionalFormatting sqref="M3:M16">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5028,9 +5106,9 @@
   <conditionalFormatting sqref="M3:M18">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5040,9 +5118,9 @@
   <conditionalFormatting sqref="P7:P18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5052,9 +5130,9 @@
   <conditionalFormatting sqref="S7:S18">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5067,14 +5145,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -5091,33 +5169,33 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:13">
+      <c r="B1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="30" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="29"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
         <v>56</v>
       </c>
@@ -5155,7 +5233,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="25" t="s">
         <v>52</v>
       </c>
@@ -5198,7 +5276,7 @@
         <v>1.031925</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="25" t="s">
         <v>53</v>
       </c>
@@ -5241,7 +5319,7 @@
         <v>1.1512249999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="25" t="s">
         <v>58</v>
       </c>
@@ -5284,7 +5362,7 @@
         <v>1.06535</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="25" t="s">
         <v>59</v>
       </c>
@@ -5327,38 +5405,38 @@
         <v>1.1748499999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -5373,9 +5451,9 @@
   <conditionalFormatting sqref="M3:M6">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -5385,9 +5463,9 @@
   <conditionalFormatting sqref="L3:L6">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5397,9 +5475,9 @@
   <conditionalFormatting sqref="B3:B6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5409,9 +5487,9 @@
   <conditionalFormatting sqref="D3:D6">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5421,9 +5499,9 @@
   <conditionalFormatting sqref="F3:F6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5433,9 +5511,9 @@
   <conditionalFormatting sqref="H3:H7">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5445,9 +5523,9 @@
   <conditionalFormatting sqref="J3:J7">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5457,9 +5535,9 @@
   <conditionalFormatting sqref="C3:C6">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -5469,9 +5547,9 @@
   <conditionalFormatting sqref="E3:E6">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -5481,9 +5559,9 @@
   <conditionalFormatting sqref="G3:G7">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -5493,9 +5571,9 @@
   <conditionalFormatting sqref="I3:I6">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -5505,9 +5583,9 @@
   <conditionalFormatting sqref="K3:K6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>

<commit_message>
Corrections to SEMAINE label extraction.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="65">
   <si>
     <t>DEVEL</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>BP4D MLP basic joint</t>
+  </si>
+  <si>
+    <t>BP4D trained (static) logistic regression - eucl err.</t>
   </si>
 </sst>
 </file>
@@ -710,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK31"/>
+  <dimension ref="A1:AK35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AJ26" sqref="AJ26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2814,155 +2817,232 @@
         <v>63</v>
       </c>
       <c r="B23" s="7">
-        <v>0.64290000000000003</v>
+        <v>0.4204</v>
       </c>
       <c r="C23" s="8">
-        <v>6.9999999999999999E-4</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="D23" s="9">
-        <v>1.2999999999999999E-3</v>
+        <v>0.4093</v>
       </c>
       <c r="E23" s="7">
-        <v>0</v>
+        <v>0.33389999999999997</v>
       </c>
       <c r="F23" s="8">
-        <v>0</v>
+        <v>0.30630000000000002</v>
       </c>
       <c r="G23" s="9">
-        <v>0</v>
+        <v>0.31950000000000001</v>
       </c>
       <c r="H23" s="7">
-        <v>0.60099999999999998</v>
+        <v>0.4572</v>
       </c>
       <c r="I23" s="8">
-        <v>5.9999999999999995E-4</v>
+        <v>0.46439999999999998</v>
       </c>
       <c r="J23" s="9">
-        <v>1.1000000000000001E-3</v>
+        <v>0.46079999999999999</v>
       </c>
       <c r="K23" s="7">
-        <v>0.76949999999999996</v>
+        <v>0.72860000000000003</v>
       </c>
       <c r="L23" s="8">
-        <v>0.81289999999999996</v>
+        <v>0.75549999999999995</v>
       </c>
       <c r="M23" s="8">
-        <v>0.79059999999999997</v>
+        <v>0.74180000000000001</v>
       </c>
       <c r="N23" s="7">
-        <v>0.74490000000000001</v>
+        <v>0.70660000000000001</v>
       </c>
       <c r="O23" s="8">
-        <v>0.69359999999999999</v>
+        <v>0.77010000000000001</v>
       </c>
       <c r="P23" s="8">
-        <v>0.71830000000000005</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="Q23" s="7">
-        <v>0.83750000000000002</v>
+        <v>0.81059999999999999</v>
       </c>
       <c r="R23" s="8">
-        <v>0.82650000000000001</v>
+        <v>0.84889999999999999</v>
       </c>
       <c r="S23" s="8">
-        <v>0.83189999999999997</v>
+        <v>0.82930000000000004</v>
       </c>
       <c r="T23" s="7">
-        <v>0.86119999999999997</v>
+        <v>0.88119999999999998</v>
       </c>
       <c r="U23" s="8">
-        <v>0.85189999999999999</v>
+        <v>0.82110000000000005</v>
       </c>
       <c r="V23" s="8">
-        <v>0.85650000000000004</v>
+        <v>0.85009999999999997</v>
       </c>
       <c r="W23" s="7">
-        <v>0.54820000000000002</v>
+        <v>0.57440000000000002</v>
       </c>
       <c r="X23" s="8">
-        <v>0.7268</v>
+        <v>0.70730000000000004</v>
       </c>
       <c r="Y23" s="8">
-        <v>0.625</v>
+        <v>0.63390000000000002</v>
       </c>
       <c r="Z23" s="7">
-        <v>0.60870000000000002</v>
+        <v>0.40820000000000001</v>
       </c>
       <c r="AA23" s="8">
-        <v>1.1999999999999999E-3</v>
+        <v>0.56110000000000004</v>
       </c>
       <c r="AB23" s="8">
-        <v>2.5000000000000001E-3</v>
+        <v>0.47249999999999998</v>
       </c>
       <c r="AC23" s="7">
-        <v>0.68440000000000001</v>
+        <v>0.53839999999999999</v>
       </c>
       <c r="AD23" s="8">
-        <v>6.9999999999999999E-4</v>
+        <v>0.70109999999999995</v>
       </c>
       <c r="AE23" s="8">
-        <v>1.4E-3</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="AF23" s="7">
-        <v>0</v>
+        <v>0.50749999999999995</v>
       </c>
       <c r="AG23" s="8">
-        <v>0</v>
+        <v>0.36890000000000001</v>
       </c>
       <c r="AH23" s="9">
-        <v>0</v>
+        <v>0.42709999999999998</v>
       </c>
       <c r="AI23" s="10">
         <f t="shared" ref="AI23" si="22">AVERAGE(B23,E23,H23,K23,N23,Q23,T23,W23,Z23,AC23,AF23)</f>
-        <v>0.57257272727272734</v>
+        <v>0.57881818181818179</v>
       </c>
       <c r="AJ23" s="11">
         <f t="shared" ref="AJ23" si="23">AVERAGE(C23,F23,I23,L23,O23,R23,U23,X23,AA23,AD23,AG23)</f>
-        <v>0.35589999999999999</v>
+        <v>0.60942727272727271</v>
       </c>
       <c r="AK23" s="12">
         <f t="shared" ref="AK23" si="24">AVERAGE(D23,G23,J23,M23,P23,S23,V23,Y23,AB23,AE23,AH23)</f>
-        <v>0.34805454545454545</v>
+        <v>0.59002727272727273</v>
       </c>
     </row>
     <row r="24" spans="1:37">
-      <c r="A24" s="1"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="8"/>
-      <c r="AB24" s="8"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="8"/>
-      <c r="AE24" s="8"/>
-      <c r="AF24" s="7"/>
-      <c r="AG24" s="8"/>
-      <c r="AH24" s="9"/>
-      <c r="AI24" s="10"/>
-      <c r="AJ24" s="11"/>
-      <c r="AK24" s="12"/>
+      <c r="A24" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.3362</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0.46060000000000001</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0.38540000000000002</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.26229999999999998</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.42070000000000002</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0.32269999999999999</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.37659999999999999</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.59319999999999995</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0.46050000000000002</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0.63539999999999996</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0.91890000000000005</v>
+      </c>
+      <c r="M24" s="8">
+        <v>0.74909999999999999</v>
+      </c>
+      <c r="N24" s="7">
+        <v>0.66810000000000003</v>
+      </c>
+      <c r="O24" s="8">
+        <v>0.88460000000000005</v>
+      </c>
+      <c r="P24" s="8">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>0.74690000000000001</v>
+      </c>
+      <c r="R24" s="8">
+        <v>0.94610000000000005</v>
+      </c>
+      <c r="S24" s="8">
+        <v>0.83479999999999999</v>
+      </c>
+      <c r="T24" s="7">
+        <v>0.82720000000000005</v>
+      </c>
+      <c r="U24" s="8">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="V24" s="8">
+        <v>0.86839999999999995</v>
+      </c>
+      <c r="W24" s="7">
+        <v>0.47960000000000003</v>
+      </c>
+      <c r="X24" s="8">
+        <v>0.93279999999999996</v>
+      </c>
+      <c r="Y24" s="8">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="Z24" s="7">
+        <v>0.33729999999999999</v>
+      </c>
+      <c r="AA24" s="8">
+        <v>0.60670000000000002</v>
+      </c>
+      <c r="AB24" s="8">
+        <v>0.432</v>
+      </c>
+      <c r="AC24" s="7">
+        <v>0.51329999999999998</v>
+      </c>
+      <c r="AD24" s="8">
+        <v>0.78610000000000002</v>
+      </c>
+      <c r="AE24" s="8">
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="AF24" s="7">
+        <v>0.3775</v>
+      </c>
+      <c r="AG24" s="8">
+        <v>0.53339999999999999</v>
+      </c>
+      <c r="AH24" s="9">
+        <v>0.44190000000000002</v>
+      </c>
+      <c r="AI24" s="10">
+        <f t="shared" ref="AI24" si="25">AVERAGE(B24,E24,H24,K24,N24,Q24,T24,W24,Z24,AC24,AF24)</f>
+        <v>0.5054909090909091</v>
+      </c>
+      <c r="AJ24" s="11">
+        <f t="shared" ref="AJ24" si="26">AVERAGE(C24,F24,I24,L24,O24,R24,U24,X24,AA24,AD24,AG24)</f>
+        <v>0.7270181818181819</v>
+      </c>
+      <c r="AK24" s="12">
+        <f t="shared" ref="AK24" si="27">AVERAGE(D24,G24,J24,M24,P24,S24,V24,Y24,AB24,AE24,AH24)</f>
+        <v>0.5917</v>
+      </c>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="1"/>
@@ -3122,8 +3202,8 @@
     <row r="30" spans="1:37">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:37">
-      <c r="A31" s="1"/>
+    <row r="35" spans="5:5">
+      <c r="E35" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3668,7 +3748,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH35">
+  <conditionalFormatting sqref="AH34:AH35 AH3:AH31">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
New SEMAINE results with fully trained data.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -159,15 +160,6 @@
     <t>Combined train, dynamic</t>
   </si>
   <si>
-    <t>Psyche (trained on DISFA and using mult bins, neutral is extracted through a median)</t>
-  </si>
-  <si>
-    <t>DISFA training with generic PCA and new alignment, static model</t>
-  </si>
-  <si>
-    <t>DISFA training with generic PCA and new alignment, dynamic model</t>
-  </si>
-  <si>
     <t>SEMAINE trained RBF (static)</t>
   </si>
   <si>
@@ -211,6 +203,15 @@
   </si>
   <si>
     <t>BP4D trained (static) logistic regression - eucl err.</t>
+  </si>
+  <si>
+    <t>Psyche (trained on DISFA and using mult bins, neutral median)</t>
+  </si>
+  <si>
+    <t>DISFA train with gen PCA, new alignment, dynamic model</t>
+  </si>
+  <si>
+    <t>DISFA train with gen PCA and new alignment, static model</t>
   </si>
 </sst>
 </file>
@@ -713,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK35"/>
+  <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2306,7 +2307,7 @@
     </row>
     <row r="18" spans="1:37">
       <c r="A18" s="25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
@@ -2386,7 +2387,7 @@
     </row>
     <row r="19" spans="1:37">
       <c r="A19" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
@@ -2466,7 +2467,7 @@
     </row>
     <row r="20" spans="1:37">
       <c r="A20" s="25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" s="7">
         <v>0.3674</v>
@@ -2582,7 +2583,7 @@
     </row>
     <row r="21" spans="1:37">
       <c r="A21" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B21" s="7">
         <v>0.3196</v>
@@ -2698,7 +2699,7 @@
     </row>
     <row r="22" spans="1:37">
       <c r="A22" s="25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B22" s="7">
         <v>0.47939999999999999</v>
@@ -2814,123 +2815,123 @@
     </row>
     <row r="23" spans="1:37">
       <c r="A23" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B23" s="7">
-        <v>0.4204</v>
+        <v>0.37940000000000002</v>
       </c>
       <c r="C23" s="8">
-        <v>0.39900000000000002</v>
+        <v>0.44479999999999997</v>
       </c>
       <c r="D23" s="9">
         <v>0.4093</v>
       </c>
       <c r="E23" s="7">
-        <v>0.33389999999999997</v>
+        <v>0.31769999999999998</v>
       </c>
       <c r="F23" s="8">
-        <v>0.30630000000000002</v>
+        <v>0.34079999999999999</v>
       </c>
       <c r="G23" s="9">
-        <v>0.31950000000000001</v>
+        <v>0.32850000000000001</v>
       </c>
       <c r="H23" s="7">
-        <v>0.4572</v>
+        <v>0.43540000000000001</v>
       </c>
       <c r="I23" s="8">
-        <v>0.46439999999999998</v>
+        <v>0.52710000000000001</v>
       </c>
       <c r="J23" s="9">
-        <v>0.46079999999999999</v>
+        <v>0.47639999999999999</v>
       </c>
       <c r="K23" s="7">
-        <v>0.72860000000000003</v>
+        <v>0.70720000000000005</v>
       </c>
       <c r="L23" s="8">
-        <v>0.75549999999999995</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="M23" s="8">
-        <v>0.74180000000000001</v>
+        <v>0.74429999999999996</v>
       </c>
       <c r="N23" s="7">
-        <v>0.70660000000000001</v>
+        <v>0.70620000000000005</v>
       </c>
       <c r="O23" s="8">
-        <v>0.77010000000000001</v>
+        <v>0.85270000000000001</v>
       </c>
       <c r="P23" s="8">
-        <v>0.73699999999999999</v>
+        <v>0.77249999999999996</v>
       </c>
       <c r="Q23" s="7">
-        <v>0.81059999999999999</v>
+        <v>0.81420000000000003</v>
       </c>
       <c r="R23" s="8">
-        <v>0.84889999999999999</v>
+        <v>0.78380000000000005</v>
       </c>
       <c r="S23" s="8">
-        <v>0.82930000000000004</v>
+        <v>0.79869999999999997</v>
       </c>
       <c r="T23" s="7">
-        <v>0.88119999999999998</v>
+        <v>0.88990000000000002</v>
       </c>
       <c r="U23" s="8">
-        <v>0.82110000000000005</v>
+        <v>0.83830000000000005</v>
       </c>
       <c r="V23" s="8">
-        <v>0.85009999999999997</v>
+        <v>0.86329999999999996</v>
       </c>
       <c r="W23" s="7">
-        <v>0.57440000000000002</v>
+        <v>0.61280000000000001</v>
       </c>
       <c r="X23" s="8">
-        <v>0.70730000000000004</v>
+        <v>0.69069999999999998</v>
       </c>
       <c r="Y23" s="8">
-        <v>0.63390000000000002</v>
+        <v>0.64890000000000003</v>
       </c>
       <c r="Z23" s="7">
-        <v>0.40820000000000001</v>
+        <v>0.42949999999999999</v>
       </c>
       <c r="AA23" s="8">
-        <v>0.56110000000000004</v>
+        <v>0.53810000000000002</v>
       </c>
       <c r="AB23" s="8">
-        <v>0.47249999999999998</v>
+        <v>0.4773</v>
       </c>
       <c r="AC23" s="7">
-        <v>0.53839999999999999</v>
+        <v>0.51480000000000004</v>
       </c>
       <c r="AD23" s="8">
-        <v>0.70109999999999995</v>
+        <v>0.70030000000000003</v>
       </c>
       <c r="AE23" s="8">
-        <v>0.60899999999999999</v>
+        <v>0.59319999999999995</v>
       </c>
       <c r="AF23" s="7">
-        <v>0.50749999999999995</v>
+        <v>0.48249999999999998</v>
       </c>
       <c r="AG23" s="8">
-        <v>0.36890000000000001</v>
+        <v>0.4027</v>
       </c>
       <c r="AH23" s="9">
-        <v>0.42709999999999998</v>
+        <v>0.4385</v>
       </c>
       <c r="AI23" s="10">
         <f t="shared" ref="AI23" si="22">AVERAGE(B23,E23,H23,K23,N23,Q23,T23,W23,Z23,AC23,AF23)</f>
-        <v>0.57881818181818179</v>
+        <v>0.57178181818181817</v>
       </c>
       <c r="AJ23" s="11">
         <f t="shared" ref="AJ23" si="23">AVERAGE(C23,F23,I23,L23,O23,R23,U23,X23,AA23,AD23,AG23)</f>
-        <v>0.60942727272727271</v>
+        <v>0.62770000000000004</v>
       </c>
       <c r="AK23" s="12">
         <f t="shared" ref="AK23" si="24">AVERAGE(D23,G23,J23,M23,P23,S23,V23,Y23,AB23,AE23,AH23)</f>
-        <v>0.59002727272727273</v>
+        <v>0.59553636363636364</v>
       </c>
     </row>
     <row r="24" spans="1:37">
       <c r="A24" s="25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B24" s="7">
         <v>0.3362</v>
@@ -3202,8 +3203,8 @@
     <row r="30" spans="1:37">
       <c r="A30" s="1"/>
     </row>
-    <row r="35" spans="5:5">
-      <c r="E35" s="1"/>
+    <row r="34" spans="5:5">
+      <c r="E34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3748,7 +3749,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH34:AH35 AH3:AH31">
+  <conditionalFormatting sqref="AH3:AH31 AH35">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3829,13 +3830,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="58" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
     <col min="3" max="6" width="5.140625" customWidth="1"/>
     <col min="7" max="7" width="4.85546875" customWidth="1"/>
@@ -3973,7 +3974,7 @@
     </row>
     <row r="3" spans="1:34" ht="17.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B3" s="10">
         <v>0.46100000000000002</v>
@@ -4091,7 +4092,7 @@
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B5" s="10">
         <v>0.16</v>
@@ -4150,7 +4151,7 @@
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B6" s="10">
         <v>0.40400000000000003</v>
@@ -4212,70 +4213,70 @@
         <v>21</v>
       </c>
       <c r="B7" s="10">
-        <v>0.23719999999999999</v>
+        <v>0.19189999999999999</v>
       </c>
       <c r="C7" s="11">
-        <v>0.36880000000000002</v>
+        <v>0.31240000000000001</v>
       </c>
       <c r="D7" s="12">
-        <v>0.28870000000000001</v>
+        <v>0.23780000000000001</v>
       </c>
       <c r="E7" s="10">
-        <v>0.52629999999999999</v>
+        <v>0.51239999999999997</v>
       </c>
       <c r="F7" s="13">
-        <v>0.4753</v>
+        <v>0.49059999999999998</v>
       </c>
       <c r="G7" s="12">
-        <v>0.4995</v>
+        <v>0.50119999999999998</v>
       </c>
       <c r="H7" s="15">
-        <v>0.30249999999999999</v>
+        <v>0.30959999999999999</v>
       </c>
       <c r="I7" s="11">
-        <v>0.1711</v>
+        <v>0.16309999999999999</v>
       </c>
       <c r="J7" s="12">
-        <v>0.21859999999999999</v>
+        <v>0.21360000000000001</v>
       </c>
       <c r="K7" s="15">
-        <v>0.36120000000000002</v>
+        <v>0.3851</v>
       </c>
       <c r="L7" s="11">
-        <v>0.45269999999999999</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="M7" s="12">
-        <v>0.40179999999999999</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="N7" s="15">
-        <v>0.75680000000000003</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="O7" s="13">
         <v>2.6200000000000001E-2</v>
       </c>
       <c r="P7" s="16">
-        <v>5.0700000000000002E-2</v>
+        <v>5.0099999999999999E-2</v>
       </c>
       <c r="Q7" s="10">
-        <v>0.23649999999999999</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="R7" s="13">
-        <v>0.62429999999999997</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="S7" s="16">
-        <v>0.34300000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="0"/>
-        <v>0.40341666666666659</v>
+        <v>0.36566666666666664</v>
       </c>
       <c r="U7" s="8">
         <f t="shared" si="1"/>
-        <v>0.3530666666666667</v>
+        <v>0.33338333333333336</v>
       </c>
       <c r="V7" s="9">
         <f t="shared" si="2"/>
-        <v>0.30038333333333328</v>
+        <v>0.28861666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:34">
@@ -4283,70 +4284,70 @@
         <v>22</v>
       </c>
       <c r="B8" s="15">
-        <v>0.62619999999999998</v>
+        <v>0.63139999999999996</v>
       </c>
       <c r="C8" s="11">
-        <v>0.42080000000000001</v>
+        <v>0.3906</v>
       </c>
       <c r="D8" s="16">
-        <v>0.50329999999999997</v>
+        <v>0.48270000000000002</v>
       </c>
       <c r="E8" s="15">
-        <v>0.67179999999999995</v>
+        <v>0.66449999999999998</v>
       </c>
       <c r="F8" s="11">
-        <v>0.45319999999999999</v>
+        <v>0.45850000000000002</v>
       </c>
       <c r="G8" s="16">
-        <v>0.54120000000000001</v>
+        <v>0.54259999999999997</v>
       </c>
       <c r="H8" s="10">
-        <v>0.2737</v>
+        <v>0.5514</v>
       </c>
       <c r="I8" s="11">
-        <v>6.2199999999999998E-2</v>
+        <v>7.2599999999999998E-2</v>
       </c>
       <c r="J8" s="12">
-        <v>0.10100000000000001</v>
+        <v>0.1283</v>
       </c>
       <c r="K8" s="10">
-        <v>0.28420000000000001</v>
+        <v>0.37130000000000002</v>
       </c>
       <c r="L8" s="11">
-        <v>0.48730000000000001</v>
+        <v>0.28149999999999997</v>
       </c>
       <c r="M8" s="12">
-        <v>0.35899999999999999</v>
+        <v>0.32019999999999998</v>
       </c>
       <c r="N8" s="10">
-        <v>0.69089999999999996</v>
+        <v>0.63329999999999997</v>
       </c>
       <c r="O8" s="11">
         <v>3.56E-2</v>
       </c>
       <c r="P8" s="12">
-        <v>6.7699999999999996E-2</v>
+        <v>6.7400000000000002E-2</v>
       </c>
       <c r="Q8" s="10">
-        <v>0.35859999999999997</v>
+        <v>0.3402</v>
       </c>
       <c r="R8" s="11">
         <v>0.53359999999999996</v>
       </c>
       <c r="S8" s="12">
-        <v>0.4289</v>
+        <v>0.41549999999999998</v>
       </c>
       <c r="T8" s="7">
         <f t="shared" si="0"/>
-        <v>0.48423333333333335</v>
+        <v>0.53201666666666669</v>
       </c>
       <c r="U8" s="8">
         <f t="shared" si="1"/>
-        <v>0.33211666666666667</v>
+        <v>0.29539999999999994</v>
       </c>
       <c r="V8" s="9">
         <f t="shared" si="2"/>
-        <v>0.33351666666666668</v>
+        <v>0.32611666666666667</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -4354,70 +4355,70 @@
         <v>24</v>
       </c>
       <c r="B9" s="7">
-        <v>0.17879999999999999</v>
+        <v>0.186</v>
       </c>
       <c r="C9" s="8">
-        <v>0.53620000000000001</v>
+        <v>0.49459999999999998</v>
       </c>
       <c r="D9" s="9">
-        <v>0.2681</v>
+        <v>0.27039999999999997</v>
       </c>
       <c r="E9" s="7">
-        <v>0.65390000000000004</v>
+        <v>0.377</v>
       </c>
       <c r="F9" s="8">
-        <v>0.44230000000000003</v>
+        <v>0.79690000000000005</v>
       </c>
       <c r="G9" s="9">
-        <v>0.52769999999999995</v>
+        <v>0.51190000000000002</v>
       </c>
       <c r="H9" s="7">
-        <v>5.74E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="I9" s="8">
-        <v>0.55200000000000005</v>
+        <v>0.59940000000000004</v>
       </c>
       <c r="J9" s="9">
-        <v>0.10390000000000001</v>
+        <v>0.1535</v>
       </c>
       <c r="K9" s="7">
-        <v>0.28110000000000002</v>
+        <v>0.3054</v>
       </c>
       <c r="L9" s="8">
-        <v>0.70089999999999997</v>
+        <v>0.73519999999999996</v>
       </c>
       <c r="M9" s="9">
-        <v>0.40129999999999999</v>
+        <v>0.43159999999999998</v>
       </c>
       <c r="N9" s="7">
-        <v>5.7299999999999997E-2</v>
+        <v>5.8500000000000003E-2</v>
       </c>
       <c r="O9" s="8">
-        <v>0.72819999999999996</v>
+        <v>0.80130000000000001</v>
       </c>
       <c r="P9" s="9">
-        <v>0.10630000000000001</v>
+        <v>0.109</v>
       </c>
       <c r="Q9" s="7">
-        <v>0.19520000000000001</v>
+        <v>0.20580000000000001</v>
       </c>
       <c r="R9" s="8">
-        <v>0.83430000000000004</v>
+        <v>0.77839999999999998</v>
       </c>
       <c r="S9" s="9">
-        <v>0.31630000000000003</v>
+        <v>0.32550000000000001</v>
       </c>
       <c r="T9" s="7">
         <f t="shared" ref="T9:T10" si="3">AVERAGE(B9,E9,H9,K9,N9,Q9)</f>
-        <v>0.23728333333333332</v>
+        <v>0.20344999999999999</v>
       </c>
       <c r="U9" s="8">
         <f t="shared" ref="U9:U10" si="4">AVERAGE(C9,F9,I9,L9,O9,R9)</f>
-        <v>0.63231666666666664</v>
+        <v>0.70096666666666663</v>
       </c>
       <c r="V9" s="9">
         <f t="shared" ref="V9:V10" si="5">AVERAGE(D9,G9,J9,M9,P9,S9)</f>
-        <v>0.28726666666666667</v>
+        <v>0.30031666666666662</v>
       </c>
     </row>
     <row r="10" spans="1:34">
@@ -4425,70 +4426,70 @@
         <v>25</v>
       </c>
       <c r="B10" s="7">
-        <v>0.63719999999999999</v>
+        <v>0.64680000000000004</v>
       </c>
       <c r="C10" s="8">
-        <v>0.48530000000000001</v>
+        <v>0.46410000000000001</v>
       </c>
       <c r="D10" s="9">
-        <v>0.55100000000000005</v>
+        <v>0.54039999999999999</v>
       </c>
       <c r="E10" s="7">
-        <v>0.65390000000000004</v>
+        <v>0.66069999999999995</v>
       </c>
       <c r="F10" s="8">
-        <v>0.44230000000000003</v>
+        <v>0.44209999999999999</v>
       </c>
       <c r="G10" s="9">
-        <v>0.52769999999999995</v>
+        <v>0.52980000000000005</v>
       </c>
       <c r="H10" s="7">
-        <v>0.2051</v>
+        <v>0.3</v>
       </c>
       <c r="I10" s="8">
-        <v>0.104</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="J10" s="9">
-        <v>0.13800000000000001</v>
+        <v>0.14330000000000001</v>
       </c>
       <c r="K10" s="7">
-        <v>0.27329999999999999</v>
+        <v>0.28839999999999999</v>
       </c>
       <c r="L10" s="8">
-        <v>0.83299999999999996</v>
+        <v>0.40439999999999998</v>
       </c>
       <c r="M10" s="9">
-        <v>0.41160000000000002</v>
+        <v>0.3367</v>
       </c>
       <c r="N10" s="7">
         <v>1</v>
       </c>
       <c r="O10" s="8">
-        <v>3.56E-2</v>
+        <v>3.4700000000000002E-2</v>
       </c>
       <c r="P10" s="9">
-        <v>6.88E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="Q10" s="7">
-        <v>0.34899999999999998</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="R10" s="8">
-        <v>0.53939999999999999</v>
+        <v>0.53810000000000002</v>
       </c>
       <c r="S10" s="9">
-        <v>0.42380000000000001</v>
+        <v>0.41889999999999999</v>
       </c>
       <c r="T10" s="7">
         <f t="shared" si="3"/>
-        <v>0.51975000000000005</v>
+        <v>0.53981666666666672</v>
       </c>
       <c r="U10" s="8">
         <f t="shared" si="4"/>
-        <v>0.40660000000000002</v>
+        <v>0.32959999999999995</v>
       </c>
       <c r="V10" s="9">
         <f t="shared" si="5"/>
-        <v>0.35348333333333332</v>
+        <v>0.33934999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:34">
@@ -4496,13 +4497,13 @@
         <v>43</v>
       </c>
       <c r="B11" s="7">
-        <v>0.1303</v>
+        <v>0.13</v>
       </c>
       <c r="C11" s="8">
         <v>0.76329999999999998</v>
       </c>
       <c r="D11" s="9">
-        <v>0.22259999999999999</v>
+        <v>0.22220000000000001</v>
       </c>
       <c r="E11" s="7">
         <v>0.31159999999999999</v>
@@ -4533,7 +4534,7 @@
       <c r="S11" s="9"/>
       <c r="T11" s="7">
         <f>AVERAGE(B11,E11,H11,K11,N11,Q11)</f>
-        <v>0.1656</v>
+        <v>0.16550000000000001</v>
       </c>
       <c r="U11" s="8">
         <f>AVERAGE(C11,F11,I11,L11,O11,R11)</f>
@@ -4541,7 +4542,7 @@
       </c>
       <c r="V11" s="9">
         <f>AVERAGE(D11,G11,J11,M11,P11,S11)</f>
-        <v>0.26429999999999998</v>
+        <v>0.26416666666666666</v>
       </c>
     </row>
     <row r="12" spans="1:34">
@@ -4549,7 +4550,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="7">
-        <v>0.24199999999999999</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="C12" s="8">
         <v>0.4909</v>
@@ -4586,7 +4587,7 @@
       <c r="S12" s="9"/>
       <c r="T12" s="7">
         <f t="shared" ref="T12:T16" si="6">AVERAGE(B12,E12,H12,K12,N12,Q12)</f>
-        <v>0.20933333333333334</v>
+        <v>0.216</v>
       </c>
       <c r="U12" s="8">
         <f t="shared" ref="U12:U16" si="7">AVERAGE(C12,F12,I12,L12,O12,R12)</f>
@@ -4602,13 +4603,13 @@
         <v>41</v>
       </c>
       <c r="B13" s="7">
-        <v>0.16300000000000001</v>
+        <v>0.16259999999999999</v>
       </c>
       <c r="C13" s="8">
         <v>0.74350000000000005</v>
       </c>
       <c r="D13" s="9">
-        <v>0.26740000000000003</v>
+        <v>0.26679999999999998</v>
       </c>
       <c r="E13" s="7">
         <v>0.31790000000000002</v>
@@ -4639,7 +4640,7 @@
       <c r="S13" s="9"/>
       <c r="T13" s="7">
         <f>AVERAGE(B13,E13,H13,K13,N13,Q13)</f>
-        <v>0.17836666666666667</v>
+        <v>0.17823333333333335</v>
       </c>
       <c r="U13" s="8">
         <f>AVERAGE(C13,F13,I13,L13,O13,R13)</f>
@@ -4647,7 +4648,7 @@
       </c>
       <c r="V13" s="9">
         <f>AVERAGE(D13,G13,J13,M13,P13,S13)</f>
-        <v>0.28043333333333337</v>
+        <v>0.28023333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:34">
@@ -4823,7 +4824,7 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B17" s="7">
         <v>0.14680000000000001</v>
@@ -4894,7 +4895,7 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" s="7">
         <v>0.54559999999999997</v>
@@ -5027,17 +5028,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="15">
@@ -5277,45 +5278,45 @@
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="7">
         <v>0.76639999999999997</v>
@@ -5358,7 +5359,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="7">
         <v>0.74750000000000005</v>
@@ -5401,7 +5402,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="7">
         <v>0.73160000000000003</v>
@@ -5444,7 +5445,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" s="7">
         <v>0.71699999999999997</v>
@@ -5487,12 +5488,12 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:13">

</xml_diff>

<commit_message>
New results on SEMAINE using logistic regression
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
   <si>
     <t>DEVEL</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>DISFA train with gen PCA and new alignment, static model</t>
+  </si>
+  <si>
+    <t>BP4D MLP basic separate</t>
   </si>
 </sst>
 </file>
@@ -714,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK34"/>
+  <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ25" sqref="AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3046,43 +3049,120 @@
       </c>
     </row>
     <row r="25" spans="1:37">
-      <c r="A25" s="1"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="7"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="7"/>
-      <c r="AA25" s="8"/>
-      <c r="AB25" s="8"/>
-      <c r="AC25" s="7"/>
-      <c r="AD25" s="8"/>
-      <c r="AE25" s="8"/>
-      <c r="AF25" s="7"/>
-      <c r="AG25" s="8"/>
-      <c r="AH25" s="9"/>
-      <c r="AI25" s="10"/>
-      <c r="AJ25" s="11"/>
-      <c r="AK25" s="12"/>
+      <c r="A25" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.36730000000000002</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.50519999999999998</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.42530000000000001</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.33879999999999999</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.39229999999999998</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0.36349999999999999</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0.37080000000000002</v>
+      </c>
+      <c r="I25" s="8">
+        <v>0.52869999999999995</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0.433</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0.72119999999999995</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.84409999999999996</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="N25" s="7">
+        <v>0.66910000000000003</v>
+      </c>
+      <c r="O25" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="P25" s="8">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>0.79479999999999995</v>
+      </c>
+      <c r="R25" s="8">
+        <v>0.93210000000000004</v>
+      </c>
+      <c r="S25" s="8">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="T25" s="7">
+        <v>0.84540000000000004</v>
+      </c>
+      <c r="U25" s="8">
+        <v>0.90610000000000002</v>
+      </c>
+      <c r="V25" s="8">
+        <v>0.87470000000000003</v>
+      </c>
+      <c r="W25" s="7">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="X25" s="8">
+        <v>0.86939999999999995</v>
+      </c>
+      <c r="Y25" s="8">
+        <v>0.64829999999999999</v>
+      </c>
+      <c r="Z25" s="7">
+        <v>0.3654</v>
+      </c>
+      <c r="AA25" s="8">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="AB25" s="8">
+        <v>0.46879999999999999</v>
+      </c>
+      <c r="AC25" s="7">
+        <v>0.51049999999999995</v>
+      </c>
+      <c r="AD25" s="8">
+        <v>0.81740000000000002</v>
+      </c>
+      <c r="AE25" s="8">
+        <v>0.62849999999999995</v>
+      </c>
+      <c r="AF25" s="7">
+        <v>0.43359999999999999</v>
+      </c>
+      <c r="AG25" s="8">
+        <v>0.55769999999999997</v>
+      </c>
+      <c r="AH25" s="9">
+        <v>0.48670000000000002</v>
+      </c>
+      <c r="AI25" s="10">
+        <f t="shared" ref="AI25" si="28">AVERAGE(B25,E25,H25,K25,N25,Q25,T25,W25,Z25,AC25,AF25)</f>
+        <v>0.53944545454545467</v>
+      </c>
+      <c r="AJ25" s="11">
+        <f t="shared" ref="AJ25" si="29">AVERAGE(C25,F25,I25,L25,O25,R25,U25,X25,AA25,AD25,AG25)</f>
+        <v>0.71972727272727266</v>
+      </c>
+      <c r="AK25" s="12">
+        <f t="shared" ref="AK25" si="30">AVERAGE(D25,G25,J25,M25,P25,S25,V25,Y25,AB25,AE25,AH25)</f>
+        <v>0.61232727272727272</v>
+      </c>
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="1"/>
@@ -3203,9 +3283,6 @@
     <row r="30" spans="1:37">
       <c r="A30" s="1"/>
     </row>
-    <row r="34" spans="5:5">
-      <c r="E34" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="AI1:AK1"/>
@@ -3222,6 +3299,18 @@
     <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3233,7 +3322,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G9">
+  <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3245,7 +3334,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3257,7 +3346,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M9">
+  <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3269,7 +3358,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P9">
+  <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3281,7 +3370,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S9">
+  <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3293,7 +3382,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V9">
+  <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3305,7 +3394,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y9">
+  <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3317,7 +3406,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB9">
+  <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3329,7 +3418,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE9">
+  <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3341,7 +3430,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH9">
+  <conditionalFormatting sqref="AK3:AK28">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3353,7 +3442,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK3:AK28">
+  <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3365,7 +3454,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D17">
+  <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3377,7 +3466,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G11">
+  <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3389,7 +3478,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J11">
+  <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3401,7 +3490,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M11">
+  <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3413,7 +3502,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P11">
+  <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3425,7 +3514,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S11">
+  <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3437,7 +3526,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V11">
+  <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3449,7 +3538,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y11">
+  <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3461,7 +3550,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB11">
+  <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3473,7 +3562,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE11">
+  <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3485,7 +3574,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH11">
+  <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3497,7 +3586,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G21">
+  <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3509,7 +3598,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V21">
+  <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3521,7 +3610,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE19 AE21">
+  <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3533,7 +3622,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J17">
+  <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3545,7 +3634,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M17">
+  <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3557,7 +3646,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB4:AB17">
+  <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3569,7 +3658,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:S18">
+  <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3581,7 +3670,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y8:Y18">
+  <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3593,7 +3682,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y8:Y19">
+  <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3605,7 +3694,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:S19">
+  <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3617,7 +3706,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M19">
+  <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3629,7 +3718,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M20">
+  <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3641,7 +3730,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH8:AH20">
+  <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3653,7 +3742,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE21">
+  <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3665,7 +3754,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB20">
+  <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3677,7 +3766,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y8:Y20">
+  <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3689,7 +3778,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S24">
+  <conditionalFormatting sqref="P3:P27">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3701,7 +3790,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P27">
+  <conditionalFormatting sqref="J3:J31 X29:X30">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3713,7 +3802,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J31 X29:X30">
+  <conditionalFormatting sqref="G3:G30">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3725,7 +3814,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G30">
+  <conditionalFormatting sqref="D3:D27">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3737,7 +3826,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D27">
+  <conditionalFormatting sqref="AH3:AH31 AH35">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3749,7 +3838,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH31 AH35">
+  <conditionalFormatting sqref="AE3:AE28">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3761,7 +3850,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE28">
+  <conditionalFormatting sqref="AB3:AB28">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3773,7 +3862,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB28">
+  <conditionalFormatting sqref="Y3:Y28">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3785,7 +3874,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y28">
+  <conditionalFormatting sqref="M3:M27">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3797,7 +3886,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M27">
+  <conditionalFormatting sqref="V3:V27">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3809,7 +3898,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V27">
+  <conditionalFormatting sqref="S3:S25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3830,8 +3919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
New results that need to be entered.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="67">
   <si>
     <t>DEVEL</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>SEMAINE MLP dynamic (scale)</t>
+  </si>
+  <si>
+    <t>SEMAINE MLP static with geom</t>
   </si>
 </sst>
 </file>
@@ -3916,10 +3919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH22"/>
+  <dimension ref="A1:AH23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5334,6 +5337,11 @@
       <c r="V22" s="9">
         <f t="shared" ref="V22" si="20">AVERAGE(D22,G22,J22,M22,P22,S22)</f>
         <v>0.22173333333333334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lost of changes: - Shuffling the data before training (duh!) - AU prediction in C++ work
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8010" activeTab="1"/>
@@ -11,7 +11,7 @@
     <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -237,8 +237,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,7 +524,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -559,7 +558,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -735,20 +733,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="B1" s="32" t="s">
         <v>2</v>
       </c>
@@ -810,7 +808,7 @@
       <c r="AJ1" s="30"/>
       <c r="AK1" s="31"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -923,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
@@ -1039,7 +1037,7 @@
         <v>0.26816666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>0.25200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1223,7 +1221,7 @@
         <v>0.23471428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="16.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1315,7 +1313,7 @@
         <v>0.3408571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1407,7 +1405,7 @@
         <v>0.21928571428571431</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1523,7 +1521,7 @@
         <v>0.60526363636363623</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1639,7 +1637,7 @@
         <v>0.59264545454545459</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1755,7 +1753,7 @@
         <v>0.59812727272727273</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -1871,7 +1869,7 @@
         <v>0.59751818181818195</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
@@ -1939,7 +1937,7 @@
         <v>0.54469999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -2007,7 +2005,7 @@
         <v>0.23713333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
@@ -2075,7 +2073,7 @@
         <v>0.53643333333333332</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -2143,7 +2141,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
@@ -2235,7 +2233,7 @@
         <v>0.56054285714285712</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" s="25" t="s">
         <v>44</v>
       </c>
@@ -2327,7 +2325,7 @@
         <v>0.54634285714285713</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37">
       <c r="A18" s="25" t="s">
         <v>47</v>
       </c>
@@ -2407,7 +2405,7 @@
         <v>0.74680000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37">
       <c r="A19" s="25" t="s">
         <v>48</v>
       </c>
@@ -2487,7 +2485,7 @@
         <v>0.71243999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37">
       <c r="A20" s="25" t="s">
         <v>55</v>
       </c>
@@ -2603,7 +2601,7 @@
         <v>0.57558181818181819</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37">
       <c r="A21" s="25" t="s">
         <v>56</v>
       </c>
@@ -2719,7 +2717,7 @@
         <v>0.58974545454545457</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37">
       <c r="A22" s="25" t="s">
         <v>57</v>
       </c>
@@ -2835,7 +2833,7 @@
         <v>0.58663636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37">
       <c r="A23" s="25" t="s">
         <v>58</v>
       </c>
@@ -2951,7 +2949,7 @@
         <v>0.58991818181818179</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37">
       <c r="A24" s="25" t="s">
         <v>59</v>
       </c>
@@ -3067,7 +3065,7 @@
         <v>0.5917</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37">
       <c r="A25" s="25" t="s">
         <v>63</v>
       </c>
@@ -3183,7 +3181,7 @@
         <v>0.61232727272727272</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37">
       <c r="A26" s="25" t="s">
         <v>71</v>
       </c>
@@ -3287,19 +3285,19 @@
         <v>0.49120000000000003</v>
       </c>
       <c r="AI26" s="10">
-        <f t="shared" ref="AI26:AI27" si="28">AVERAGE(B26,E26,H26,K26,N26,Q26,T26,W26,Z26,AC26,AF26)</f>
+        <f t="shared" ref="AI26" si="28">AVERAGE(B26,E26,H26,K26,N26,Q26,T26,W26,Z26,AC26,AF26)</f>
         <v>0.56283636363636369</v>
       </c>
       <c r="AJ26" s="11">
-        <f t="shared" ref="AJ26:AJ27" si="29">AVERAGE(C26,F26,I26,L26,O26,R26,U26,X26,AA26,AD26,AG26)</f>
+        <f t="shared" ref="AJ26" si="29">AVERAGE(C26,F26,I26,L26,O26,R26,U26,X26,AA26,AD26,AG26)</f>
         <v>0.62217272727272721</v>
       </c>
       <c r="AK26" s="12">
-        <f t="shared" ref="AK26:AK27" si="30">AVERAGE(D26,G26,J26,M26,P26,S26,V26,Y26,AB26,AE26,AH26)</f>
+        <f t="shared" ref="AK26" si="30">AVERAGE(D26,G26,J26,M26,P26,S26,V26,Y26,AB26,AE26,AH26)</f>
         <v>0.58963636363636374</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37">
       <c r="A27" s="25" t="s">
         <v>70</v>
       </c>
@@ -3340,7 +3338,7 @@
       <c r="AJ27" s="11"/>
       <c r="AK27" s="12"/>
     </row>
-    <row r="28" spans="1:37" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="23.25">
       <c r="A28" s="25" t="s">
         <v>69</v>
       </c>
@@ -3381,10 +3379,10 @@
       <c r="AJ28" s="11"/>
       <c r="AK28" s="12"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37">
       <c r="A30" s="1"/>
     </row>
   </sheetData>
@@ -3405,9 +3403,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="76">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3417,9 +3415,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="75">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3429,9 +3427,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="74">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3441,9 +3439,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="73">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3453,9 +3451,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="72">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3465,9 +3463,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="71">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3477,9 +3475,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="70">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3489,9 +3487,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="69">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3501,9 +3499,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="68">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3513,9 +3511,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="67">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3525,9 +3523,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="66">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3537,9 +3535,9 @@
   <conditionalFormatting sqref="AK3:AK28">
     <cfRule type="colorScale" priority="65">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3549,9 +3547,9 @@
   <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="64">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3561,9 +3559,9 @@
   <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3573,9 +3571,9 @@
   <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3585,9 +3583,9 @@
   <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3597,9 +3595,9 @@
   <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3609,9 +3607,9 @@
   <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3621,9 +3619,9 @@
   <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3633,9 +3631,9 @@
   <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3645,9 +3643,9 @@
   <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3657,9 +3655,9 @@
   <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3669,9 +3667,9 @@
   <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3681,9 +3679,9 @@
   <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3693,9 +3691,9 @@
   <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3705,9 +3703,9 @@
   <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3717,9 +3715,9 @@
   <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3729,9 +3727,9 @@
   <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3741,9 +3739,9 @@
   <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3753,9 +3751,9 @@
   <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3765,9 +3763,9 @@
   <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3777,9 +3775,9 @@
   <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3789,9 +3787,9 @@
   <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3801,9 +3799,9 @@
   <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3813,9 +3811,9 @@
   <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3825,9 +3823,9 @@
   <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3837,9 +3835,9 @@
   <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3849,9 +3847,9 @@
   <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3861,9 +3859,9 @@
   <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3873,9 +3871,9 @@
   <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3885,9 +3883,9 @@
   <conditionalFormatting sqref="P3:P25 P27:P28">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3897,9 +3895,9 @@
   <conditionalFormatting sqref="J3:J25 X29:X30 J27:J31">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3909,9 +3907,9 @@
   <conditionalFormatting sqref="G3:G25 G27:G30">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3921,9 +3919,9 @@
   <conditionalFormatting sqref="D3:D25 D27:D28">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3933,9 +3931,9 @@
   <conditionalFormatting sqref="AH3:AH25 AH27:AH31">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3945,9 +3943,9 @@
   <conditionalFormatting sqref="AE3:AE25 AE27:AE28">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3957,9 +3955,9 @@
   <conditionalFormatting sqref="AB3:AB25 AB27:AB28">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3969,9 +3967,9 @@
   <conditionalFormatting sqref="Y3:Y25 Y27:Y28">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3981,9 +3979,9 @@
   <conditionalFormatting sqref="M3:M25 M27:M28">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -3993,9 +3991,9 @@
   <conditionalFormatting sqref="V3:V25 V27:V28">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4005,9 +4003,9 @@
   <conditionalFormatting sqref="S3:S25">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4017,9 +4015,9 @@
   <conditionalFormatting sqref="S26">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4029,9 +4027,9 @@
   <conditionalFormatting sqref="P26">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4041,9 +4039,9 @@
   <conditionalFormatting sqref="J26">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4053,9 +4051,9 @@
   <conditionalFormatting sqref="G26">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4065,9 +4063,9 @@
   <conditionalFormatting sqref="D26">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4077,9 +4075,9 @@
   <conditionalFormatting sqref="AH26">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4089,9 +4087,9 @@
   <conditionalFormatting sqref="AE26">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4101,9 +4099,9 @@
   <conditionalFormatting sqref="AB26">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4113,9 +4111,9 @@
   <conditionalFormatting sqref="Y26">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4125,9 +4123,9 @@
   <conditionalFormatting sqref="M26">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4137,9 +4135,9 @@
   <conditionalFormatting sqref="V26">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4149,9 +4147,9 @@
   <conditionalFormatting sqref="S26">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4161,9 +4159,9 @@
   <conditionalFormatting sqref="AH3:AH28">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4173,9 +4171,9 @@
   <conditionalFormatting sqref="AE3:AE28">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4185,9 +4183,9 @@
   <conditionalFormatting sqref="AB3:AB28">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4197,9 +4195,9 @@
   <conditionalFormatting sqref="AB3:AB26">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4209,9 +4207,9 @@
   <conditionalFormatting sqref="Y3:Y26">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4221,9 +4219,9 @@
   <conditionalFormatting sqref="V3:V26">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4233,9 +4231,9 @@
   <conditionalFormatting sqref="S3:S26">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4245,9 +4243,9 @@
   <conditionalFormatting sqref="P3:P26">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4257,9 +4255,9 @@
   <conditionalFormatting sqref="M3:M26">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4269,9 +4267,9 @@
   <conditionalFormatting sqref="J3:J26">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4281,9 +4279,9 @@
   <conditionalFormatting sqref="G3:G26">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4293,9 +4291,9 @@
   <conditionalFormatting sqref="D3:D26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4308,14 +4306,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -4336,7 +4334,7 @@
     <col min="22" max="22" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="B1" s="32" t="s">
         <v>3</v>
       </c>
@@ -4385,7 +4383,7 @@
       <c r="AG1" s="33"/>
       <c r="AH1" s="33"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4453,7 +4451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>60</v>
       </c>
@@ -4512,7 +4510,7 @@
         <v>0.40849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -4571,7 +4569,7 @@
         <v>0.42475000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>62</v>
       </c>
@@ -4630,7 +4628,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>61</v>
       </c>
@@ -4689,7 +4687,7 @@
         <v>0.42574999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -4760,7 +4758,7 @@
         <v>0.28861666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -4831,7 +4829,7 @@
         <v>0.32611666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -4902,7 +4900,7 @@
         <v>0.30031666666666662</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -4973,7 +4971,7 @@
         <v>0.33934999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
@@ -5026,7 +5024,7 @@
         <v>0.26416666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34">
       <c r="A12" s="5" t="s">
         <v>42</v>
       </c>
@@ -5079,7 +5077,7 @@
         <v>0.30256666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34">
       <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
@@ -5132,7 +5130,7 @@
         <v>0.28023333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -5185,7 +5183,7 @@
         <v>0.28770000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34">
       <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
@@ -5244,7 +5242,7 @@
         <v>0.40457500000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34">
       <c r="A16" s="25" t="s">
         <v>44</v>
       </c>
@@ -5303,7 +5301,7 @@
         <v>0.44357500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="A17" s="25" t="s">
         <v>45</v>
       </c>
@@ -5374,7 +5372,7 @@
         <v>0.24411666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="A18" s="25" t="s">
         <v>46</v>
       </c>
@@ -5445,7 +5443,7 @@
         <v>0.29361666666666664</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="A19" s="5" t="s">
         <v>33</v>
       </c>
@@ -5516,7 +5514,7 @@
         <v>0.24851666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -5593,7 +5591,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25">
       <c r="A21" s="5" t="s">
         <v>64</v>
       </c>
@@ -5664,7 +5662,7 @@
         <v>0.26086666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25">
       <c r="A22" s="5" t="s">
         <v>65</v>
       </c>
@@ -5735,7 +5733,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
@@ -5806,7 +5804,7 @@
         <v>0.26210000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="A24" s="5" t="s">
         <v>67</v>
       </c>
@@ -5820,61 +5818,61 @@
         <v>0.46400000000000002</v>
       </c>
       <c r="E24" s="7">
-        <v>0.46829999999999999</v>
+        <v>0.69469999999999998</v>
       </c>
       <c r="F24" s="8">
-        <v>0.44340000000000002</v>
+        <v>0.29820000000000002</v>
       </c>
       <c r="G24" s="9">
-        <v>0.45550000000000002</v>
+        <v>0.4173</v>
       </c>
       <c r="H24" s="7">
-        <v>0.40870000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I24" s="8">
-        <v>9.7799999999999998E-2</v>
+        <v>6.7999999999999996E-3</v>
       </c>
       <c r="J24" s="9">
-        <v>0.15790000000000001</v>
+        <v>1.34E-2</v>
       </c>
       <c r="K24" s="7">
-        <v>0.37919999999999998</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="L24" s="8">
-        <v>0.33879999999999999</v>
+        <v>0.2397</v>
       </c>
       <c r="M24" s="9">
-        <v>0.3579</v>
+        <v>0.31590000000000001</v>
       </c>
       <c r="N24" s="7">
-        <v>0.29070000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="O24" s="8">
-        <v>2.3400000000000001E-2</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="P24" s="9">
-        <v>4.3400000000000001E-2</v>
+        <v>1.9E-3</v>
       </c>
       <c r="Q24" s="7">
-        <v>0.2203</v>
+        <v>0.27039999999999997</v>
       </c>
       <c r="R24" s="8">
-        <v>0.47260000000000002</v>
+        <v>0.62009999999999998</v>
       </c>
       <c r="S24" s="9">
-        <v>0.30049999999999999</v>
+        <v>0.37659999999999999</v>
       </c>
       <c r="T24" s="7">
         <f t="shared" ref="T24" si="24">AVERAGE(B24,E24,H24,K24,N24,Q24)</f>
-        <v>0.3601833333333333</v>
+        <v>0.47866666666666663</v>
       </c>
       <c r="U24" s="8">
         <f t="shared" ref="U24" si="25">AVERAGE(C24,F24,I24,L24,O24,R24)</f>
-        <v>0.32339999999999997</v>
+        <v>0.28834999999999994</v>
       </c>
       <c r="V24" s="9">
         <f t="shared" ref="V24" si="26">AVERAGE(D24,G24,J24,M24,P24,S24)</f>
-        <v>0.29653333333333332</v>
+        <v>0.26484999999999997</v>
       </c>
       <c r="W24">
         <v>250</v>
@@ -5888,24 +5886,24 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5915,9 +5913,9 @@
   <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5927,9 +5925,9 @@
   <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5939,9 +5937,9 @@
   <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5951,9 +5949,9 @@
   <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5963,9 +5961,9 @@
   <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5975,9 +5973,9 @@
   <conditionalFormatting sqref="V3:V24">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5987,9 +5985,9 @@
   <conditionalFormatting sqref="D3:D24">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5999,9 +5997,9 @@
   <conditionalFormatting sqref="G3:G24">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6011,9 +6009,9 @@
   <conditionalFormatting sqref="J3:J24">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6023,9 +6021,9 @@
   <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6035,9 +6033,9 @@
   <conditionalFormatting sqref="M3:M16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6047,9 +6045,9 @@
   <conditionalFormatting sqref="M3:M18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6059,9 +6057,9 @@
   <conditionalFormatting sqref="P7:P18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6071,9 +6069,9 @@
   <conditionalFormatting sqref="S7:S18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6083,9 +6081,9 @@
   <conditionalFormatting sqref="M4:M21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6095,9 +6093,9 @@
   <conditionalFormatting sqref="P4:P21">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6107,9 +6105,9 @@
   <conditionalFormatting sqref="S4:S21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6119,9 +6117,9 @@
   <conditionalFormatting sqref="M3:M24">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6131,9 +6129,9 @@
   <conditionalFormatting sqref="P3:P24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6143,9 +6141,9 @@
   <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6158,14 +6156,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -6182,7 +6180,7 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="B1" s="32" t="s">
         <v>5</v>
       </c>
@@ -6208,7 +6206,7 @@
       </c>
       <c r="M1" s="31"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
         <v>51</v>
       </c>
@@ -6246,7 +6244,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="25" t="s">
         <v>47</v>
       </c>
@@ -6289,7 +6287,7 @@
         <v>1.031925</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="25" t="s">
         <v>48</v>
       </c>
@@ -6332,7 +6330,7 @@
         <v>1.1512249999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="25" t="s">
         <v>53</v>
       </c>
@@ -6375,7 +6373,7 @@
         <v>1.06535</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="25" t="s">
         <v>54</v>
       </c>
@@ -6418,38 +6416,38 @@
         <v>1.1748499999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -6464,9 +6462,9 @@
   <conditionalFormatting sqref="M3:M6">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -6476,9 +6474,9 @@
   <conditionalFormatting sqref="L3:L6">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6488,9 +6486,9 @@
   <conditionalFormatting sqref="B3:B6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6500,9 +6498,9 @@
   <conditionalFormatting sqref="D3:D6">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6512,9 +6510,9 @@
   <conditionalFormatting sqref="F3:F6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6524,9 +6522,9 @@
   <conditionalFormatting sqref="H3:H7">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6536,9 +6534,9 @@
   <conditionalFormatting sqref="J3:J7">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6548,9 +6546,9 @@
   <conditionalFormatting sqref="C3:C6">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -6560,9 +6558,9 @@
   <conditionalFormatting sqref="E3:E6">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -6572,9 +6570,9 @@
   <conditionalFormatting sqref="G3:G7">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -6584,9 +6582,9 @@
   <conditionalFormatting sqref="I3:I6">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -6596,9 +6594,9 @@
   <conditionalFormatting sqref="K3:K6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>

<commit_message>
Geometry results with SEMAINE.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13920" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="71">
   <si>
     <t>DEVEL</t>
   </si>
@@ -72,9 +72,6 @@
     <t>AU25</t>
   </si>
   <si>
-    <t>AU28</t>
-  </si>
-  <si>
     <t>AU45</t>
   </si>
   <si>
@@ -225,13 +222,13 @@
     <t>still climbing after 1000epochs at 100 hiddent and 0.0001</t>
   </si>
   <si>
-    <t>BP4D MLP basic joint scale (working on caelum 104)</t>
-  </si>
-  <si>
-    <t>BP4D MLP geometry</t>
-  </si>
-  <si>
     <t>BP4D MLP scale</t>
+  </si>
+  <si>
+    <t>AU28 *might need sep model</t>
+  </si>
+  <si>
+    <t>BP4D MLP dynamic</t>
   </si>
 </sst>
 </file>
@@ -736,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AK27" sqref="AK27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -803,7 +800,7 @@
       <c r="AG1" s="30"/>
       <c r="AH1" s="31"/>
       <c r="AI1" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AJ1" s="30"/>
       <c r="AK1" s="31"/>
@@ -923,7 +920,7 @@
     </row>
     <row r="3" spans="1:37">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="10">
         <v>0.48799999999999999</v>
@@ -1131,7 +1128,7 @@
     </row>
     <row r="5" spans="1:37">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="10">
         <v>0.39</v>
@@ -1223,7 +1220,7 @@
     </row>
     <row r="6" spans="1:37" ht="16.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="10">
         <v>0.52600000000000002</v>
@@ -1315,7 +1312,7 @@
     </row>
     <row r="7" spans="1:37">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="15">
         <v>0.59199999999999997</v>
@@ -1407,7 +1404,7 @@
     </row>
     <row r="8" spans="1:37">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="10">
         <v>0.3589</v>
@@ -1523,7 +1520,7 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="10">
         <v>0.39240000000000003</v>
@@ -1639,7 +1636,7 @@
     </row>
     <row r="10" spans="1:37">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="7">
         <v>0.3664</v>
@@ -1755,7 +1752,7 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="7">
         <v>0.39410000000000001</v>
@@ -1871,7 +1868,7 @@
     </row>
     <row r="12" spans="1:37">
       <c r="A12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -1939,7 +1936,7 @@
     </row>
     <row r="13" spans="1:37">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -2007,7 +2004,7 @@
     </row>
     <row r="14" spans="1:37">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -2075,7 +2072,7 @@
     </row>
     <row r="15" spans="1:37">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
@@ -2143,7 +2140,7 @@
     </row>
     <row r="16" spans="1:37">
       <c r="A16" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="7">
         <v>0.34510000000000002</v>
@@ -2235,7 +2232,7 @@
     </row>
     <row r="17" spans="1:37">
       <c r="A17" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="7">
         <v>0.49569999999999997</v>
@@ -2327,7 +2324,7 @@
     </row>
     <row r="18" spans="1:37">
       <c r="A18" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
@@ -2407,7 +2404,7 @@
     </row>
     <row r="19" spans="1:37">
       <c r="A19" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
@@ -2487,7 +2484,7 @@
     </row>
     <row r="20" spans="1:37">
       <c r="A20" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="7">
         <v>0.3674</v>
@@ -2603,7 +2600,7 @@
     </row>
     <row r="21" spans="1:37">
       <c r="A21" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="7">
         <v>0.3196</v>
@@ -2719,7 +2716,7 @@
     </row>
     <row r="22" spans="1:37">
       <c r="A22" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="7">
         <v>0.47939999999999999</v>
@@ -2835,123 +2832,123 @@
     </row>
     <row r="23" spans="1:37">
       <c r="A23" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="7">
-        <v>0.31380000000000002</v>
+        <v>0.38929999999999998</v>
       </c>
       <c r="C23" s="8">
-        <v>0.42530000000000001</v>
+        <v>0.44629999999999997</v>
       </c>
       <c r="D23" s="9">
-        <v>0.36120000000000002</v>
+        <v>0.41589999999999999</v>
       </c>
       <c r="E23" s="7">
-        <v>0.28789999999999999</v>
+        <v>0.3347</v>
       </c>
       <c r="F23" s="8">
-        <v>0.33300000000000002</v>
+        <v>0.31719999999999998</v>
       </c>
       <c r="G23" s="9">
-        <v>0.30880000000000002</v>
+        <v>0.32569999999999999</v>
       </c>
       <c r="H23" s="7">
-        <v>0.52610000000000001</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="I23" s="8">
-        <v>0.4577</v>
+        <v>0.49480000000000002</v>
       </c>
       <c r="J23" s="9">
-        <v>0.48949999999999999</v>
+        <v>0.45660000000000001</v>
       </c>
       <c r="K23" s="7">
-        <v>0.7288</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="L23" s="8">
-        <v>0.76980000000000004</v>
+        <v>0.80589999999999995</v>
       </c>
       <c r="M23" s="8">
-        <v>0.74870000000000003</v>
+        <v>0.74639999999999995</v>
       </c>
       <c r="N23" s="7">
-        <v>0.71550000000000002</v>
+        <v>0.71740000000000004</v>
       </c>
       <c r="O23" s="8">
-        <v>0.82830000000000004</v>
+        <v>0.82540000000000002</v>
       </c>
       <c r="P23" s="8">
-        <v>0.76780000000000004</v>
+        <v>0.76759999999999995</v>
       </c>
       <c r="Q23" s="7">
-        <v>0.79600000000000004</v>
+        <v>0.8034</v>
       </c>
       <c r="R23" s="8">
-        <v>0.8518</v>
+        <v>0.81189999999999996</v>
       </c>
       <c r="S23" s="8">
-        <v>0.82299999999999995</v>
+        <v>0.80759999999999998</v>
       </c>
       <c r="T23" s="7">
-        <v>0.87680000000000002</v>
+        <v>0.87109999999999999</v>
       </c>
       <c r="U23" s="8">
-        <v>0.82</v>
+        <v>0.84719999999999995</v>
       </c>
       <c r="V23" s="8">
-        <v>0.84740000000000004</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="W23" s="7">
-        <v>0.61119999999999997</v>
+        <v>0.59589999999999999</v>
       </c>
       <c r="X23" s="8">
-        <v>0.74150000000000005</v>
+        <v>0.70479999999999998</v>
       </c>
       <c r="Y23" s="8">
-        <v>0.67010000000000003</v>
+        <v>0.64580000000000004</v>
       </c>
       <c r="Z23" s="7">
-        <v>0.38890000000000002</v>
+        <v>0.4158</v>
       </c>
       <c r="AA23" s="8">
-        <v>0.55300000000000005</v>
+        <v>0.5343</v>
       </c>
       <c r="AB23" s="8">
-        <v>0.45669999999999999</v>
+        <v>0.4677</v>
       </c>
       <c r="AC23" s="7">
-        <v>0.53500000000000003</v>
+        <v>0.51249999999999996</v>
       </c>
       <c r="AD23" s="8">
-        <v>0.68520000000000003</v>
+        <v>0.69010000000000005</v>
       </c>
       <c r="AE23" s="8">
-        <v>0.6008</v>
+        <v>0.58819999999999995</v>
       </c>
       <c r="AF23" s="7">
-        <v>0.56769999999999998</v>
+        <v>0.52749999999999997</v>
       </c>
       <c r="AG23" s="8">
-        <v>0.3271</v>
+        <v>0.44230000000000003</v>
       </c>
       <c r="AH23" s="9">
-        <v>0.41510000000000002</v>
+        <v>0.48110000000000003</v>
       </c>
       <c r="AI23" s="10">
         <f t="shared" ref="AI23" si="22">AVERAGE(B23,E23,H23,K23,N23,Q23,T23,W23,Z23,AC23,AF23)</f>
-        <v>0.57706363636363645</v>
+        <v>0.57150909090909086</v>
       </c>
       <c r="AJ23" s="11">
         <f t="shared" ref="AJ23" si="23">AVERAGE(C23,F23,I23,L23,O23,R23,U23,X23,AA23,AD23,AG23)</f>
-        <v>0.61751818181818185</v>
+        <v>0.62910909090909095</v>
       </c>
       <c r="AK23" s="12">
         <f t="shared" ref="AK23" si="24">AVERAGE(D23,G23,J23,M23,P23,S23,V23,Y23,AB23,AE23,AH23)</f>
-        <v>0.58991818181818179</v>
+        <v>0.59650909090909088</v>
       </c>
     </row>
     <row r="24" spans="1:37">
       <c r="A24" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="7">
         <v>0.3362</v>
@@ -3067,7 +3064,7 @@
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="7">
         <v>0.36730000000000002</v>
@@ -3183,7 +3180,7 @@
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B26" s="7">
         <v>0.3624</v>
@@ -3301,47 +3298,120 @@
       <c r="A27" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="8"/>
-      <c r="AB27" s="8"/>
-      <c r="AC27" s="7"/>
-      <c r="AD27" s="8"/>
-      <c r="AE27" s="8"/>
-      <c r="AF27" s="7"/>
-      <c r="AG27" s="8"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="10"/>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="12"/>
-    </row>
-    <row r="28" spans="1:37" ht="23.25">
-      <c r="A28" s="25" t="s">
-        <v>69</v>
-      </c>
+      <c r="B27" s="7">
+        <v>0.4219</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.44350000000000001</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.4325</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.38229999999999997</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.2429</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0.29709999999999998</v>
+      </c>
+      <c r="H27" s="7">
+        <v>0.4874</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0.4864</v>
+      </c>
+      <c r="K27" s="7">
+        <v>0.76559999999999995</v>
+      </c>
+      <c r="L27" s="8">
+        <v>0.75790000000000002</v>
+      </c>
+      <c r="M27" s="8">
+        <v>0.76170000000000004</v>
+      </c>
+      <c r="N27" s="7">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="O27" s="8">
+        <v>0.71279999999999999</v>
+      </c>
+      <c r="P27" s="8">
+        <v>0.71970000000000001</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>0.76559999999999995</v>
+      </c>
+      <c r="R27" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="S27" s="8">
+        <v>0.80559999999999998</v>
+      </c>
+      <c r="T27" s="7">
+        <v>0.82969999999999999</v>
+      </c>
+      <c r="U27" s="8">
+        <v>0.86339999999999995</v>
+      </c>
+      <c r="V27" s="8">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="W27" s="7">
+        <v>0.54079999999999995</v>
+      </c>
+      <c r="X27" s="8">
+        <v>0.69750000000000001</v>
+      </c>
+      <c r="Y27" s="8">
+        <v>0.60919999999999996</v>
+      </c>
+      <c r="Z27" s="7">
+        <v>0.3735</v>
+      </c>
+      <c r="AA27" s="8">
+        <v>0.34770000000000001</v>
+      </c>
+      <c r="AB27" s="8">
+        <v>0.36009999999999998</v>
+      </c>
+      <c r="AC27" s="7">
+        <v>0.59770000000000001</v>
+      </c>
+      <c r="AD27" s="8">
+        <v>0.47849999999999998</v>
+      </c>
+      <c r="AE27" s="8">
+        <v>0.53149999999999997</v>
+      </c>
+      <c r="AF27" s="7">
+        <v>0.4733</v>
+      </c>
+      <c r="AG27" s="8">
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="AH27" s="9">
+        <v>0.3412</v>
+      </c>
+      <c r="AI27" s="10">
+        <f t="shared" ref="AI27" si="31">AVERAGE(B27,E27,H27,K27,N27,Q27,T27,W27,Z27,AC27,AF27)</f>
+        <v>0.57859090909090904</v>
+      </c>
+      <c r="AJ27" s="11">
+        <f t="shared" ref="AJ27" si="32">AVERAGE(C27,F27,I27,L27,O27,R27,U27,X27,AA27,AD27,AG27)</f>
+        <v>0.55876363636363635</v>
+      </c>
+      <c r="AK27" s="12">
+        <f t="shared" ref="AK27" si="33">AVERAGE(D27,G27,J27,M27,P27,S27,V27,Y27,AB27,AE27,AH27)</f>
+        <v>0.56283636363636358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="A28" s="25"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
@@ -3892,7 +3962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J25 X29:X30 J27:J31">
+  <conditionalFormatting sqref="J3:J25 X29:X30 J27:J30">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3928,7 +3998,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH25 AH27:AH31">
+  <conditionalFormatting sqref="AH3:AH25 AH27:AH30">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4012,7 +4082,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S26">
+  <conditionalFormatting sqref="S26:S27">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4024,7 +4094,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P26">
+  <conditionalFormatting sqref="P26:P27">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4036,7 +4106,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J26">
+  <conditionalFormatting sqref="J26:J27">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4048,7 +4118,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
+  <conditionalFormatting sqref="G26:G27">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4060,7 +4130,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
+  <conditionalFormatting sqref="D26:D27">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4072,7 +4142,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH26">
+  <conditionalFormatting sqref="AH26:AH27">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4084,7 +4154,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE26">
+  <conditionalFormatting sqref="AE26:AE27">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4096,7 +4166,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB26">
+  <conditionalFormatting sqref="AB26:AB27">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4108,7 +4178,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y26">
+  <conditionalFormatting sqref="Y26:Y27">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4120,7 +4190,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
+  <conditionalFormatting sqref="M26:M27">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4132,20 +4202,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V26">
+  <conditionalFormatting sqref="V26:V27">
     <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S26">
-    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -4192,7 +4250,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB26">
+  <conditionalFormatting sqref="AB3:AB27">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4204,7 +4262,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y26">
+  <conditionalFormatting sqref="Y3:Y27">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4216,7 +4274,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V26">
+  <conditionalFormatting sqref="V3:V27">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4228,7 +4286,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S26">
+  <conditionalFormatting sqref="S3:S27">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4240,7 +4298,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P26">
+  <conditionalFormatting sqref="P3:P27">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4252,7 +4310,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M26">
+  <conditionalFormatting sqref="M3:M27">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4264,7 +4322,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J26">
+  <conditionalFormatting sqref="J3:J27">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4276,7 +4334,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G26">
+  <conditionalFormatting sqref="G3:G27">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4288,7 +4346,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D26">
+  <conditionalFormatting sqref="D3:D27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4309,8 +4367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4356,17 +4414,17 @@
       <c r="L1" s="30"/>
       <c r="M1" s="31"/>
       <c r="N1" s="32" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="O1" s="30"/>
       <c r="P1" s="31"/>
       <c r="Q1" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R1" s="30"/>
       <c r="S1" s="31"/>
       <c r="T1" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U1" s="30"/>
       <c r="V1" s="31"/>
@@ -4453,7 +4511,7 @@
     </row>
     <row r="3" spans="1:34" ht="17.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="10">
         <v>0.46100000000000002</v>
@@ -4571,7 +4629,7 @@
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="10">
         <v>0.16</v>
@@ -4630,7 +4688,7 @@
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="10">
         <v>0.40400000000000003</v>
@@ -4689,7 +4747,7 @@
     </row>
     <row r="7" spans="1:34">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="10">
         <v>0.19189999999999999</v>
@@ -4760,7 +4818,7 @@
     </row>
     <row r="8" spans="1:34">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="15">
         <v>0.63139999999999996</v>
@@ -4831,7 +4889,7 @@
     </row>
     <row r="9" spans="1:34">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7">
         <v>0.186</v>
@@ -4902,7 +4960,7 @@
     </row>
     <row r="10" spans="1:34">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7">
         <v>0.64680000000000004</v>
@@ -4973,7 +5031,7 @@
     </row>
     <row r="11" spans="1:34">
       <c r="A11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="7">
         <v>0.13</v>
@@ -5026,7 +5084,7 @@
     </row>
     <row r="12" spans="1:34">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="7">
         <v>0.26200000000000001</v>
@@ -5079,7 +5137,7 @@
     </row>
     <row r="13" spans="1:34">
       <c r="A13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="7">
         <v>0.16259999999999999</v>
@@ -5132,7 +5190,7 @@
     </row>
     <row r="14" spans="1:34">
       <c r="A14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="7">
         <v>0.19009999999999999</v>
@@ -5185,7 +5243,7 @@
     </row>
     <row r="15" spans="1:34">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="7">
         <v>0.28349999999999997</v>
@@ -5244,7 +5302,7 @@
     </row>
     <row r="16" spans="1:34">
       <c r="A16" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="7">
         <v>0.58560000000000001</v>
@@ -5303,7 +5361,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="7">
         <v>0.14680000000000001</v>
@@ -5374,7 +5432,7 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="7">
         <v>0.54559999999999997</v>
@@ -5445,78 +5503,78 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="7">
-        <v>0.1305</v>
+        <v>0.16</v>
       </c>
       <c r="C19" s="8">
-        <v>0.2883</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="D19" s="9">
-        <v>0.1797</v>
+        <v>0.19719999999999999</v>
       </c>
       <c r="E19" s="7">
-        <v>0.34860000000000002</v>
+        <v>0.49940000000000001</v>
       </c>
       <c r="F19" s="8">
-        <v>0.49959999999999999</v>
+        <v>0.43319999999999997</v>
       </c>
       <c r="G19" s="9">
-        <v>0.41060000000000002</v>
+        <v>0.46379999999999999</v>
       </c>
       <c r="H19" s="7">
-        <v>0.4249</v>
+        <v>0.23280000000000001</v>
       </c>
       <c r="I19" s="8">
-        <v>7.1400000000000005E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="J19" s="9">
-        <v>0.1222</v>
+        <v>3.3399999999999999E-2</v>
       </c>
       <c r="K19" s="7">
-        <v>0.312</v>
+        <v>0.32740000000000002</v>
       </c>
       <c r="L19" s="8">
-        <v>0.26100000000000001</v>
+        <v>0.24610000000000001</v>
       </c>
       <c r="M19" s="9">
-        <v>0.28420000000000001</v>
+        <v>0.28089999999999998</v>
       </c>
       <c r="N19" s="7">
-        <v>0.4022</v>
+        <v>0</v>
       </c>
       <c r="O19" s="8">
-        <v>0.1368</v>
+        <v>0</v>
       </c>
       <c r="P19" s="9">
-        <v>0.20419999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="7">
-        <v>0.2122</v>
+        <v>0.21940000000000001</v>
       </c>
       <c r="R19" s="8">
-        <v>0.45929999999999999</v>
+        <v>0.41170000000000001</v>
       </c>
       <c r="S19" s="9">
-        <v>0.29020000000000001</v>
+        <v>0.2863</v>
       </c>
       <c r="T19" s="7">
         <f t="shared" ref="T19" si="12">AVERAGE(B19,E19,H19,K19,N19,Q19)</f>
-        <v>0.30506666666666665</v>
+        <v>0.23983333333333334</v>
       </c>
       <c r="U19" s="8">
         <f t="shared" ref="U19" si="13">AVERAGE(C19,F19,I19,L19,O19,R19)</f>
-        <v>0.28606666666666669</v>
+        <v>0.22768333333333332</v>
       </c>
       <c r="V19" s="9">
         <f t="shared" ref="V19" si="14">AVERAGE(D19,G19,J19,M19,P19,S19)</f>
-        <v>0.24851666666666669</v>
+        <v>0.21026666666666669</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="7">
         <v>0.33329999999999999</v>
@@ -5593,7 +5651,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="7">
         <v>0.26500000000000001</v>
@@ -5664,7 +5722,7 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="7">
         <v>0.4204</v>
@@ -5735,7 +5793,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="7">
         <v>0.1726</v>
@@ -5806,7 +5864,7 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="7">
         <v>0.39389999999999997</v>
@@ -5881,22 +5939,22 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="Y24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
@@ -6202,51 +6260,51 @@
       </c>
       <c r="K1" s="31"/>
       <c r="L1" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="D2" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="H2" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="J2" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="L2" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="7">
         <v>0.76639999999999997</v>
@@ -6289,7 +6347,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7">
         <v>0.74750000000000005</v>
@@ -6332,7 +6390,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="7">
         <v>0.73160000000000003</v>
@@ -6375,7 +6433,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="7">
         <v>0.71699999999999997</v>
@@ -6418,12 +6476,12 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:13">

</xml_diff>

<commit_message>
Updated results, and attempts at running BP4D AU predictions.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="74">
   <si>
     <t>DEVEL</t>
   </si>
@@ -219,9 +219,6 @@
     <t>SEMAINE MLP dynamic with geom</t>
   </si>
   <si>
-    <t>still climbing after 1000epochs at 100 hiddent and 0.0001</t>
-  </si>
-  <si>
     <t>BP4D MLP scale</t>
   </si>
   <si>
@@ -229,6 +226,18 @@
   </si>
   <si>
     <t>BP4D MLP dynamic</t>
+  </si>
+  <si>
+    <t>MLP</t>
+  </si>
+  <si>
+    <t>BP4D MLP static geom</t>
+  </si>
+  <si>
+    <t>Combined train MLP</t>
+  </si>
+  <si>
+    <t>SEMAINE MLP combined</t>
   </si>
 </sst>
 </file>
@@ -733,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK27" sqref="AK27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3180,7 +3189,7 @@
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="7">
         <v>0.3624</v>
@@ -3296,164 +3305,357 @@
     </row>
     <row r="27" spans="1:37">
       <c r="A27" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="7">
-        <v>0.4219</v>
+        <v>0.3306</v>
       </c>
       <c r="C27" s="8">
-        <v>0.44350000000000001</v>
+        <v>0.56730000000000003</v>
       </c>
       <c r="D27" s="9">
-        <v>0.4325</v>
+        <v>0.4178</v>
       </c>
       <c r="E27" s="7">
-        <v>0.38229999999999997</v>
+        <v>0.32579999999999998</v>
       </c>
       <c r="F27" s="8">
-        <v>0.2429</v>
+        <v>0.37809999999999999</v>
       </c>
       <c r="G27" s="9">
-        <v>0.29709999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="H27" s="7">
-        <v>0.4874</v>
+        <v>0.55820000000000003</v>
       </c>
       <c r="I27" s="8">
-        <v>0.48549999999999999</v>
+        <v>0.41360000000000002</v>
       </c>
       <c r="J27" s="9">
-        <v>0.4864</v>
+        <v>0.47520000000000001</v>
       </c>
       <c r="K27" s="7">
-        <v>0.76559999999999995</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="L27" s="8">
-        <v>0.75790000000000002</v>
+        <v>0.72019999999999995</v>
       </c>
       <c r="M27" s="8">
-        <v>0.76170000000000004</v>
+        <v>0.78269999999999995</v>
       </c>
       <c r="N27" s="7">
-        <v>0.72670000000000001</v>
+        <v>0.77869999999999995</v>
       </c>
       <c r="O27" s="8">
-        <v>0.71279999999999999</v>
+        <v>0.66559999999999997</v>
       </c>
       <c r="P27" s="8">
-        <v>0.71970000000000001</v>
+        <v>0.7177</v>
       </c>
       <c r="Q27" s="7">
-        <v>0.76559999999999995</v>
+        <v>0.83609999999999995</v>
       </c>
       <c r="R27" s="8">
-        <v>0.85</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="S27" s="8">
-        <v>0.80559999999999998</v>
+        <v>0.81869999999999998</v>
       </c>
       <c r="T27" s="7">
-        <v>0.82969999999999999</v>
+        <v>0.88880000000000003</v>
       </c>
       <c r="U27" s="8">
-        <v>0.86339999999999995</v>
+        <v>0.79349999999999998</v>
       </c>
       <c r="V27" s="8">
-        <v>0.84619999999999995</v>
+        <v>0.83840000000000003</v>
       </c>
       <c r="W27" s="7">
-        <v>0.54079999999999995</v>
+        <v>0.48880000000000001</v>
       </c>
       <c r="X27" s="8">
-        <v>0.69750000000000001</v>
+        <v>0.9103</v>
       </c>
       <c r="Y27" s="8">
-        <v>0.60919999999999996</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="Z27" s="7">
-        <v>0.3735</v>
+        <v>0.4778</v>
       </c>
       <c r="AA27" s="8">
-        <v>0.34770000000000001</v>
+        <v>0.29870000000000002</v>
       </c>
       <c r="AB27" s="8">
-        <v>0.36009999999999998</v>
+        <v>0.36759999999999998</v>
       </c>
       <c r="AC27" s="7">
-        <v>0.59770000000000001</v>
+        <v>0.54169999999999996</v>
       </c>
       <c r="AD27" s="8">
-        <v>0.47849999999999998</v>
+        <v>0.7208</v>
       </c>
       <c r="AE27" s="8">
-        <v>0.53149999999999997</v>
+        <v>0.61850000000000005</v>
       </c>
       <c r="AF27" s="7">
-        <v>0.4733</v>
+        <v>0.51280000000000003</v>
       </c>
       <c r="AG27" s="8">
-        <v>0.26669999999999999</v>
+        <v>0.26</v>
       </c>
       <c r="AH27" s="9">
-        <v>0.3412</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="AI27" s="10">
         <f t="shared" ref="AI27" si="31">AVERAGE(B27,E27,H27,K27,N27,Q27,T27,W27,Z27,AC27,AF27)</f>
-        <v>0.57859090909090904</v>
+        <v>0.5996636363636364</v>
       </c>
       <c r="AJ27" s="11">
         <f t="shared" ref="AJ27" si="32">AVERAGE(C27,F27,I27,L27,O27,R27,U27,X27,AA27,AD27,AG27)</f>
-        <v>0.55876363636363635</v>
+        <v>0.59364545454545459</v>
       </c>
       <c r="AK27" s="12">
         <f t="shared" ref="AK27" si="33">AVERAGE(D27,G27,J27,M27,P27,S27,V27,Y27,AB27,AE27,AH27)</f>
-        <v>0.56283636363636358</v>
+        <v>0.57887272727272732</v>
       </c>
     </row>
     <row r="28" spans="1:37">
-      <c r="A28" s="25"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="7"/>
-      <c r="AA28" s="8"/>
-      <c r="AB28" s="8"/>
-      <c r="AC28" s="7"/>
-      <c r="AD28" s="8"/>
-      <c r="AE28" s="8"/>
-      <c r="AF28" s="7"/>
-      <c r="AG28" s="8"/>
-      <c r="AH28" s="9"/>
-      <c r="AI28" s="10"/>
-      <c r="AJ28" s="11"/>
-      <c r="AK28" s="12"/>
+      <c r="A28" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.41089999999999999</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.45540000000000003</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.43180000000000002</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0.37359999999999999</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.35570000000000002</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0.36430000000000001</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0.37340000000000001</v>
+      </c>
+      <c r="I28" s="8">
+        <v>0.52390000000000003</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0.43590000000000001</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0.71120000000000005</v>
+      </c>
+      <c r="L28" s="8">
+        <v>0.81179999999999997</v>
+      </c>
+      <c r="M28" s="8">
+        <v>0.7581</v>
+      </c>
+      <c r="N28" s="7">
+        <v>0.71950000000000003</v>
+      </c>
+      <c r="O28" s="8">
+        <v>0.82479999999999998</v>
+      </c>
+      <c r="P28" s="8">
+        <v>0.76849999999999996</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>0.82150000000000001</v>
+      </c>
+      <c r="R28" s="8">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="S28" s="8">
+        <v>0.81969999999999998</v>
+      </c>
+      <c r="T28" s="7">
+        <v>0.88290000000000002</v>
+      </c>
+      <c r="U28" s="8">
+        <v>0.85660000000000003</v>
+      </c>
+      <c r="V28" s="8">
+        <v>0.86960000000000004</v>
+      </c>
+      <c r="W28" s="7">
+        <v>0.59589999999999999</v>
+      </c>
+      <c r="X28" s="8">
+        <v>0.67610000000000003</v>
+      </c>
+      <c r="Y28" s="8">
+        <v>0.63339999999999996</v>
+      </c>
+      <c r="Z28" s="7">
+        <v>0.46750000000000003</v>
+      </c>
+      <c r="AA28" s="8">
+        <v>0.50619999999999998</v>
+      </c>
+      <c r="AB28" s="8">
+        <v>0.4859</v>
+      </c>
+      <c r="AC28" s="7">
+        <v>0.51990000000000003</v>
+      </c>
+      <c r="AD28" s="8">
+        <v>0.68789999999999996</v>
+      </c>
+      <c r="AE28" s="8">
+        <v>0.59219999999999995</v>
+      </c>
+      <c r="AF28" s="7">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="AG28" s="8">
+        <v>0.47589999999999999</v>
+      </c>
+      <c r="AH28" s="9">
+        <v>0.46510000000000001</v>
+      </c>
+      <c r="AI28" s="10">
+        <f t="shared" ref="AI28:AI30" si="34">AVERAGE(B28,E28,H28,K28,N28,Q28,T28,W28,Z28,AC28,AF28)</f>
+        <v>0.57566363636363649</v>
+      </c>
+      <c r="AJ28" s="11">
+        <f t="shared" ref="AJ28:AJ30" si="35">AVERAGE(C28,F28,I28,L28,O28,R28,U28,X28,AA28,AD28,AG28)</f>
+        <v>0.63566363636363632</v>
+      </c>
+      <c r="AK28" s="12">
+        <f t="shared" ref="AK28:AK30" si="36">AVERAGE(D28,G28,J28,M28,P28,S28,V28,Y28,AB28,AE28,AH28)</f>
+        <v>0.60222727272727272</v>
+      </c>
     </row>
     <row r="29" spans="1:37">
-      <c r="A29" s="1"/>
+      <c r="A29" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="7">
+        <v>0.40329999999999999</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.4178</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.41039999999999999</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.33279999999999998</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.39710000000000001</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0.36209999999999998</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0.46460000000000001</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0.4748</v>
+      </c>
+      <c r="K29" s="7">
+        <v>0.73819999999999997</v>
+      </c>
+      <c r="L29" s="8">
+        <v>0.80759999999999998</v>
+      </c>
+      <c r="M29" s="8">
+        <v>0.77139999999999997</v>
+      </c>
+      <c r="N29" s="7"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="7">
+        <v>0.87339999999999995</v>
+      </c>
+      <c r="U29" s="8">
+        <v>0.82869999999999999</v>
+      </c>
+      <c r="V29" s="8">
+        <v>0.85040000000000004</v>
+      </c>
+      <c r="W29" s="7"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+      <c r="Z29" s="7">
+        <v>0.60160000000000002</v>
+      </c>
+      <c r="AA29" s="8">
+        <v>0.45629999999999998</v>
+      </c>
+      <c r="AB29" s="8">
+        <v>0.51890000000000003</v>
+      </c>
+      <c r="AC29" s="7">
+        <v>0.51290000000000002</v>
+      </c>
+      <c r="AD29" s="8">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="AE29" s="8">
+        <v>0.59160000000000001</v>
+      </c>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="8"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="10"/>
+      <c r="AJ29" s="11"/>
+      <c r="AK29" s="12"/>
     </row>
     <row r="30" spans="1:37">
       <c r="A30" s="1"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="8"/>
+      <c r="AB30" s="8"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="8"/>
+      <c r="AE30" s="8"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="8"/>
+      <c r="AH30" s="9"/>
+      <c r="AI30" s="10"/>
+      <c r="AJ30" s="11"/>
+      <c r="AK30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3602,7 +3804,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK3:AK28">
+  <conditionalFormatting sqref="AK3:AK30">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3950,7 +4152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P25 P27:P28">
+  <conditionalFormatting sqref="P3:P25 P27:P30">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3986,7 +4188,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D25 D27:D28">
+  <conditionalFormatting sqref="D3:D25 D27:D30">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4010,7 +4212,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE25 AE27:AE28">
+  <conditionalFormatting sqref="AE3:AE25 AE27:AE30">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4022,7 +4224,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB25 AB27:AB28">
+  <conditionalFormatting sqref="AB3:AB25 AB27:AB30">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4034,7 +4236,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y25 Y27:Y28">
+  <conditionalFormatting sqref="Y3:Y25 Y27:Y30">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4046,7 +4248,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M25 M27:M28">
+  <conditionalFormatting sqref="M3:M25 M27:M30">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4058,7 +4260,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V25 V27:V28">
+  <conditionalFormatting sqref="V3:V25 V27:V30">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4082,7 +4284,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S26:S27">
+  <conditionalFormatting sqref="S26:S30">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4094,7 +4296,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P26:P27">
+  <conditionalFormatting sqref="P26:P30">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4106,7 +4308,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J26:J27">
+  <conditionalFormatting sqref="J26:J30">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4118,7 +4320,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26:G27">
+  <conditionalFormatting sqref="G26:G30">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4130,7 +4332,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D27">
+  <conditionalFormatting sqref="D26:D30">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4142,7 +4344,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH26:AH27">
+  <conditionalFormatting sqref="AH26:AH30">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4154,7 +4356,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE26:AE27">
+  <conditionalFormatting sqref="AE26:AE30">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4166,7 +4368,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB26:AB27">
+  <conditionalFormatting sqref="AB26:AB30">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4178,7 +4380,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y26:Y27">
+  <conditionalFormatting sqref="Y26:Y30">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4190,7 +4392,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26:M27">
+  <conditionalFormatting sqref="M26:M30">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4202,7 +4404,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V26:V27">
+  <conditionalFormatting sqref="V26:V30">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4214,7 +4416,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH28">
+  <conditionalFormatting sqref="AH3:AH30">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4226,7 +4428,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE28">
+  <conditionalFormatting sqref="AE3:AE30">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4238,7 +4440,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB28">
+  <conditionalFormatting sqref="AB3:AB30">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4250,19 +4452,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB27">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y27">
+  <conditionalFormatting sqref="Y3:Y30">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4274,7 +4464,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V27">
+  <conditionalFormatting sqref="V3:V30">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4286,7 +4476,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S27">
+  <conditionalFormatting sqref="S3:S30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4298,7 +4488,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P27">
+  <conditionalFormatting sqref="P3:P30">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4310,7 +4500,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M27">
+  <conditionalFormatting sqref="M3:M30">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4322,7 +4512,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J27">
+  <conditionalFormatting sqref="J3:J30">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4334,7 +4524,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G27">
+  <conditionalFormatting sqref="G3:G30">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4346,7 +4536,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D27">
+  <conditionalFormatting sqref="D3:D30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4365,10 +4555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH24"/>
+  <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4414,7 +4604,7 @@
       <c r="L1" s="30"/>
       <c r="M1" s="31"/>
       <c r="N1" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O1" s="30"/>
       <c r="P1" s="31"/>
@@ -5359,7 +5549,7 @@
         <v>0.44357500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:22">
       <c r="A17" s="25" t="s">
         <v>44</v>
       </c>
@@ -5430,7 +5620,7 @@
         <v>0.24411666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:22">
       <c r="A18" s="25" t="s">
         <v>45</v>
       </c>
@@ -5501,7 +5691,7 @@
         <v>0.29361666666666664</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:22">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -5572,84 +5762,78 @@
         <v>0.21026666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:22">
       <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="7">
-        <v>0.33329999999999999</v>
+        <v>0.51049999999999995</v>
       </c>
       <c r="C20" s="8">
-        <v>0.51239999999999997</v>
+        <v>0.36270000000000002</v>
       </c>
       <c r="D20" s="9">
-        <v>0.40389999999999998</v>
+        <v>0.41699999999999998</v>
       </c>
       <c r="E20" s="7">
-        <v>0.77359999999999995</v>
+        <v>0.7107</v>
       </c>
       <c r="F20" s="8">
-        <v>0.2999</v>
+        <v>0.40570000000000001</v>
       </c>
       <c r="G20" s="9">
-        <v>0.43230000000000002</v>
+        <v>0.51190000000000002</v>
       </c>
       <c r="H20" s="7">
-        <v>0.53959999999999997</v>
+        <v>0.45710000000000001</v>
       </c>
       <c r="I20" s="8">
-        <v>0.1089</v>
+        <v>7.5300000000000006E-2</v>
       </c>
       <c r="J20" s="9">
-        <v>0.18129999999999999</v>
+        <v>0.12920000000000001</v>
       </c>
       <c r="K20" s="7">
-        <v>0.43959999999999999</v>
+        <v>0.42220000000000002</v>
       </c>
       <c r="L20" s="8">
-        <v>0.2016</v>
+        <v>0.32840000000000003</v>
       </c>
       <c r="M20" s="9">
-        <v>0.27650000000000002</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="N20" s="7">
-        <v>0.88500000000000001</v>
+        <v>0.74870000000000003</v>
       </c>
       <c r="O20" s="8">
-        <v>0.16589999999999999</v>
+        <v>0.159</v>
       </c>
       <c r="P20" s="9">
-        <v>0.27650000000000002</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="Q20" s="7">
-        <v>0.30640000000000001</v>
+        <v>0.37569999999999998</v>
       </c>
       <c r="R20" s="8">
-        <v>0.48270000000000002</v>
+        <v>0.44369999999999998</v>
       </c>
       <c r="S20" s="9">
-        <v>0.37490000000000001</v>
+        <v>0.39169999999999999</v>
       </c>
       <c r="T20" s="7">
         <f t="shared" ref="T20:T21" si="15">AVERAGE(B20,E20,H20,K20,N20,Q20)</f>
-        <v>0.54625000000000001</v>
+        <v>0.53748333333333342</v>
       </c>
       <c r="U20" s="8">
         <f t="shared" ref="U20:U21" si="16">AVERAGE(C20,F20,I20,L20,O20,R20)</f>
-        <v>0.29523333333333329</v>
+        <v>0.29580000000000001</v>
       </c>
       <c r="V20" s="9">
         <f t="shared" ref="V20:V21" si="17">AVERAGE(D20,G20,J20,M20,P20,S20)</f>
-        <v>0.32423333333333332</v>
-      </c>
-      <c r="W20">
-        <v>250</v>
-      </c>
-      <c r="X20">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
+        <v>0.33863333333333334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
         <v>63</v>
       </c>
@@ -5720,7 +5904,7 @@
         <v>0.26086666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:22">
       <c r="A22" s="5" t="s">
         <v>64</v>
       </c>
@@ -5791,7 +5975,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:22">
       <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
@@ -5862,99 +6046,186 @@
         <v>0.26210000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:22">
       <c r="A24" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B24" s="7">
-        <v>0.39389999999999997</v>
+        <v>0.52569999999999995</v>
       </c>
       <c r="C24" s="8">
-        <v>0.56440000000000001</v>
+        <v>0.45579999999999998</v>
       </c>
       <c r="D24" s="9">
-        <v>0.46400000000000002</v>
+        <v>0.46489999999999998</v>
       </c>
       <c r="E24" s="7">
-        <v>0.69469999999999998</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="F24" s="8">
-        <v>0.29820000000000002</v>
+        <v>0.62009999999999998</v>
       </c>
       <c r="G24" s="9">
-        <v>0.4173</v>
+        <v>0.56869999999999998</v>
       </c>
       <c r="H24" s="7">
-        <v>0.55000000000000004</v>
+        <v>0.50719999999999998</v>
       </c>
       <c r="I24" s="8">
-        <v>6.7999999999999996E-3</v>
+        <v>0.1239</v>
       </c>
       <c r="J24" s="9">
-        <v>1.34E-2</v>
+        <v>0.18859999999999999</v>
       </c>
       <c r="K24" s="7">
-        <v>0.46300000000000002</v>
+        <v>0.40229999999999999</v>
       </c>
       <c r="L24" s="8">
-        <v>0.2397</v>
+        <v>0.40529999999999999</v>
       </c>
       <c r="M24" s="9">
-        <v>0.31590000000000001</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="N24" s="7">
-        <v>0.5</v>
+        <v>0.82950000000000002</v>
       </c>
       <c r="O24" s="8">
-        <v>8.9999999999999998E-4</v>
+        <v>0.1187</v>
       </c>
       <c r="P24" s="9">
-        <v>1.9E-3</v>
+        <v>0.20030000000000001</v>
       </c>
       <c r="Q24" s="7">
-        <v>0.27039999999999997</v>
+        <v>0.37309999999999999</v>
       </c>
       <c r="R24" s="8">
-        <v>0.62009999999999998</v>
+        <v>0.38779999999999998</v>
       </c>
       <c r="S24" s="9">
-        <v>0.37659999999999999</v>
+        <v>0.37459999999999999</v>
       </c>
       <c r="T24" s="7">
         <f t="shared" ref="T24" si="24">AVERAGE(B24,E24,H24,K24,N24,Q24)</f>
-        <v>0.47866666666666663</v>
+        <v>0.53013333333333323</v>
       </c>
       <c r="U24" s="8">
         <f t="shared" ref="U24" si="25">AVERAGE(C24,F24,I24,L24,O24,R24)</f>
-        <v>0.28834999999999994</v>
+        <v>0.35193333333333326</v>
       </c>
       <c r="V24" s="9">
         <f t="shared" ref="V24" si="26">AVERAGE(D24,G24,J24,M24,P24,S24)</f>
-        <v>0.26484999999999997</v>
-      </c>
-      <c r="W24">
-        <v>250</v>
-      </c>
-      <c r="X24">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>67</v>
-      </c>
+        <v>0.36651666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="A25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.40510000000000002</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.24429999999999999</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.60209999999999997</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0.45679999999999998</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0.3347</v>
+      </c>
+      <c r="I25" s="8">
+        <v>0.29720000000000002</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0.31490000000000001</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.30990000000000001</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0.33179999999999998</v>
+      </c>
+      <c r="N25" s="7"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="9"/>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="9"/>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
@@ -6028,7 +6299,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V24">
+  <conditionalFormatting sqref="V3:V27">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6040,7 +6311,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D24">
+  <conditionalFormatting sqref="D3:D27">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6052,7 +6323,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G24">
+  <conditionalFormatting sqref="G3:G27">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6064,7 +6335,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J24">
+  <conditionalFormatting sqref="J3:J27">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6172,7 +6443,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M24">
+  <conditionalFormatting sqref="M3:M27">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6184,7 +6455,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P24">
+  <conditionalFormatting sqref="P3:P27">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6196,7 +6467,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S24">
+  <conditionalFormatting sqref="S3:S27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6218,7 +6489,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6478,14 +6749,40 @@
       <c r="A7" s="25" t="s">
         <v>48</v>
       </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="25" t="s">
         <v>49</v>
       </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="1"/>
+      <c r="A9" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0.70020000000000004</v>
+      </c>
+      <c r="D9" s="28">
+        <v>0.70840000000000003</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0.86580000000000001</v>
+      </c>
+      <c r="H9" s="28">
+        <v>0.49419999999999997</v>
+      </c>
+      <c r="J9" s="28">
+        <v>0.44690000000000002</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" ref="L7:L9" si="2">AVERAGE(D9,F9,H9,J9)</f>
+        <v>0.62882499999999997</v>
+      </c>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1"/>
@@ -6517,7 +6814,7 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="M3:M6">
+  <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6529,7 +6826,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L6">
+  <conditionalFormatting sqref="L3:L9">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6541,7 +6838,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B6">
+  <conditionalFormatting sqref="B3:B6 B9">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6553,7 +6850,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D6">
+  <conditionalFormatting sqref="D3:D6 D9">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6565,7 +6862,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F6">
+  <conditionalFormatting sqref="F3:F6 F9">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6577,7 +6874,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H7">
+  <conditionalFormatting sqref="H3:H7 H9">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6589,7 +6886,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J7">
+  <conditionalFormatting sqref="J3:J7 J9">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
Some more updated results.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="84">
   <si>
     <t>DEVEL</t>
   </si>
@@ -255,10 +255,19 @@
     <t>BP4D SVM static geometry</t>
   </si>
   <si>
-    <t>MLP joint</t>
-  </si>
-  <si>
     <t>Combined train MLP geom</t>
+  </si>
+  <si>
+    <t>MLP combined</t>
+  </si>
+  <si>
+    <t>MLP combined geom</t>
+  </si>
+  <si>
+    <t>SEMAINE SVM geometry stat</t>
+  </si>
+  <si>
+    <t>DISFA SVM geometry dyn</t>
   </si>
 </sst>
 </file>
@@ -449,6 +458,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,7 +471,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -767,76 +776,76 @@
   <dimension ref="A1:AK40"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="32" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="32" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="32" t="s">
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="32" t="s">
+      <c r="O1" s="31"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="30"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="32" t="s">
+      <c r="R1" s="31"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="32" t="s">
+      <c r="U1" s="31"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="32" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="32" t="s">
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="30" t="s">
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="30" t="s">
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="32"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3769,7 +3778,7 @@
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="7">
         <v>0.49170000000000003</v>
@@ -5099,10 +5108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH27"/>
+  <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5127,53 +5136,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="32" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="32" t="s">
+      <c r="L1" s="31"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="32" t="s">
+      <c r="O1" s="31"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="30"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="32" t="s">
+      <c r="R1" s="31"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6784,85 +6793,282 @@
         <v>77</v>
       </c>
       <c r="B27" s="7">
-        <v>0.55149999999999999</v>
+        <v>0.5837</v>
       </c>
       <c r="C27" s="8">
-        <v>0.5524</v>
+        <v>0.54169999999999996</v>
       </c>
       <c r="D27" s="9">
-        <v>0.55189999999999995</v>
+        <v>0.56189999999999996</v>
       </c>
       <c r="E27" s="7">
-        <v>0.66080000000000005</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="F27" s="8">
-        <v>0.47320000000000001</v>
+        <v>0.46089999999999998</v>
       </c>
       <c r="G27" s="9">
-        <v>0.55149999999999999</v>
+        <v>0.55159999999999998</v>
       </c>
       <c r="H27" s="7">
-        <v>0.51919999999999999</v>
+        <v>0.66</v>
       </c>
       <c r="I27" s="8">
-        <v>9.9699999999999997E-2</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="J27" s="9">
-        <v>0.1673</v>
+        <v>0.17510000000000001</v>
       </c>
       <c r="K27" s="7">
-        <v>0.33760000000000001</v>
+        <v>0.3281</v>
       </c>
       <c r="L27" s="8">
-        <v>0.27510000000000001</v>
+        <v>0.40589999999999998</v>
       </c>
       <c r="M27" s="9">
-        <v>0.30320000000000003</v>
+        <v>0.3629</v>
       </c>
       <c r="N27" s="7">
-        <v>0.4713</v>
+        <v>0.4607</v>
       </c>
       <c r="O27" s="8">
-        <v>3.8399999999999997E-2</v>
+        <v>3.5900000000000001E-2</v>
       </c>
       <c r="P27" s="9">
-        <v>7.1099999999999997E-2</v>
+        <v>6.6600000000000006E-2</v>
       </c>
       <c r="Q27" s="7">
-        <v>0.34129999999999999</v>
+        <v>0.33550000000000002</v>
       </c>
       <c r="R27" s="8">
-        <v>0.56950000000000001</v>
+        <v>0.56859999999999999</v>
       </c>
       <c r="S27" s="9">
-        <v>0.42680000000000001</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="T27" s="7">
         <f>AVERAGE(B27,E27,H27,K27,N27,Q27)</f>
-        <v>0.48028333333333334</v>
+        <v>0.50916666666666677</v>
       </c>
       <c r="U27" s="8">
         <f>AVERAGE(C27,F27,I27,L27,O27,R27)</f>
-        <v>0.33471666666666661</v>
+        <v>0.35233333333333333</v>
       </c>
       <c r="V27" s="9">
         <f>AVERAGE(D27,G27,J27,M27,P27,S27)</f>
-        <v>0.3453</v>
-      </c>
+        <v>0.3566833333333333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.26919999999999999</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.33660000000000001</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="9"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="7">
+        <v>0.57879999999999998</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.4456</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.50349999999999995</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.57879999999999998</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.4456</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0.50349999999999995</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0.71040000000000003</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0.2717</v>
+      </c>
+      <c r="K29" s="7">
+        <v>0.28949999999999998</v>
+      </c>
+      <c r="L29" s="8">
+        <v>0.45350000000000001</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0.35339999999999999</v>
+      </c>
+      <c r="N29" s="7"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="9"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="9"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="9"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="9"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="9"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
@@ -6936,7 +7142,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V27">
+  <conditionalFormatting sqref="V3:V34">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -6948,7 +7154,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D27">
+  <conditionalFormatting sqref="D3:D34">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -6960,7 +7166,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G27">
+  <conditionalFormatting sqref="G3:G34">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -6972,7 +7178,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J27">
+  <conditionalFormatting sqref="J3:J34">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -7080,7 +7286,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M27">
+  <conditionalFormatting sqref="M3:M34">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -7092,7 +7298,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P27">
+  <conditionalFormatting sqref="P3:P34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -7104,7 +7310,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S27">
+  <conditionalFormatting sqref="S3:S34">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -7125,8 +7331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7147,30 +7353,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="32" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="32"/>
+      <c r="L1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="31"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
@@ -7492,25 +7698,25 @@
         <v>0.90169999999999995</v>
       </c>
       <c r="L10" s="7">
-        <f t="shared" ref="L9:L10" si="2">AVERAGE(D10,F10,H10,J10)</f>
+        <f t="shared" ref="L10" si="2">AVERAGE(D10,F10,H10,J10)</f>
         <v>0.65042500000000003</v>
       </c>
       <c r="M10" s="9">
-        <f t="shared" ref="M9:M10" si="3">AVERAGE(E10,G10,I10,K10)</f>
+        <f t="shared" ref="M10" si="3">AVERAGE(E10,G10,I10,K10)</f>
         <v>0.93589999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="34">
+        <v>80</v>
+      </c>
+      <c r="B11" s="30">
         <v>0.76670000000000005</v>
       </c>
       <c r="C11">
         <v>0.79520000000000002</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="30">
         <v>0.8669</v>
       </c>
       <c r="G11">
@@ -7532,7 +7738,35 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="30">
+        <v>0.75880000000000003</v>
+      </c>
+      <c r="C12">
+        <v>0.83179999999999998</v>
+      </c>
+      <c r="F12" s="30">
+        <v>0.871</v>
+      </c>
+      <c r="G12" s="30">
+        <v>0.60240000000000005</v>
+      </c>
+      <c r="J12">
+        <v>0.51029999999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.87029999999999996</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" ref="L12" si="6">AVERAGE(D12,F12,H12,J12)</f>
+        <v>0.69064999999999999</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" ref="M12" si="7">AVERAGE(E12,G12,I12,K12)</f>
+        <v>0.73635000000000006</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -7555,7 +7789,7 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="M3:M11">
+  <conditionalFormatting sqref="M3:M12">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -7567,7 +7801,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L11">
+  <conditionalFormatting sqref="L3:L12">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -7699,7 +7933,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B11">
+  <conditionalFormatting sqref="B3:B12">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -7711,7 +7945,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C11">
+  <conditionalFormatting sqref="C3:C12">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -7747,7 +7981,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F11">
+  <conditionalFormatting sqref="F3:F12">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -7759,7 +7993,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G11">
+  <conditionalFormatting sqref="G3:G12">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -7795,7 +8029,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J11">
+  <conditionalFormatting sqref="J3:J12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -7807,7 +8041,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K11">
+  <conditionalFormatting sqref="K3:K12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Towards geometry in C++.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
     <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="87">
   <si>
     <t>DEVEL</t>
   </si>
@@ -269,12 +270,21 @@
   <si>
     <t>DISFA SVM geometry dyn</t>
   </si>
+  <si>
+    <t>BP4D SVM geometry dyn</t>
+  </si>
+  <si>
+    <t>BP4D SVM geometry stat</t>
+  </si>
+  <si>
+    <t>BP4D SVM dynamic geometry</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,7 +571,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -596,7 +605,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -772,20 +780,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:AK4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="B1" s="33" t="s">
         <v>2</v>
       </c>
@@ -847,7 +855,7 @@
       <c r="AJ1" s="31"/>
       <c r="AK1" s="32"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -960,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -1076,7 +1084,7 @@
         <v>0.26816666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1168,7 +1176,7 @@
         <v>0.25200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1260,7 +1268,7 @@
         <v>0.23471428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="16.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1352,7 +1360,7 @@
         <v>0.3408571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1444,7 +1452,7 @@
         <v>0.21928571428571431</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1560,7 +1568,7 @@
         <v>0.60526363636363623</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1676,7 +1684,7 @@
         <v>0.59264545454545459</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -1792,7 +1800,7 @@
         <v>0.59812727272727273</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1908,7 +1916,7 @@
         <v>0.59751818181818195</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -1976,7 +1984,7 @@
         <v>0.54469999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -2044,7 +2052,7 @@
         <v>0.23713333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -2112,7 +2120,7 @@
         <v>0.53643333333333332</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -2180,7 +2188,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -2272,7 +2280,7 @@
         <v>0.56054285714285712</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" s="25" t="s">
         <v>43</v>
       </c>
@@ -2364,7 +2372,7 @@
         <v>0.54634285714285713</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37">
       <c r="A18" s="25" t="s">
         <v>46</v>
       </c>
@@ -2444,7 +2452,7 @@
         <v>0.74680000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37">
       <c r="A19" s="25" t="s">
         <v>47</v>
       </c>
@@ -2524,7 +2532,7 @@
         <v>0.71243999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37">
       <c r="A20" s="25" t="s">
         <v>54</v>
       </c>
@@ -2640,7 +2648,7 @@
         <v>0.57558181818181819</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37">
       <c r="A21" s="25" t="s">
         <v>55</v>
       </c>
@@ -2756,7 +2764,7 @@
         <v>0.58974545454545457</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37">
       <c r="A22" s="25" t="s">
         <v>56</v>
       </c>
@@ -2872,7 +2880,7 @@
         <v>0.58663636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37">
       <c r="A23" s="25" t="s">
         <v>57</v>
       </c>
@@ -2988,7 +2996,7 @@
         <v>0.59650909090909088</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37">
       <c r="A24" s="25" t="s">
         <v>58</v>
       </c>
@@ -3104,7 +3112,7 @@
         <v>0.5917</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37">
       <c r="A25" s="25" t="s">
         <v>62</v>
       </c>
@@ -3220,7 +3228,7 @@
         <v>0.61232727272727272</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37">
       <c r="A26" s="25" t="s">
         <v>67</v>
       </c>
@@ -3336,7 +3344,7 @@
         <v>0.58963636363636374</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37">
       <c r="A27" s="25" t="s">
         <v>69</v>
       </c>
@@ -3452,7 +3460,7 @@
         <v>0.57887272727272732</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37">
       <c r="A28" s="25" t="s">
         <v>71</v>
       </c>
@@ -3568,7 +3576,7 @@
         <v>0.60222727272727272</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37">
       <c r="A29" s="25" t="s">
         <v>72</v>
       </c>
@@ -3660,7 +3668,7 @@
         <v>0.57781428571428584</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37">
       <c r="A30" s="25" t="s">
         <v>78</v>
       </c>
@@ -3692,49 +3700,49 @@
         <v>0.43869999999999998</v>
       </c>
       <c r="K30" s="7">
-        <v>0.67200000000000004</v>
+        <v>0.68489999999999995</v>
       </c>
       <c r="L30" s="8">
-        <v>0.84450000000000003</v>
+        <v>0.87690000000000001</v>
       </c>
       <c r="M30" s="8">
-        <v>0.74850000000000005</v>
+        <v>0.76910000000000001</v>
       </c>
       <c r="N30" s="7">
-        <v>0.66810000000000003</v>
+        <v>0.66059999999999997</v>
       </c>
       <c r="O30" s="8">
-        <v>0.88819999999999999</v>
+        <v>0.9345</v>
       </c>
       <c r="P30" s="8">
-        <v>0.76259999999999994</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="Q30" s="7">
-        <v>0.78480000000000005</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="R30" s="8">
-        <v>0.91920000000000002</v>
+        <v>0.94889999999999997</v>
       </c>
       <c r="S30" s="8">
-        <v>0.84670000000000001</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="T30" s="7">
-        <v>0.83140000000000003</v>
+        <v>0.82779999999999998</v>
       </c>
       <c r="U30" s="8">
-        <v>0.90810000000000002</v>
+        <v>0.92459999999999998</v>
       </c>
       <c r="V30" s="8">
-        <v>0.86799999999999999</v>
+        <v>0.87360000000000004</v>
       </c>
       <c r="W30" s="7">
-        <v>0.51849999999999996</v>
+        <v>0.51880000000000004</v>
       </c>
       <c r="X30" s="8">
-        <v>0.87639999999999996</v>
+        <v>0.87560000000000004</v>
       </c>
       <c r="Y30" s="8">
-        <v>0.65159999999999996</v>
+        <v>0.65149999999999997</v>
       </c>
       <c r="Z30" s="7">
         <v>0.35070000000000001</v>
@@ -3765,18 +3773,18 @@
       </c>
       <c r="AI30" s="10">
         <f t="shared" si="37"/>
-        <v>0.51865454545454548</v>
+        <v>0.51868181818181813</v>
       </c>
       <c r="AJ30" s="11">
         <f t="shared" si="38"/>
-        <v>0.71680909090909084</v>
+        <v>0.72809090909090912</v>
       </c>
       <c r="AK30" s="12">
         <f t="shared" si="39"/>
-        <v>0.59760909090909109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+        <v>0.60204545454545466</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37">
       <c r="A31" s="25" t="s">
         <v>79</v>
       </c>
@@ -3868,7 +3876,10 @@
         <v>0.57524285714285717</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37">
+      <c r="A32" s="25" t="s">
+        <v>86</v>
+      </c>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
@@ -3906,7 +3917,7 @@
       <c r="AJ32" s="11"/>
       <c r="AK32" s="12"/>
     </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:37">
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
@@ -3944,7 +3955,7 @@
       <c r="AJ33" s="11"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:37">
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
@@ -3982,7 +3993,7 @@
       <c r="AJ34" s="11"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:37">
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
@@ -4020,7 +4031,7 @@
       <c r="AJ35" s="11"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:37">
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
@@ -4058,7 +4069,7 @@
       <c r="AJ36" s="11"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:37">
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
@@ -4096,7 +4107,7 @@
       <c r="AJ37" s="11"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:37">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
@@ -4134,7 +4145,7 @@
       <c r="AJ38" s="11"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:37">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
@@ -4172,7 +4183,7 @@
       <c r="AJ39" s="11"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:37">
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
@@ -4228,9 +4239,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="76">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4240,9 +4251,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="75">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4252,9 +4263,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="74">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4264,9 +4275,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="73">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4276,9 +4287,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="72">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4288,9 +4299,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="71">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4300,9 +4311,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="70">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4312,9 +4323,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="69">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4324,9 +4335,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="68">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4336,9 +4347,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="67">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4348,9 +4359,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="66">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4360,9 +4371,9 @@
   <conditionalFormatting sqref="AK3:AK40">
     <cfRule type="colorScale" priority="65">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4372,9 +4383,9 @@
   <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="64">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4384,9 +4395,9 @@
   <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4396,9 +4407,9 @@
   <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4408,9 +4419,9 @@
   <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4420,9 +4431,9 @@
   <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4432,9 +4443,9 @@
   <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4444,9 +4455,9 @@
   <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4456,9 +4467,9 @@
   <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4468,9 +4479,9 @@
   <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4480,9 +4491,9 @@
   <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4492,9 +4503,9 @@
   <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4504,9 +4515,9 @@
   <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4516,9 +4527,9 @@
   <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4528,9 +4539,9 @@
   <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4540,9 +4551,9 @@
   <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4552,9 +4563,9 @@
   <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4564,9 +4575,9 @@
   <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4576,9 +4587,9 @@
   <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4588,9 +4599,9 @@
   <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4600,9 +4611,9 @@
   <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4612,9 +4623,9 @@
   <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4624,9 +4635,9 @@
   <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4636,9 +4647,9 @@
   <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4648,9 +4659,9 @@
   <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4660,9 +4671,9 @@
   <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4672,9 +4683,9 @@
   <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4684,9 +4695,9 @@
   <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4696,9 +4707,9 @@
   <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4708,9 +4719,9 @@
   <conditionalFormatting sqref="P3:P25 P27:P40">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4720,9 +4731,9 @@
   <conditionalFormatting sqref="J3:J25 X29:X40 J27:J40">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4732,9 +4743,9 @@
   <conditionalFormatting sqref="G3:G25 G27:G40">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4744,9 +4755,9 @@
   <conditionalFormatting sqref="D3:D25 D27:D40">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4756,9 +4767,9 @@
   <conditionalFormatting sqref="AH3:AH25 AH27:AH40">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4768,9 +4779,9 @@
   <conditionalFormatting sqref="AE3:AE25 AE27:AE40">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4780,9 +4791,9 @@
   <conditionalFormatting sqref="AB3:AB25 AB27:AB40">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4792,9 +4803,9 @@
   <conditionalFormatting sqref="Y3:Y25 Y27:Y40">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4804,9 +4815,9 @@
   <conditionalFormatting sqref="M3:M25 M27:M40">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4816,9 +4827,9 @@
   <conditionalFormatting sqref="V3:V25 V27:V40">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4828,9 +4839,9 @@
   <conditionalFormatting sqref="S3:S25">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4840,9 +4851,9 @@
   <conditionalFormatting sqref="S26:S40">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4852,9 +4863,9 @@
   <conditionalFormatting sqref="P26:P40">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4864,9 +4875,9 @@
   <conditionalFormatting sqref="J26:J40">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4876,9 +4887,9 @@
   <conditionalFormatting sqref="G26:G40">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4888,9 +4899,9 @@
   <conditionalFormatting sqref="D26:D40">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4900,9 +4911,9 @@
   <conditionalFormatting sqref="AH26:AH40">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4912,9 +4923,9 @@
   <conditionalFormatting sqref="AE26:AE40">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4924,9 +4935,9 @@
   <conditionalFormatting sqref="AB26:AB40">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4936,9 +4947,9 @@
   <conditionalFormatting sqref="Y26:Y40">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4948,9 +4959,9 @@
   <conditionalFormatting sqref="M26:M40">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4960,9 +4971,9 @@
   <conditionalFormatting sqref="V26:V40">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4972,9 +4983,9 @@
   <conditionalFormatting sqref="AH3:AH40">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4984,9 +4995,9 @@
   <conditionalFormatting sqref="AE3:AE40">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4996,9 +5007,9 @@
   <conditionalFormatting sqref="AB3:AB40">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5008,9 +5019,9 @@
   <conditionalFormatting sqref="Y3:Y40">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5020,9 +5031,9 @@
   <conditionalFormatting sqref="V3:V40">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5032,9 +5043,9 @@
   <conditionalFormatting sqref="S3:S40">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5044,9 +5055,9 @@
   <conditionalFormatting sqref="P3:P40">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5056,9 +5067,9 @@
   <conditionalFormatting sqref="M3:M40">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5068,9 +5079,9 @@
   <conditionalFormatting sqref="J3:J40">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5080,9 +5091,9 @@
   <conditionalFormatting sqref="G3:G40">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5092,9 +5103,9 @@
   <conditionalFormatting sqref="D3:D40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5107,14 +5118,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J31" sqref="C30:J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -5135,7 +5146,7 @@
     <col min="22" max="22" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
@@ -5184,7 +5195,7 @@
       <c r="AG1" s="34"/>
       <c r="AH1" s="34"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5252,7 +5263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
@@ -5311,7 +5322,7 @@
         <v>0.40849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -5370,7 +5381,7 @@
         <v>0.42475000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
@@ -5429,7 +5440,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>60</v>
       </c>
@@ -5488,7 +5499,7 @@
         <v>0.42574999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -5559,7 +5570,7 @@
         <v>0.28861666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -5630,7 +5641,7 @@
         <v>0.32611666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -5701,7 +5712,7 @@
         <v>0.30031666666666662</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -5772,7 +5783,7 @@
         <v>0.33934999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="5" t="s">
         <v>40</v>
       </c>
@@ -5825,7 +5836,7 @@
         <v>0.26416666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -5878,7 +5889,7 @@
         <v>0.30256666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -5931,7 +5942,7 @@
         <v>0.28023333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -5984,7 +5995,7 @@
         <v>0.28770000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
@@ -6043,7 +6054,7 @@
         <v>0.40457500000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34">
       <c r="A16" s="25" t="s">
         <v>43</v>
       </c>
@@ -6102,7 +6113,7 @@
         <v>0.44357500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="25" t="s">
         <v>44</v>
       </c>
@@ -6173,7 +6184,7 @@
         <v>0.24411666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" s="25" t="s">
         <v>45</v>
       </c>
@@ -6244,7 +6255,7 @@
         <v>0.29361666666666664</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -6315,7 +6326,7 @@
         <v>0.21026666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
@@ -6386,7 +6397,7 @@
         <v>0.33863333333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
         <v>63</v>
       </c>
@@ -6457,7 +6468,7 @@
         <v>0.26086666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="5" t="s">
         <v>64</v>
       </c>
@@ -6528,7 +6539,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
@@ -6599,7 +6610,7 @@
         <v>0.2364333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="5" t="s">
         <v>66</v>
       </c>
@@ -6670,7 +6681,7 @@
         <v>0.36651666666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" s="5" t="s">
         <v>75</v>
       </c>
@@ -6729,7 +6740,7 @@
         <v>0.36202499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" s="5" t="s">
         <v>76</v>
       </c>
@@ -6788,7 +6799,7 @@
         <v>0.38167500000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="5" t="s">
         <v>77</v>
       </c>
@@ -6859,7 +6870,7 @@
         <v>0.3566833333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" s="5" t="s">
         <v>82</v>
       </c>
@@ -6890,20 +6901,47 @@
       <c r="J28" s="9">
         <v>0.1285</v>
       </c>
-      <c r="K28" s="7"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="9"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K28" s="7">
+        <v>0.42680000000000001</v>
+      </c>
+      <c r="L28" s="8">
+        <v>0.42359999999999998</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0.42520000000000002</v>
+      </c>
+      <c r="N28" s="7">
+        <v>0.40739999999999998</v>
+      </c>
+      <c r="O28" s="8">
+        <v>4.82E-2</v>
+      </c>
+      <c r="P28" s="9">
+        <v>8.6099999999999996E-2</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="R28" s="8">
+        <v>0.59509999999999996</v>
+      </c>
+      <c r="S28" s="9">
+        <v>0.35489999999999999</v>
+      </c>
+      <c r="T28" s="7">
+        <f>AVERAGE(B28,E28,H28,K28,N28,Q28)</f>
+        <v>0.35180000000000006</v>
+      </c>
+      <c r="U28" s="8">
+        <f>AVERAGE(C28,F28,I28,L28,O28,R28)</f>
+        <v>0.35824999999999996</v>
+      </c>
+      <c r="V28" s="9">
+        <f>AVERAGE(D28,G28,J28,M28,P28,S28)</f>
+        <v>0.31143333333333334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="25" t="s">
         <v>83</v>
       </c>
@@ -6953,16 +6991,37 @@
       <c r="U29" s="8"/>
       <c r="V29" s="9"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="9"/>
+    <row r="30" spans="1:22">
+      <c r="A30" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.26519999999999999</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0.35720000000000002</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0.33639999999999998</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.80989999999999995</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0.47539999999999999</v>
+      </c>
+      <c r="H30" s="7">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.94850000000000001</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0.1145</v>
+      </c>
       <c r="K30" s="7"/>
       <c r="L30" s="8"/>
       <c r="M30" s="9"/>
@@ -6976,16 +7035,37 @@
       <c r="U30" s="8"/>
       <c r="V30" s="9"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="9"/>
+    <row r="31" spans="1:22">
+      <c r="A31" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0.1608</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.89570000000000005</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.2727</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0.33310000000000001</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.95279999999999998</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0.49359999999999998</v>
+      </c>
+      <c r="H31" s="7">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="I31" s="8">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0.12230000000000001</v>
+      </c>
       <c r="K31" s="7"/>
       <c r="L31" s="8"/>
       <c r="M31" s="9"/>
@@ -6999,7 +7079,7 @@
       <c r="U31" s="8"/>
       <c r="V31" s="9"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
@@ -7022,7 +7102,7 @@
       <c r="U32" s="8"/>
       <c r="V32" s="9"/>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22">
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
@@ -7045,7 +7125,7 @@
       <c r="U33" s="8"/>
       <c r="V33" s="9"/>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22">
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
@@ -7070,24 +7150,24 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7097,9 +7177,9 @@
   <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7109,9 +7189,9 @@
   <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7121,9 +7201,9 @@
   <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7133,9 +7213,9 @@
   <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7145,9 +7225,9 @@
   <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7157,9 +7237,9 @@
   <conditionalFormatting sqref="V3:V34">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7169,9 +7249,9 @@
   <conditionalFormatting sqref="D3:D34">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7181,9 +7261,9 @@
   <conditionalFormatting sqref="G3:G34">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7193,9 +7273,9 @@
   <conditionalFormatting sqref="J3:J34">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7205,9 +7285,9 @@
   <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7217,9 +7297,9 @@
   <conditionalFormatting sqref="M3:M16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7229,9 +7309,9 @@
   <conditionalFormatting sqref="M3:M18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7241,9 +7321,9 @@
   <conditionalFormatting sqref="P7:P18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7253,9 +7333,9 @@
   <conditionalFormatting sqref="S7:S18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7265,9 +7345,9 @@
   <conditionalFormatting sqref="M4:M21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7277,9 +7357,9 @@
   <conditionalFormatting sqref="P4:P21">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7289,9 +7369,9 @@
   <conditionalFormatting sqref="S4:S21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7301,9 +7381,9 @@
   <conditionalFormatting sqref="M3:M34">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7313,9 +7393,9 @@
   <conditionalFormatting sqref="P3:P34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7325,9 +7405,9 @@
   <conditionalFormatting sqref="S3:S34">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7340,14 +7420,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -7364,7 +7444,7 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="B1" s="33" t="s">
         <v>5</v>
       </c>
@@ -7390,7 +7470,7 @@
       </c>
       <c r="M1" s="32"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
         <v>50</v>
       </c>
@@ -7428,7 +7508,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="25" t="s">
         <v>46</v>
       </c>
@@ -7476,7 +7556,7 @@
         <v>1.0845751025000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
@@ -7524,7 +7604,7 @@
         <v>1.3607243325</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="25" t="s">
         <v>52</v>
       </c>
@@ -7572,7 +7652,7 @@
         <v>1.1540821750000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="25" t="s">
         <v>53</v>
       </c>
@@ -7620,21 +7700,21 @@
         <v>1.4101859700000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="25" t="s">
         <v>48</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="25" t="s">
         <v>49</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="25" t="s">
         <v>70</v>
       </c>
@@ -7675,7 +7755,7 @@
         <v>0.942025</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="25" t="s">
         <v>73</v>
       </c>
@@ -7718,7 +7798,7 @@
         <v>0.93589999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="25" t="s">
         <v>80</v>
       </c>
@@ -7749,7 +7829,7 @@
         <v>0.73710000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="25" t="s">
         <v>81</v>
       </c>
@@ -7780,16 +7860,16 @@
         <v>0.73635000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -7804,9 +7884,9 @@
   <conditionalFormatting sqref="M3:M12">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7816,9 +7896,9 @@
   <conditionalFormatting sqref="L3:L12">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7828,9 +7908,9 @@
   <conditionalFormatting sqref="B3:B6 B9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7840,9 +7920,9 @@
   <conditionalFormatting sqref="D3:D6 D9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7852,9 +7932,9 @@
   <conditionalFormatting sqref="F3:F6 F9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7864,9 +7944,9 @@
   <conditionalFormatting sqref="H3:H7 H9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7876,9 +7956,9 @@
   <conditionalFormatting sqref="J3:J7 J9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7888,9 +7968,9 @@
   <conditionalFormatting sqref="C3:C6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7900,9 +7980,9 @@
   <conditionalFormatting sqref="E3:E6">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7912,9 +7992,9 @@
   <conditionalFormatting sqref="G3:G7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7924,9 +8004,9 @@
   <conditionalFormatting sqref="I3:I6">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7936,9 +8016,9 @@
   <conditionalFormatting sqref="K3:K6">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7948,9 +8028,9 @@
   <conditionalFormatting sqref="B3:B12">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7960,9 +8040,9 @@
   <conditionalFormatting sqref="C3:C12">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7972,9 +8052,9 @@
   <conditionalFormatting sqref="D3:D11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7984,9 +8064,9 @@
   <conditionalFormatting sqref="E3:E11">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7996,9 +8076,9 @@
   <conditionalFormatting sqref="F3:F12">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8008,9 +8088,9 @@
   <conditionalFormatting sqref="G3:G12">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8020,9 +8100,9 @@
   <conditionalFormatting sqref="H3:H11">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8032,9 +8112,9 @@
   <conditionalFormatting sqref="I3:I11">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8044,9 +8124,9 @@
   <conditionalFormatting sqref="J3:J12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8056,9 +8136,9 @@
   <conditionalFormatting sqref="K3:K12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8068,4 +8148,999 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AK4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="13" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="31" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37">
+      <c r="B1" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="31"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="31"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="31"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="32"/>
+    </row>
+    <row r="2" spans="1:37">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="17" t="e">
+        <f>AVERAGE(B3,E3,H3,K3,N3,Q3,T3,W3,Z3,AC3,AF3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ3" s="18" t="e">
+        <f t="shared" ref="AJ3:AK4" si="0">AVERAGE(C3,F3,I3,L3,O3,R3,U3,X3,AA3,AD3,AG3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK3" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="10" t="e">
+        <f t="shared" ref="AI4" si="1">AVERAGE(B4,E4,H4,K4,N4,Q4,T4,W4,Z4,AC4,AF4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ4" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK4" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D3:D4">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J4">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M4">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P4">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S4">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V4">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y4">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB4">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE4">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH4">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK3:AK4">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D4">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J4">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M4">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P4">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S4">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V4">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y4">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB4">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE4">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH4">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V4">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE4">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J4">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M4">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB4">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M4">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M4">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE4">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB4">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S4">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P4">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J4">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D4">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH4">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE4">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB4">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y4">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M4">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V4">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S4">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH4">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE4">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB4">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y4">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V4">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S4">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P4">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M4">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J4">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D4">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Preparing final SEMAINE submission.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" refMode="R1C1"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="90">
   <si>
     <t>DEVEL</t>
   </si>
@@ -279,12 +279,21 @@
   <si>
     <t>BP4D SVM dynamic geometry</t>
   </si>
+  <si>
+    <t>DISFA SVM geometry stat</t>
+  </si>
+  <si>
+    <t>Combined SVM geometry stat</t>
+  </si>
+  <si>
+    <t>Combined SVM geometry dyn v sem</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,6 +580,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -605,6 +615,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -780,20 +791,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:AK4"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1" s="33" t="s">
         <v>2</v>
       </c>
@@ -855,7 +866,7 @@
       <c r="AJ1" s="31"/>
       <c r="AK1" s="32"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -968,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -1084,7 +1095,7 @@
         <v>0.26816666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1176,7 +1187,7 @@
         <v>0.25200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1268,7 +1279,7 @@
         <v>0.23471428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1">
+    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1360,7 +1371,7 @@
         <v>0.3408571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1452,7 +1463,7 @@
         <v>0.21928571428571431</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1568,7 +1579,7 @@
         <v>0.60526363636363623</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1684,7 +1695,7 @@
         <v>0.59264545454545459</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -1800,7 +1811,7 @@
         <v>0.59812727272727273</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1916,7 +1927,7 @@
         <v>0.59751818181818195</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -1984,7 +1995,7 @@
         <v>0.54469999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -2052,7 +2063,7 @@
         <v>0.23713333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -2120,7 +2131,7 @@
         <v>0.53643333333333332</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -2188,7 +2199,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -2280,7 +2291,7 @@
         <v>0.56054285714285712</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>43</v>
       </c>
@@ -2372,7 +2383,7 @@
         <v>0.54634285714285713</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>46</v>
       </c>
@@ -2452,7 +2463,7 @@
         <v>0.74680000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>47</v>
       </c>
@@ -2532,7 +2543,7 @@
         <v>0.71243999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>54</v>
       </c>
@@ -2648,7 +2659,7 @@
         <v>0.57558181818181819</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>55</v>
       </c>
@@ -2764,7 +2775,7 @@
         <v>0.58974545454545457</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>56</v>
       </c>
@@ -2880,7 +2891,7 @@
         <v>0.58663636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>57</v>
       </c>
@@ -2996,7 +3007,7 @@
         <v>0.59650909090909088</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>58</v>
       </c>
@@ -3112,7 +3123,7 @@
         <v>0.5917</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>62</v>
       </c>
@@ -3228,7 +3239,7 @@
         <v>0.61232727272727272</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>67</v>
       </c>
@@ -3344,7 +3355,7 @@
         <v>0.58963636363636374</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>69</v>
       </c>
@@ -3460,7 +3471,7 @@
         <v>0.57887272727272732</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>71</v>
       </c>
@@ -3576,7 +3587,7 @@
         <v>0.60222727272727272</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>72</v>
       </c>
@@ -3668,7 +3679,7 @@
         <v>0.57781428571428584</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>78</v>
       </c>
@@ -3784,7 +3795,7 @@
         <v>0.60204545454545466</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>79</v>
       </c>
@@ -3876,7 +3887,7 @@
         <v>0.57524285714285717</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>86</v>
       </c>
@@ -3917,7 +3928,7 @@
       <c r="AJ32" s="11"/>
       <c r="AK32" s="12"/>
     </row>
-    <row r="33" spans="2:37">
+    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
@@ -3955,7 +3966,7 @@
       <c r="AJ33" s="11"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="2:37">
+    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
@@ -3993,7 +4004,7 @@
       <c r="AJ34" s="11"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="2:37">
+    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
@@ -4031,7 +4042,7 @@
       <c r="AJ35" s="11"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="2:37">
+    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
@@ -4069,7 +4080,7 @@
       <c r="AJ36" s="11"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="2:37">
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
@@ -4107,7 +4118,7 @@
       <c r="AJ37" s="11"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="2:37">
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
@@ -4145,7 +4156,7 @@
       <c r="AJ38" s="11"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="2:37">
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
@@ -4183,7 +4194,7 @@
       <c r="AJ39" s="11"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="2:37">
+    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
@@ -4239,9 +4250,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="76">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4251,9 +4262,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="75">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4263,9 +4274,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="74">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4275,9 +4286,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="73">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4287,9 +4298,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="72">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4299,9 +4310,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="71">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4311,9 +4322,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="70">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4323,9 +4334,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="69">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4335,9 +4346,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="68">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4347,9 +4358,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="67">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4359,9 +4370,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="66">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4371,9 +4382,9 @@
   <conditionalFormatting sqref="AK3:AK40">
     <cfRule type="colorScale" priority="65">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4383,9 +4394,9 @@
   <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="64">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4395,9 +4406,9 @@
   <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4407,9 +4418,9 @@
   <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4419,9 +4430,9 @@
   <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4431,9 +4442,9 @@
   <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4443,9 +4454,9 @@
   <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4455,9 +4466,9 @@
   <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4467,9 +4478,9 @@
   <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4479,9 +4490,9 @@
   <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4491,9 +4502,9 @@
   <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4503,9 +4514,9 @@
   <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4515,9 +4526,9 @@
   <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4527,9 +4538,9 @@
   <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4539,9 +4550,9 @@
   <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4551,9 +4562,9 @@
   <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4563,9 +4574,9 @@
   <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4575,9 +4586,9 @@
   <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4587,9 +4598,9 @@
   <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4599,9 +4610,9 @@
   <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4611,9 +4622,9 @@
   <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4623,9 +4634,9 @@
   <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4635,9 +4646,9 @@
   <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4647,9 +4658,9 @@
   <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4659,9 +4670,9 @@
   <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4671,9 +4682,9 @@
   <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4683,9 +4694,9 @@
   <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4695,9 +4706,9 @@
   <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4707,9 +4718,9 @@
   <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4719,9 +4730,9 @@
   <conditionalFormatting sqref="P3:P25 P27:P40">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4731,9 +4742,9 @@
   <conditionalFormatting sqref="J3:J25 X29:X40 J27:J40">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4743,9 +4754,9 @@
   <conditionalFormatting sqref="G3:G25 G27:G40">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4755,9 +4766,9 @@
   <conditionalFormatting sqref="D3:D25 D27:D40">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4767,9 +4778,9 @@
   <conditionalFormatting sqref="AH3:AH25 AH27:AH40">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4779,9 +4790,9 @@
   <conditionalFormatting sqref="AE3:AE25 AE27:AE40">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4791,9 +4802,9 @@
   <conditionalFormatting sqref="AB3:AB25 AB27:AB40">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4803,9 +4814,9 @@
   <conditionalFormatting sqref="Y3:Y25 Y27:Y40">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4815,9 +4826,9 @@
   <conditionalFormatting sqref="M3:M25 M27:M40">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4827,9 +4838,9 @@
   <conditionalFormatting sqref="V3:V25 V27:V40">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4839,9 +4850,9 @@
   <conditionalFormatting sqref="S3:S25">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4851,9 +4862,9 @@
   <conditionalFormatting sqref="S26:S40">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4863,9 +4874,9 @@
   <conditionalFormatting sqref="P26:P40">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4875,9 +4886,9 @@
   <conditionalFormatting sqref="J26:J40">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4887,9 +4898,9 @@
   <conditionalFormatting sqref="G26:G40">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4899,9 +4910,9 @@
   <conditionalFormatting sqref="D26:D40">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4911,9 +4922,9 @@
   <conditionalFormatting sqref="AH26:AH40">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4923,9 +4934,9 @@
   <conditionalFormatting sqref="AE26:AE40">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4935,9 +4946,9 @@
   <conditionalFormatting sqref="AB26:AB40">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4947,9 +4958,9 @@
   <conditionalFormatting sqref="Y26:Y40">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4959,9 +4970,9 @@
   <conditionalFormatting sqref="M26:M40">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4971,9 +4982,9 @@
   <conditionalFormatting sqref="V26:V40">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4983,9 +4994,9 @@
   <conditionalFormatting sqref="AH3:AH40">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4995,9 +5006,9 @@
   <conditionalFormatting sqref="AE3:AE40">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5007,9 +5018,9 @@
   <conditionalFormatting sqref="AB3:AB40">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5019,9 +5030,9 @@
   <conditionalFormatting sqref="Y3:Y40">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5031,9 +5042,9 @@
   <conditionalFormatting sqref="V3:V40">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5043,9 +5054,9 @@
   <conditionalFormatting sqref="S3:S40">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5055,9 +5066,9 @@
   <conditionalFormatting sqref="P3:P40">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5067,9 +5078,9 @@
   <conditionalFormatting sqref="M3:M40">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5079,9 +5090,9 @@
   <conditionalFormatting sqref="J3:J40">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5091,9 +5102,9 @@
   <conditionalFormatting sqref="G3:G40">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5103,9 +5114,9 @@
   <conditionalFormatting sqref="D3:D40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5118,14 +5129,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="C30:J31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -5146,7 +5157,7 @@
     <col min="22" max="22" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
@@ -5195,7 +5206,7 @@
       <c r="AG1" s="34"/>
       <c r="AH1" s="34"/>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5263,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" customHeight="1">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
@@ -5322,7 +5333,7 @@
         <v>0.40849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -5381,7 +5392,7 @@
         <v>0.42475000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1">
+    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
@@ -5440,7 +5451,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1">
+    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>60</v>
       </c>
@@ -5499,7 +5510,7 @@
         <v>0.42574999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -5570,7 +5581,7 @@
         <v>0.28861666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -5641,7 +5652,7 @@
         <v>0.32611666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -5712,7 +5723,7 @@
         <v>0.30031666666666662</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -5783,7 +5794,7 @@
         <v>0.33934999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>40</v>
       </c>
@@ -5836,7 +5847,7 @@
         <v>0.26416666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -5889,7 +5900,7 @@
         <v>0.30256666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -5942,7 +5953,7 @@
         <v>0.28023333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -5995,7 +6006,7 @@
         <v>0.28770000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
@@ -6054,7 +6065,7 @@
         <v>0.40457500000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>43</v>
       </c>
@@ -6113,7 +6124,7 @@
         <v>0.44357500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>44</v>
       </c>
@@ -6184,7 +6195,7 @@
         <v>0.24411666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>45</v>
       </c>
@@ -6255,7 +6266,7 @@
         <v>0.29361666666666664</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -6326,7 +6337,7 @@
         <v>0.21026666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
@@ -6397,7 +6408,7 @@
         <v>0.33863333333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>63</v>
       </c>
@@ -6468,7 +6479,7 @@
         <v>0.26086666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>64</v>
       </c>
@@ -6539,7 +6550,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
@@ -6610,7 +6621,7 @@
         <v>0.2364333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>66</v>
       </c>
@@ -6681,7 +6692,7 @@
         <v>0.36651666666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>75</v>
       </c>
@@ -6740,7 +6751,7 @@
         <v>0.36202499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>76</v>
       </c>
@@ -6799,7 +6810,7 @@
         <v>0.38167500000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>77</v>
       </c>
@@ -6858,19 +6869,19 @@
         <v>0.42199999999999999</v>
       </c>
       <c r="T27" s="7">
-        <f>AVERAGE(B27,E27,H27,K27,N27,Q27)</f>
+        <f t="shared" ref="T27:V28" si="30">AVERAGE(B27,E27,H27,K27,N27,Q27)</f>
         <v>0.50916666666666677</v>
       </c>
       <c r="U27" s="8">
-        <f>AVERAGE(C27,F27,I27,L27,O27,R27)</f>
+        <f t="shared" si="30"/>
         <v>0.35233333333333333</v>
       </c>
       <c r="V27" s="9">
-        <f>AVERAGE(D27,G27,J27,M27,P27,S27)</f>
+        <f t="shared" si="30"/>
         <v>0.3566833333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>82</v>
       </c>
@@ -6929,57 +6940,57 @@
         <v>0.35489999999999999</v>
       </c>
       <c r="T28" s="7">
-        <f>AVERAGE(B28,E28,H28,K28,N28,Q28)</f>
+        <f t="shared" si="30"/>
         <v>0.35180000000000006</v>
       </c>
       <c r="U28" s="8">
-        <f>AVERAGE(C28,F28,I28,L28,O28,R28)</f>
+        <f t="shared" si="30"/>
         <v>0.35824999999999996</v>
       </c>
       <c r="V28" s="9">
-        <f>AVERAGE(D28,G28,J28,M28,P28,S28)</f>
+        <f t="shared" si="30"/>
         <v>0.31143333333333334</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B29" s="7">
-        <v>0.57879999999999998</v>
+        <v>0.21</v>
       </c>
       <c r="C29" s="8">
-        <v>0.4456</v>
+        <v>0.64</v>
       </c>
       <c r="D29" s="9">
-        <v>0.50349999999999995</v>
+        <v>0.32</v>
       </c>
       <c r="E29" s="7">
-        <v>0.57879999999999998</v>
+        <v>0.38</v>
       </c>
       <c r="F29" s="8">
-        <v>0.4456</v>
+        <v>0.76</v>
       </c>
       <c r="G29" s="9">
-        <v>0.50349999999999995</v>
+        <v>0.51</v>
       </c>
       <c r="H29" s="7">
-        <v>0.16800000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="I29" s="8">
-        <v>0.71040000000000003</v>
+        <v>0.88</v>
       </c>
       <c r="J29" s="9">
-        <v>0.2717</v>
+        <v>0.18</v>
       </c>
       <c r="K29" s="7">
-        <v>0.28949999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="L29" s="8">
-        <v>0.45350000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="M29" s="9">
-        <v>0.35339999999999999</v>
+        <v>0.43</v>
       </c>
       <c r="N29" s="7"/>
       <c r="O29" s="8"/>
@@ -6991,40 +7002,46 @@
       <c r="U29" s="8"/>
       <c r="V29" s="9"/>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="7">
-        <v>0.26519999999999999</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="C30" s="8">
-        <v>0.54700000000000004</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="D30" s="9">
-        <v>0.35720000000000002</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="E30" s="7">
-        <v>0.33639999999999998</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="F30" s="8">
-        <v>0.80989999999999995</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="G30" s="9">
-        <v>0.47539999999999999</v>
+        <v>0.28399999999999997</v>
       </c>
       <c r="H30" s="7">
-        <v>6.0900000000000003E-2</v>
+        <v>0.158</v>
       </c>
       <c r="I30" s="8">
-        <v>0.94850000000000001</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="J30" s="9">
-        <v>0.1145</v>
-      </c>
-      <c r="K30" s="7"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="9"/>
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="K30" s="7">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="L30" s="8">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0.33</v>
+      </c>
       <c r="N30" s="7"/>
       <c r="O30" s="8"/>
       <c r="P30" s="9"/>
@@ -7035,36 +7052,36 @@
       <c r="U30" s="8"/>
       <c r="V30" s="9"/>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="7">
-        <v>0.1608</v>
+        <v>0.26519999999999999</v>
       </c>
       <c r="C31" s="8">
-        <v>0.89570000000000005</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="D31" s="9">
-        <v>0.2727</v>
+        <v>0.35720000000000002</v>
       </c>
       <c r="E31" s="7">
-        <v>0.33310000000000001</v>
+        <v>0.33639999999999998</v>
       </c>
       <c r="F31" s="8">
-        <v>0.95279999999999998</v>
+        <v>0.80989999999999995</v>
       </c>
       <c r="G31" s="9">
-        <v>0.49359999999999998</v>
+        <v>0.47539999999999999</v>
       </c>
       <c r="H31" s="7">
-        <v>6.5500000000000003E-2</v>
+        <v>6.0900000000000003E-2</v>
       </c>
       <c r="I31" s="8">
-        <v>0.92100000000000004</v>
+        <v>0.94850000000000001</v>
       </c>
       <c r="J31" s="9">
-        <v>0.12230000000000001</v>
+        <v>0.1145</v>
       </c>
       <c r="K31" s="7"/>
       <c r="L31" s="8"/>
@@ -7079,16 +7096,37 @@
       <c r="U31" s="8"/>
       <c r="V31" s="9"/>
     </row>
-    <row r="32" spans="1:22">
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="9"/>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.1608</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0.89570000000000005</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.2727</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.33310000000000001</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.95279999999999998</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0.49359999999999998</v>
+      </c>
+      <c r="H32" s="7">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="I32" s="8">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.12230000000000001</v>
+      </c>
       <c r="K32" s="7"/>
       <c r="L32" s="8"/>
       <c r="M32" s="9"/>
@@ -7102,10 +7140,19 @@
       <c r="U32" s="8"/>
       <c r="V32" s="9"/>
     </row>
-    <row r="33" spans="2:22">
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="7">
+        <v>0.30349999999999999</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.40039999999999998</v>
+      </c>
       <c r="E33" s="7"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
@@ -7125,19 +7172,46 @@
       <c r="U33" s="8"/>
       <c r="V33" s="9"/>
     </row>
-    <row r="34" spans="2:22">
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="9"/>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="7">
+        <v>0.63</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.51529999999999998</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0.56689999999999996</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.42509999999999998</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.61870000000000003</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0.50390000000000001</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.19220000000000001</v>
+      </c>
+      <c r="I34" s="8">
+        <v>0.24679999999999999</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0.21609999999999999</v>
+      </c>
+      <c r="K34" s="7">
+        <v>0.28810000000000002</v>
+      </c>
+      <c r="L34" s="8">
+        <v>0.57509999999999994</v>
+      </c>
+      <c r="M34" s="9">
+        <v>0.38379999999999997</v>
+      </c>
       <c r="N34" s="7"/>
       <c r="O34" s="8"/>
       <c r="P34" s="9"/>
@@ -7148,26 +7222,49 @@
       <c r="U34" s="8"/>
       <c r="V34" s="9"/>
     </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7177,9 +7274,9 @@
   <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7189,9 +7286,9 @@
   <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7201,9 +7298,9 @@
   <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7213,9 +7310,9 @@
   <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7225,57 +7322,57 @@
   <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V34">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V35">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D34">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D35">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G34">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G35">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J34">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J35">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7285,9 +7382,9 @@
   <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7297,9 +7394,9 @@
   <conditionalFormatting sqref="M3:M16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7309,9 +7406,9 @@
   <conditionalFormatting sqref="M3:M18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7321,9 +7418,9 @@
   <conditionalFormatting sqref="P7:P18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7333,9 +7430,9 @@
   <conditionalFormatting sqref="S7:S18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7345,9 +7442,9 @@
   <conditionalFormatting sqref="M4:M21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7357,9 +7454,9 @@
   <conditionalFormatting sqref="P4:P21">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7369,45 +7466,45 @@
   <conditionalFormatting sqref="S4:S21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M34">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M35">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P34">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S34">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7420,14 +7517,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -7444,7 +7541,7 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="33" t="s">
         <v>5</v>
       </c>
@@ -7470,7 +7567,7 @@
       </c>
       <c r="M1" s="32"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>50</v>
       </c>
@@ -7508,7 +7605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>46</v>
       </c>
@@ -7556,7 +7653,7 @@
         <v>1.0845751025000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
@@ -7604,7 +7701,7 @@
         <v>1.3607243325</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>52</v>
       </c>
@@ -7652,7 +7749,7 @@
         <v>1.1540821750000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>53</v>
       </c>
@@ -7700,21 +7797,21 @@
         <v>1.4101859700000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>48</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>49</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>70</v>
       </c>
@@ -7755,7 +7852,7 @@
         <v>0.942025</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>73</v>
       </c>
@@ -7798,7 +7895,7 @@
         <v>0.93589999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>80</v>
       </c>
@@ -7829,7 +7926,7 @@
         <v>0.73710000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>81</v>
       </c>
@@ -7860,16 +7957,16 @@
         <v>0.73635000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -7884,9 +7981,9 @@
   <conditionalFormatting sqref="M3:M12">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7896,9 +7993,9 @@
   <conditionalFormatting sqref="L3:L12">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7908,9 +8005,9 @@
   <conditionalFormatting sqref="B3:B6 B9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7920,9 +8017,9 @@
   <conditionalFormatting sqref="D3:D6 D9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7932,9 +8029,9 @@
   <conditionalFormatting sqref="F3:F6 F9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7944,9 +8041,9 @@
   <conditionalFormatting sqref="H3:H7 H9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7956,9 +8053,9 @@
   <conditionalFormatting sqref="J3:J7 J9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7968,9 +8065,9 @@
   <conditionalFormatting sqref="C3:C6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7980,9 +8077,9 @@
   <conditionalFormatting sqref="E3:E6">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -7992,9 +8089,9 @@
   <conditionalFormatting sqref="G3:G7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8004,9 +8101,9 @@
   <conditionalFormatting sqref="I3:I6">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8016,9 +8113,9 @@
   <conditionalFormatting sqref="K3:K6">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8028,9 +8125,9 @@
   <conditionalFormatting sqref="B3:B12">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8040,9 +8137,9 @@
   <conditionalFormatting sqref="C3:C12">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8052,9 +8149,9 @@
   <conditionalFormatting sqref="D3:D11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8064,9 +8161,9 @@
   <conditionalFormatting sqref="E3:E11">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8076,9 +8173,9 @@
   <conditionalFormatting sqref="F3:F12">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8088,9 +8185,9 @@
   <conditionalFormatting sqref="G3:G12">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8100,9 +8197,9 @@
   <conditionalFormatting sqref="H3:H11">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8112,9 +8209,9 @@
   <conditionalFormatting sqref="I3:I11">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8124,9 +8221,9 @@
   <conditionalFormatting sqref="J3:J12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8136,9 +8233,9 @@
   <conditionalFormatting sqref="K3:K12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8151,14 +8248,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="13" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -8179,7 +8276,7 @@
     <col min="35" max="37" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1" s="33" t="s">
         <v>2</v>
       </c>
@@ -8241,7 +8338,7 @@
       <c r="AJ1" s="31"/>
       <c r="AK1" s="32"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8354,7 +8451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -8404,7 +8501,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -8456,11 +8553,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
@@ -8468,13 +8560,18 @@
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D4">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8484,9 +8581,9 @@
   <conditionalFormatting sqref="G3:G4">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8496,9 +8593,9 @@
   <conditionalFormatting sqref="J3:J4">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8508,9 +8605,9 @@
   <conditionalFormatting sqref="M3:M4">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8520,9 +8617,9 @@
   <conditionalFormatting sqref="P3:P4">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8532,9 +8629,9 @@
   <conditionalFormatting sqref="S3:S4">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8544,9 +8641,9 @@
   <conditionalFormatting sqref="V3:V4">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8556,9 +8653,9 @@
   <conditionalFormatting sqref="Y3:Y4">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8568,9 +8665,9 @@
   <conditionalFormatting sqref="AB3:AB4">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8580,9 +8677,9 @@
   <conditionalFormatting sqref="AE3:AE4">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8592,9 +8689,9 @@
   <conditionalFormatting sqref="AH3:AH4">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8604,9 +8701,9 @@
   <conditionalFormatting sqref="AK3:AK4">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8616,9 +8713,9 @@
   <conditionalFormatting sqref="D3:D4">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8628,9 +8725,9 @@
   <conditionalFormatting sqref="G3:G4">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8640,9 +8737,9 @@
   <conditionalFormatting sqref="J3:J4">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8652,9 +8749,9 @@
   <conditionalFormatting sqref="M3:M4">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8664,9 +8761,9 @@
   <conditionalFormatting sqref="P3:P4">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8676,9 +8773,9 @@
   <conditionalFormatting sqref="S3:S4">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8688,9 +8785,9 @@
   <conditionalFormatting sqref="V3:V4">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8700,9 +8797,9 @@
   <conditionalFormatting sqref="Y3:Y4">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8712,9 +8809,9 @@
   <conditionalFormatting sqref="AB3:AB4">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8724,9 +8821,9 @@
   <conditionalFormatting sqref="AE3:AE4">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8736,9 +8833,9 @@
   <conditionalFormatting sqref="AH3:AH4">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8748,9 +8845,9 @@
   <conditionalFormatting sqref="G3:G4">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8760,9 +8857,9 @@
   <conditionalFormatting sqref="V3:V4">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8772,9 +8869,9 @@
   <conditionalFormatting sqref="AE3:AE4">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8784,9 +8881,9 @@
   <conditionalFormatting sqref="J3:J4">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8796,9 +8893,9 @@
   <conditionalFormatting sqref="M3:M4">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8808,9 +8905,9 @@
   <conditionalFormatting sqref="AB4">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8820,9 +8917,9 @@
   <conditionalFormatting sqref="M3:M4">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8832,9 +8929,9 @@
   <conditionalFormatting sqref="M3:M4">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8844,9 +8941,9 @@
   <conditionalFormatting sqref="AE3:AE4">
     <cfRule type="colorScale" priority="25">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8856,9 +8953,9 @@
   <conditionalFormatting sqref="AB3:AB4">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8868,9 +8965,9 @@
   <conditionalFormatting sqref="S3:S4">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8880,9 +8977,9 @@
   <conditionalFormatting sqref="P3:P4">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8892,9 +8989,9 @@
   <conditionalFormatting sqref="J3:J4">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8904,9 +9001,9 @@
   <conditionalFormatting sqref="G3:G4">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8916,9 +9013,9 @@
   <conditionalFormatting sqref="D3:D4">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8928,9 +9025,9 @@
   <conditionalFormatting sqref="AH3:AH4">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8940,9 +9037,9 @@
   <conditionalFormatting sqref="AE3:AE4">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8952,9 +9049,9 @@
   <conditionalFormatting sqref="AB3:AB4">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8964,9 +9061,9 @@
   <conditionalFormatting sqref="Y3:Y4">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8976,9 +9073,9 @@
   <conditionalFormatting sqref="M3:M4">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8988,9 +9085,9 @@
   <conditionalFormatting sqref="V3:V4">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9000,9 +9097,9 @@
   <conditionalFormatting sqref="S3:S4">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9012,9 +9109,9 @@
   <conditionalFormatting sqref="AH3:AH4">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9024,9 +9121,9 @@
   <conditionalFormatting sqref="AE3:AE4">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9036,9 +9133,9 @@
   <conditionalFormatting sqref="AB3:AB4">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9048,9 +9145,9 @@
   <conditionalFormatting sqref="Y3:Y4">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9060,9 +9157,9 @@
   <conditionalFormatting sqref="V3:V4">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9072,9 +9169,9 @@
   <conditionalFormatting sqref="S3:S4">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9084,9 +9181,9 @@
   <conditionalFormatting sqref="P3:P4">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9096,9 +9193,9 @@
   <conditionalFormatting sqref="M3:M4">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9108,9 +9205,9 @@
   <conditionalFormatting sqref="J3:J4">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9120,9 +9217,9 @@
   <conditionalFormatting sqref="G3:G4">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9132,9 +9229,9 @@
   <conditionalFormatting sqref="D3:D4">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>

</xml_diff>